<commit_message>
Improve ParseTable function to better extract OCR data
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -182,6 +182,219 @@
     <x:t xml:space="preserve">NOTES </x:t>
   </x:si>
   <x:si>
+    <x:t>Noe POINT NAME 708 cont — IMTERPOSNG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INTERPOSING aie CRD ae RW NO: —— case No.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>‘DIA INNNOON Noe POINT NAME 78 cont — TMTERPOGNE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INTERPOSING OIG a OUTPUT —— CASE NO.) DIAG. iNNOON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTU MONITOR (JUMPER) CONTROL INHIBIT 0 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM — — [or t-t — = = = 81__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{GATE ~\ 79 1C7 96-24T/C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DI 5-80 [RM 5-35/36 W58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STINGER SWITCH 115KV 1 1 auto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOLID = — [or 1-2 = 10 = 82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FUPS TROUBLE F 80 1c8 DI 6-81 — W59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 [ftnyo 115KV CB 1 F———-~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OPEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-I/AT RK Z — [or 1-3 [RM 1-172 1B, 2A _ 83 [UI15KV CONTROL BUS AL) 81 95-1 DI 6-82 = W60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[INYO 115KV CB 2 [3 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-2/AT RK Z — [or 1-4 [Rm 1-374 1B, 2A _ 84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV RELAY BUS AL 82 95-2 DI 6-83 = W61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO 115KV CB 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 1 CLOSE OPEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-3/AT RK Z _— DI 1-5 [RM 1-5/6 1B, 2A — 85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV BACK-UP BUS AL 83 95-3 DI 6-84 = W62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 [CASA DIABLO-SHERWIN 115KV CB 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-5/AT RK Z — [or 1-6 [RM 1-7/8 1B, 2A _ 86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV OPERATING BUS AL 84 95-4 DI 6-85 = W63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV CB 7 6 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-7/AT RK 234 — [or t-7__ [RM 2-9/10 1B, 2A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640030 = 87_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV ELECTRONIC BUS AL 85 95-5 = DI 6-86 = W64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV CB 9 7 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-9/AT RK 235 — [or i-8 [RM 2-11712 1B, 24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640034 = 88__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DUPLICATE ELECTRONIC BUS 86 95-6 = DI 6-87 = W65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(BISHOP CREEK PLANT NO. 3 &amp; 4 115KV CB E</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-15/AT RK Z —  fori-9 [RM 2-13/14 1B, 2A = 89_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV _LBFB BUS 87 95-7 = DI 6-88 — W66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 [lOXBOW 115KV CB 17 lg 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-I7/AT RK Z — [or 1-10 [RM 2-15/16 1B, 2A = 90 __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV INTERFACE BUS 88 95-8 = DI 6-89 = W67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/OXBOW CUST CB I} 10 1 CLOSE OPEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95- X/AT RK Z = DI 1-11 [RM 3-17/18 1B, 2A = 91 __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>E115KVFMETER BUS F 89 95-9 = DI 6-90 = W68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12 [WWIXIE VALLEY CUST CBF Tn 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A = 92_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 90 = DI 6-91 = = W69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 [</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BUS TIE 115KV CB 23 12 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B, 24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640038 = 93__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 91 = DI 6-92 = = W70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 3 [—</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = = — [or 1-14 [RM 3-23/24 = = = 94 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(115KV W/BUS POT ALE 92 = DI 6-93 = Ww</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 4f{[—</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[— = = = — [or 1-15 [RM 4-25/26 = = = 95 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LI5KV_E/BUS POT ALJ 93 = DI 6-94 = W712</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 [fNO. 1 BANK T15KV CB 11) 15 1 CLOSE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-1I/AT RK Z — [or 1-16 [RM 4-27/28 1B, 2A = 96 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LOW DC VOLTAGE 94 1c-9 = DI 6-95 = W713</x:t>
+  </x:si>
+  <x:si>
     <x:t>17 {INO. 3 BANK 115KV CB 13 F 16 1 CLOSE OPEN</x:t>
   </x:si>
   <x:si>
@@ -194,6 +407,384 @@
     <x:t>BATT CHG FAIL FAIL LOSS OF AC 95 1C-10 _— DI 6-96 _— w74</x:t>
   </x:si>
   <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 17 = = = = — [ot 2-18 [RM 4-31/32 = = = 98 __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POSITIVE DC GRD 96 1c-11 = DI 7-97 = W75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ENTRY ALARM 18 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM TAI — [or 2-19 = 8 = 99 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NEGATIVE DC GRD 97 1C-12 = DI 7-98 = 4 W76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fi1S5KV CB LOW GAS7AIR 19 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM TA2 — [pI 2-20 = 6C W1 100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(SEL-2030 FAIL -—~—~~~~—~\({—«C98 1C-13 = DI 7-99 = 4 WT?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(115KV_CB GEN ALARM F 20 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1A3 — [or 2-21 = 6C Ww2 101 INO. 1 BANK LTC AUTO/MAN I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>99 = — DI 7-100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 5-37/38 4 Ww78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 21 = = = 1A4 — __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b1 2-22 = = = = 102 INO. 3 BANK LTC AUTO/MAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100 = = DI 7-101 [RM 5-39/40 4 w79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(NO. 1 BANKTHIGH TEMP AL = 22 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A5 — [or 2-23 — 6B W3 103 INO. 1 BANK TAP RATSE/LOWER I] 101 = = DI 7-102 [RM 6-41/42 4 W80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK GEN AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23 o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A6 — [pr 2-24 = 6B W4 104</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 3 BANK TAP RAISE/LOWER I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>102 — = DI 7-103 [RM 6-43/44 4 W81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK ITM FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL TAT — [or 2-25 — 6B W5 105 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISPARE I] 103 = = DI 7-104 [RM 6-45/46 4 — W82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK HYDROGEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A8 — [or 2-26 — 6B W6 106</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE JI 104 = — DI 7-105 _ 4 W83</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 FINO. 1 BANK WATER F 26 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A9 — [ol 2-27 — 6B WT 107</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>105 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 114 — DI 7-106 = 6B 5704099 Ww84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK HI GAS ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL TAI0 — [oI 2-28 = 6B W8 108</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1C15 = DI 7-107 = 6B 5704099 W85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 2 BANK HIGH TEMP AL J 28 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL TAIT — [or 2-29 — 6B W9 109 [115KV BUS TIE POS. 1X SEL-311C A/S [</x:t>
+  </x:si>
+  <x:si>
+    <x:t>107 1 AuTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOLID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8-1/AT RK Z51 = DI 7-108 = 3 5704099 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 2a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>—</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1A12 — [oI 2-30 — = = w10 110 [f- F[ 108 1C16 = DI 7-109 = 4 W86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1A13 — [or 2-31 — = = Wi mt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>109 = = DI 7-110 [RM 7-49/50 4 W87</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE ax</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1A14 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 2-32 = = = wi2 112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>110 ici? = DI ?-111 — 4 W88</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1A15 — [or 3-33 — = = W13 113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ant 1c18 — DI 7-112 = 4 W89</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 3 ]—i/— = = 1A16 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 3-34 = = = wi4 114</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RESERVED FOR 115KV LINE Pos. 2x ll 112 1c19 = DI 8-113 = 4 w90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(NO. 3 BANK HIGH TEMP AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A17 — DI 3-35 = 6B W15 115 {</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PROTECTION RELAYS ALARMS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>113 120 DI 8-114 = w91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36 FINO. 3 BANK GEN AL F 35 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1A18 — [or 3-36 = 6B Wi6 116</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 114 = DI 8-115 [RM 7-51/52 w92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[NO. 3 BANKFITM FAI ) 36 0 [ ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL TAS — [or 3-37 — 6B WI7 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 115 = DI 8-116 = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE x f[—i[— = = 1A20 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 3-38 = - = Wi8 18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 116 1021 DI 8-117 = W93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1A21 — [or 3-39 = = — wig 119</x:t>
+  </x:si>
+  <x:si>
+    <x:t>117 122 DI 8-118 = wo4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40 __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— = = 1422 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 3-40 = - = w20 120</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 118 1¢23 DI 8-119 = w95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FTRANS BK SUDDENTPRESS RESET “1 - = = — [RM 5-33/34 28 = 121</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F I] 119 1024 DI 8-120 = w96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK SEL-387 DIFF FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1A23 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 3-41 — 6B W21 122</x:t>
+  </x:si>
+  <x:si>
+    <x:t>120 = DI 8-121 = WoT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK SEL-387 DIFF TRIP Ifa 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1A24 — [pr 3-42 = 6B W22 123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I 121 — DI 8-122 [RM 7-53/54 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 1 BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B1 — [or 3-43 = 6B W23 124</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L RESERVED FOR 115KV LINE Pos. 1__l</x:t>
+  </x:si>
+  <x:si>
+    <x:t>122 1D-1 DI 8-123 = w98</x:t>
+  </x:si>
+  <x:si>
     <x:t>45</x:t>
   </x:si>
   <x:si>
@@ -209,6 +800,135 @@
     <x:t>[ PROTECTION RELAYS ALARMS I 123 1D-2 DI 8-124 — w99</x:t>
   </x:si>
   <x:si>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FNO. 1 BANK C30 FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B3 — [or 3-45 — 6B W25 126</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 124 10-3 DI 8-125 = W100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47_[ NO. 1 BANK C30 TRIP F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B4 — [ol 3-46 = 6B W26 127</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 125 10-4 DI 8-126 _— W101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B5 — [or 3-47 — 6B W27 128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>126 = DI 8-127 = W102 NOTES:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF FAIL I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B6 — [or 3-48 — 6B W28 129</x:t>
+  </x:si>
+  <x:si>
+    <x:t>127 = DI 8-128 [RM 7-55/56 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>48 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 187 — [or 4-49 — 6B W29 130</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F[_ 128 10-5 DI 9-129 = W103 " ane SINE RO SSE TRIPPING RECS.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B8 —  [dI 4-50 = 6B W30 131</x:t>
+  </x:si>
+  <x:si>
+    <x:t>129 10-6 DI 9-130 — W104 AN INDICATION IS TAKEN FROM EACH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INO. 3 BANK SEL-351 OC TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[ 50 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B9 — [or 4-51 = 6B W31 132</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 130 10-7 DI 9-131 — W105 RUA SUDDEN PRESSURE TRIPPING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53 NO. 3 BANK C30 FAIL I] 51 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B10 — [ol 4-52 = 6B W32 133</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I] 131 10-8 DI 9-132 = W106 .</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK C30 TRIP F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B11 — DI 4-53 = 6B W33 134</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I 132 = DI 9-133 — W107 2. OY IN A BLOCK INDICATES A VIRTUAL</x:t>
+  </x:si>
+  <x:si>
     <x:t>55</x:t>
   </x:si>
   <x:si>
@@ -230,9 +950,6 @@
     <x:t>115KV_UNDERFREQ POT FAIL 54 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM</x:t>
-  </x:si>
-  <x:si>
     <x:t>74/AT RK Z58 —_ DI 4-55 a 3 5704102 W35 136_</x:t>
   </x:si>
   <x:si>
@@ -242,6 +959,27 @@
     <x:t>134 1D-9 DI 9-135 _ W108 TS INTERCHANGED BETWEEN THE PLC</x:t>
   </x:si>
   <x:si>
+    <x:t>57_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV_UNDERFREQ TRIP/RESTORE 55 1 [NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B14 —___</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 4-56 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704103 W36 137_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F [PROTECTION RELAYS ALARMS i135 10-10 DI 9-136</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— W109 Ma a PROTOS Lee CALLY VIA THE</x:t>
+  </x:si>
+  <x:si>
     <x:t>58</x:t>
   </x:si>
   <x:si>
@@ -257,6 +995,477 @@
     <x:t>I! 136 10-11 DI 9-137 — WH10 "WA BLOCK MEANS THAT NO</x:t>
   </x:si>
   <x:si>
+    <x:t>59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>57 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B16 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ol 4-58 = 6A 5640043 W438 139</x:t>
+  </x:si>
+  <x:si>
+    <x:t>137 10-12 DI 9-138 = Witt DATA IS APPLICABLE FOR THAT BLOCK.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS A RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B17 — [oI 459 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640046 W39 140</x:t>
+  </x:si>
+  <x:si>
+    <x:t>138 = DI 9-139 = Wi12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1B18 = DI 4-60 = 6A 5640046 w40 141 {I [139 _ DI 9-140 [RM 8-59/60 = 3. FOR CASE NUMBER REFER TO DWG. 5640064.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS A RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM = — [or 4-61 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640043 wal 142 [J _J</x:t>
+  </x:si>
+  <x:si>
+    <x:t>140 1013 DI 9-141 = Wi13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS B RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM = — [oI 462 — 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640043 w42__</x:t>
+  </x:si>
+  <x:si>
+    <x:t>904962788 F743</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV1D60] TRIP 141 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1014 DI 9-142 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(5804239 wit4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM = — [di 4-63 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640046 W43 144</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KVID6O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>142 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1D15 DI 9-143 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58042391</x:t>
+  </x:si>
+  <x:si>
+    <x:t>wits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM _ —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 4-64 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640046 waa 145</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV[D60JA/S 143 1 auTo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8-2/AT RK 254 DI 9-144 _ 3 580423977</x:t>
+  </x:si>
+  <x:si>
+    <x:t>=</x:t>
+  </x:si>
+  <x:si>
+    <x:t>904962788</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR FAIL 64 1B19 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dI 5-65 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640062 W45 146</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>144 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1D16 DI 10-145] — 6B 5704087 WIIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR OPERATION 65 1820 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 5-66 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640062 Ww46 147</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL[ 145 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1D17 DI 10-146 6B 5704087 WHI?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY PICK UP 66 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1821 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 5-67 = 6A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704103 W47 148.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>146 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1018 DI 10-147, — 6A 5704087 Wwi18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY FAIL 67 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1822 — [br 5-68 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704103 w48 149</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>147 1 AUTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43-2/AT RK 54 DI 10-148] — 3 5704087 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>70 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FCASA DIABLO REACTOR CS 7} 68 95-21/AT RK Z —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 5-69 = 1B, 2A = 150</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>148 1 AUTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8-1/AT RK 754 DI_10-149</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 8-63/64 2B, 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704087 = *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ICASA DIABLO REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69 1C1 = DI 5-70 = 6A wag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>904562794 “Ts 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN T15KV{D60) TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>149 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1D19 DI 10-150 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(5804244)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>wii9 &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ICASA DIABLO REACTOR UV ] 70 1¢2 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[ors-71 = 6A W50 152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV(D60[RLY FAIL 150 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1020 DI 10-151 = 6B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5804244</x:t>
+  </x:si>
+  <x:si>
+    <x:t>W120 é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ICASA D-SHERWIN REACTOR CSF 71 95-22/AT RKZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— __</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DI 5-72 = 1B, 2A = 153</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV[D60/A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>151 1 AUTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6-2/AT RK 255 DI 10-152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2B, 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>se042aap</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— 904562794 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ICASA D-SHERWIN REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72 1C3 — [or 5-73 = 6A W51 154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>152 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1021 DI 10-153] — 6B 5704097 wi2t Q</x:t>
+  </x:si>
+  <x:si>
+    <x:t>75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FCASA D-SHERWIN REACTOR UV ] 3 1c4 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 5-74 = 6A W52 155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>153 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1022 DI 10-154] — 6B 5704097 W122 a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR OC RELAY BUS AL ] 74 95-7 AT PNLC3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>— _—‘</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DI 5-75 = 4 W53 156</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>154 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM 1023 DI 10-155, — 6A 5704097 W123 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR DC BACK-UP BUS AL ] 15 95-8 AT C3 — [ol 5-76 = 4 W54 157</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>155 1 AUTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43-2/AT RK 255 DI 10-156] — 3 5704097 = 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR OPERATING BUS AL F 16 95-9 AT C3 — [or 5-7 = 4 W55 158</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>156 1 AuTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8-1/AT RK 255 DI_10-157</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 9-67/68 2B, 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704097 = :</x:t>
+  </x:si>
+  <x:si>
+    <x:t>79 [[cD SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TT 105 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p 5-78 = 6A W56 159</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HATWEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>157 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1024 DI 10-158] — 6B 5704087 wi24 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[CD-S SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>78 1C6 — [or 5-79 = 6A W57 160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>158 0 ALARM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL 1E1 DI 10-159] — 6B 5704097 W128 2</x:t>
+  </x:si>
+  <x:si>
     <x:t>——</x:t>
   </x:si>
   <x:si>
@@ -266,9 +1475,6 @@
     <x:t>] 904562794 LOCATION: CONTROL SUBSTATION SHEET NO.</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
     <x:t>ADDED POINT FOR 115KV LINE POS. 4 RELAY</x:t>
   </x:si>
   <x:si>
@@ -320,6 +1526,9 @@
     <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. 3 RLY'S 903536612 SH. 1</x:t>
   </x:si>
   <x:si>
+    <x:t>5640065-3</x:t>
+  </x:si>
+  <x:si>
     <x:t>CONTRL_D  DNP Analog Point List</x:t>
   </x:si>
   <x:si>
@@ -449,6 +1658,30 @@
     <x:t xml:space="preserve">TESTMAN </x:t>
   </x:si>
   <x:si>
+    <x:t>rte POINT NAME INTERPOSNG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INTERPOSING SST TGUUT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASE.NO-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pia _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ANNUNCTATOR ire POINT NAME INTERPOSNG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INTERPOSING SUT TUTPUT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>prac. _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ANNUNCTATOR</x:t>
+  </x:si>
+  <x:si>
     <x:t>NUMBER Bee CONT</x:t>
   </x:si>
   <x:si>
@@ -470,15 +1703,66 @@
     <x:t>RELAY NO. TNT NS oupuy io. MPT MOT (NOTE 3)} pwc. WINDOW</x:t>
   </x:si>
   <x:si>
+    <x:t>161</x:t>
+  </x:si>
+  <x:si>
+    <x:t>] 159 1 1£2 = DI 10-160 = W129 241</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(SILVERPEAK A A ToT ' \ 239 = -</x:t>
+  </x:si>
+  <x:si>
+    <x:t>162_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>160 1 1E3 DI 11-161 10 W130 242</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISILVERPEAK A B TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>240 = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>163_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_L ReserVeD FOR 115KV LINE pos. 4_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>161 1 164 DI 11-162 TA, 2A W131 243</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISILVERPEAK A C TCT E 24 = =</x:t>
+  </x:si>
+  <x:si>
     <x:t>164</x:t>
   </x:si>
   <x:si>
-    <x:t>PROTECTION RELAYS ALARMS</x:t>
-  </x:si>
-  <x:si>
     <x:t>162 1 _— DI 11-163 W132 244 FSTLVERPEAK A GRD ToT Ji 904562788) 240 904562788 — rT 904562788 _</x:t>
   </x:si>
   <x:si>
+    <x:t>165</x:t>
+  </x:si>
+  <x:si>
+    <x:t>163 1 _— DI 11-164</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 9-67/68 = 245</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(HAIWEE-INYOKERN 115KV D60 OPD A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>243 1 NORMAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16-15 DI 15-228 { 6A "</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5804239 ) wig92</x:t>
+  </x:si>
+  <x:si>
     <x:t>166 [fF F</x:t>
   </x:si>
   <x:si>
@@ -503,9 +1787,6 @@
     <x:t>167</x:t>
   </x:si>
   <x:si>
-    <x:t>I</x:t>
-  </x:si>
-  <x:si>
     <x:t>165 1 166 DI 11-166 W134 247</x:t>
   </x:si>
   <x:si>
@@ -563,6 +1844,36 @@
     <x:t>W196</x:t>
   </x:si>
   <x:si>
+    <x:t>170</x:t>
+  </x:si>
+  <x:si>
+    <x:t>168 1 = DI 11-169 W137 250 [\COSO-HAIWEESINYOKERN 115KV 060 OPO TRIP _)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>248 Lt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALARM J 16-20 DI 15-233 \_6A_,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_ 5804244 J] W197</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>169 1 = DI 11-170</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 9-69/70 = 251_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE L 904562794 249 Lt 904562794 16-21 DI 15-234 LT gn4562794</x:t>
+  </x:si>
+  <x:si>
+    <x:t>W198</x:t>
+  </x:si>
+  <x:si>
     <x:t>172 [i RESERVED FOR 115KV LINE Pos. 7_[</x:t>
   </x:si>
   <x:si>
@@ -590,6 +1901,15 @@
     <x:t>SPARE 252 16-24 DI 15-237 W201</x:t>
   </x:si>
   <x:si>
+    <x:t>175.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>173 1 1E12 DI 11-174 wi4i 255</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PMU TROUBLE ALARM 253 = DI 15-238 W202</x:t>
+  </x:si>
+  <x:si>
     <x:t>176</x:t>
   </x:si>
   <x:si>
@@ -599,6 +1919,30 @@
     <x:t>SPARE 254 DI 15-239 —</x:t>
   </x:si>
   <x:si>
+    <x:t>177</x:t>
+  </x:si>
+  <x:si>
+    <x:t>175 1 = DI 11-176</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 9-71/72 _ 257</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 255 DI 15-240 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>178</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>176 1 1E13 DI 12-177 W143 258</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 256 = DI 16-241 W203</x:t>
+  </x:si>
+  <x:si>
     <x:t>179</x:t>
   </x:si>
   <x:si>
@@ -611,6 +1955,126 @@
     <x:t>SPARE 257 _— DI 16-242 W204</x:t>
   </x:si>
   <x:si>
+    <x:t>180</x:t>
+  </x:si>
+  <x:si>
+    <x:t>178 1 1E15 DI 12-179 W145 260</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 258 = DI 16-243 W205</x:t>
+  </x:si>
+  <x:si>
+    <x:t>181</x:t>
+  </x:si>
+  <x:si>
+    <x:t>179 1 1E16 DI 12-180 W146 261 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 259 = DI 16-244 W206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>182_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>180 1 = DI 12-181 W147 262 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 260 = DI 16-245 W207</x:t>
+  </x:si>
+  <x:si>
+    <x:t>183</x:t>
+  </x:si>
+  <x:si>
+    <x:t>181 1 = DI 12-182</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 10-73/74 = 263</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 261 = DI 16-246 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>184 [fF L RESERVED FOR 115KV LINE POs. 8 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>182 1 1E17 DI 12-183 W148 264</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 262 — DI 16-247</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 10-77/78 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>185</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{ PROTECTION RELAYS ALARMS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>183 1 1E18 DI 12-184 149 265 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 263 = DI 16-248]RM 10-79/80 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>186 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>184 1 1E19 DI 12-185 W150 266</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 264 = DI 16-249]RM 11-81/82 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>187</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fl 195 1 1£20 DI 12-186 W151 267</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 265 = DI 16-250</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/RM 11-83/84 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>188_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>186 1 = DI 12-187 W152 268 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 266 = DI 16-251</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 11-85/86 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>189</x:t>
+  </x:si>
+  <x:si>
+    <x:t>187 1 = DI 12-188]RM 10-75/76 _ 269</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 267 = DI 16-252]RM 11-87/88 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>190</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p_____J</x:t>
+  </x:si>
+  <x:si>
+    <x:t>188 1 1621 DI 12-189 W153 270</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 268 = DI 16-253</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RM 12-89/90 =</x:t>
+  </x:si>
+  <x:si>
     <x:t>191</x:t>
   </x:si>
   <x:si>
@@ -620,6 +2084,30 @@
     <x:t>SPARE 269 _ DI 16-254]RM 12-91/92 _</x:t>
   </x:si>
   <x:si>
+    <x:t>192</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB TRIP 190 1 1F2 DI 12-191 NOTE 4 W155 272_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 270 = DI 16-255</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/RM 12-93/94 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>193</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(15KV CB I'LBFB RELAY PS % FAIL \</x:t>
+  </x:si>
+  <x:si>
+    <x:t>191 1 1F3 DI 12-192 W156 273</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE on = DI 16-256]/RM 12-95/96 =</x:t>
+  </x:si>
+  <x:si>
     <x:t>194</x:t>
   </x:si>
   <x:si>
@@ -629,6 +2117,12 @@
     <x:t>192 1 1F4 DI 13-193 WI57</x:t>
   </x:si>
   <x:si>
+    <x:t>195 [f115KV CB 2 LBFB RELAY PS % FAIL F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>193 1 1F5 DI 13-194 W158</x:t>
+  </x:si>
+  <x:si>
     <x:t>196</x:t>
   </x:si>
   <x:si>
@@ -761,6 +2255,12 @@
     <x:t>115KV CB 23 LBFB RELAY FAIL 212 1 1F24 DI 14-213 5640038 WI77</x:t>
   </x:si>
   <x:si>
+    <x:t>215 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 213 161 DI 14-214 W178</x:t>
+  </x:si>
+  <x:si>
     <x:t>216</x:t>
   </x:si>
   <x:si>
@@ -776,12 +2276,21 @@
     <x:t>2t5 163 DI 14-216 W180 NOTES:</x:t>
   </x:si>
   <x:si>
+    <x:t>218 Hake CB 2 TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>216 164 DI 14-217 wie!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>220 [[115KV CB 5 TCM [</x:t>
+  </x:si>
+  <x:si>
+    <x:t>218 166 DI 14-219 W183 ALL SUDDEN PRESSURE TRIPPING RELAYS.</x:t>
+  </x:si>
+  <x:si>
     <x:t>221 F15KV CB 7 TCM</x:t>
   </x:si>
   <x:si>
-    <x:t>_</x:t>
-  </x:si>
-  <x:si>
     <x:t>219 167 DI 14-220 W184 INDIVIDUAL SUDDEN PRESSURE TRIPPING</x:t>
   </x:si>
   <x:si>
@@ -839,6 +2348,12 @@
     <x:t>226 1614 DI 15-227 W191 b) " — "IN A BLOCK MEANS THAT NO</x:t>
   </x:si>
   <x:si>
+    <x:t>909 IIMWE-INYOKERN A TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>207 — — DATA IS APPLICABLE FOR THAT BLOCK.</x:t>
+  </x:si>
+  <x:si>
     <x:t>230_</x:t>
   </x:si>
   <x:si>
@@ -846,6 +2361,93 @@
   </x:si>
   <x:si>
     <x:t>228 _— _ 3. FOR CASE NUMBER REFER TO DWG. 5640064. *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>231 _fHWE-INYOKERN C TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>229 = _ &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>232_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IHWE-INYOKERN GRD_TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>230 = = FE Ey BEB RN LAVS, Te ANN FOR ALL 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>233</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE A TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>231 = = a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE B TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>232 = _ @</x:t>
+  </x:si>
+  <x:si>
+    <x:t>235 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso_HWE C_TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>233 = = 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>236</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE GRD TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>234 = = é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>237 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISILVERPEAK C A TCT F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>235 = = 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>238_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISILVERPEAK C_B TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>236 = = :</x:t>
+  </x:si>
+  <x:si>
+    <x:t>239</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISILVERPEAK C C TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>237 = _ °</x:t>
+  </x:si>
+  <x:si>
+    <x:t>240</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK C GRD TcT ps (</x:t>
+  </x:si>
+  <x:si>
+    <x:t>238 = _ 2</x:t>
   </x:si>
   <x:si>
     <x:t>ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
@@ -1244,7 +2846,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AB25"/>
+  <x:dimension ref="A1:AB102"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1475,124 +3077,1598 @@
       <x:c r="D18" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
     </x:row>
     <x:row r="19" spans="1:28">
       <x:c r="A19" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B19" s="0" t="s">
+      <x:c r="C19" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="C19" s="0" t="s">
+      <x:c r="D19" s="0" t="s">
         <x:v>71</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="F19" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:28">
       <x:c r="A20" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
         <x:v>75</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:28">
       <x:c r="A21" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
         <x:v>80</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:28">
       <x:c r="A22" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
         <x:v>83</x:v>
       </x:c>
-      <x:c r="B22" s="0" t="s">
+      <x:c r="E22" s="0" t="s">
         <x:v>84</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="E22" s="0" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="F22" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="G22" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="H22" s="0" t="s">
-        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:28">
       <x:c r="A23" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:28">
       <x:c r="A24" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
         <x:v>92</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
+      <x:c r="E24" s="0" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="C24" s="0" t="s">
+      <x:c r="F24" s="0" t="s">
         <x:v>94</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="F24" s="0" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="G24" s="0" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="H24" s="0" t="s">
-        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:28">
       <x:c r="A25" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="B25" s="0" t="s">
+    </x:row>
+    <x:row r="26" spans="1:28">
+      <x:c r="A26" s="0" t="s">
         <x:v>100</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:28">
+      <x:c r="A27" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:28">
+      <x:c r="A28" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:28">
+      <x:c r="A29" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:28">
+      <x:c r="A30" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:28">
+      <x:c r="A31" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:28">
+      <x:c r="A32" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:28">
+      <x:c r="A33" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:28">
+      <x:c r="A34" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:28">
+      <x:c r="A35" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:28">
+      <x:c r="A36" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:28">
+      <x:c r="A37" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:28">
+      <x:c r="A38" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:28">
+      <x:c r="A39" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:28">
+      <x:c r="A40" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="G40" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:28">
+      <x:c r="A41" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:28">
+      <x:c r="A42" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:28">
+      <x:c r="A43" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:28">
+      <x:c r="A44" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="G44" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="H44" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:28">
+      <x:c r="A45" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="G45" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:28">
+      <x:c r="A46" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:28">
+      <x:c r="A47" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:28">
+      <x:c r="A48" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:28">
+      <x:c r="A49" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:28">
+      <x:c r="A50" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:28">
+      <x:c r="A51" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="G51" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="H51" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:28">
+      <x:c r="A52" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:28">
+      <x:c r="A53" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:28">
+      <x:c r="A54" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:28">
+      <x:c r="A55" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:28">
+      <x:c r="A56" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="E56" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+      <x:c r="F56" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:28">
+      <x:c r="A57" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:28">
+      <x:c r="A58" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="E58" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="F58" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="G58" s="0" t="s">
+        <x:v>245</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:28">
+      <x:c r="A59" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>248</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:28">
+      <x:c r="A60" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="F60" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:28">
+      <x:c r="A61" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="E61" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:28">
+      <x:c r="A62" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E62" s="0" t="s">
+        <x:v>265</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:28">
+      <x:c r="A63" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:28">
+      <x:c r="A64" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="D64" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="E64" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="F64" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:28">
+      <x:c r="A65" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="D65" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="E65" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:28">
+      <x:c r="A66" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="D66" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="E66" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:28">
+      <x:c r="A67" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="D67" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="E67" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="F67" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:28">
+      <x:c r="A68" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="E68" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="F68" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:28">
+      <x:c r="A69" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:28">
+      <x:c r="A70" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="E70" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:28">
+      <x:c r="A71" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="E71" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:28">
+      <x:c r="A72" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D72" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="E72" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="F72" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:28">
+      <x:c r="A73" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="D73" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="E73" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="F73" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+      <x:c r="G73" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:28">
+      <x:c r="A74" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="D74" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="E74" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:28">
+      <x:c r="A75" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="E75" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="F75" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="G75" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:28">
+      <x:c r="A76" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="D76" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="E76" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="F76" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:28">
+      <x:c r="A77" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:28">
+      <x:c r="A78" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="D78" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="E78" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="F78" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:28">
+      <x:c r="A79" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="D79" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="E79" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="F79" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="G79" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="H79" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="I79" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:28">
+      <x:c r="A80" s="0" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="D80" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="E80" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="F80" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="G80" s="0" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="H80" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="I80" s="0" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="J80" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="K80" s="0" t="s">
+        <x:v>367</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:28">
+      <x:c r="A81" s="0" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="D81" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="E81" s="0" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="F81" s="0" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="G81" s="0" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="H81" s="0" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="I81" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="J81" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="K81" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="L81" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:28">
+      <x:c r="A82" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="D82" s="0" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="E82" s="0" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="F82" s="0" t="s">
+        <x:v>383</x:v>
+      </x:c>
+      <x:c r="G82" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:28">
+      <x:c r="A83" s="0" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="E83" s="0" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="F83" s="0" t="s">
+        <x:v>390</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:28">
+      <x:c r="A84" s="0" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="D84" s="0" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="E84" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="F84" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="G84" s="0" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="H84" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:28">
+      <x:c r="A85" s="0" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="E85" s="0" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="F85" s="0" t="s">
+        <x:v>404</x:v>
+      </x:c>
+      <x:c r="G85" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="H85" s="0" t="s">
+        <x:v>405</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:28">
+      <x:c r="A86" s="0" t="s">
+        <x:v>406</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>407</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="D86" s="0" t="s">
+        <x:v>409</x:v>
+      </x:c>
+      <x:c r="E86" s="0" t="s">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="F86" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="G86" s="0" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="H86" s="0" t="s">
+        <x:v>412</x:v>
+      </x:c>
+      <x:c r="I86" s="0" t="s">
+        <x:v>413</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:28">
+      <x:c r="A87" s="0" t="s">
+        <x:v>414</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>415</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>417</x:v>
+      </x:c>
+      <x:c r="E87" s="0" t="s">
+        <x:v>418</x:v>
+      </x:c>
+      <x:c r="F87" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+      <x:c r="G87" s="0" t="s">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="H87" s="0" t="s">
+        <x:v>421</x:v>
+      </x:c>
+      <x:c r="I87" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:28">
+      <x:c r="A88" s="0" t="s">
+        <x:v>423</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>424</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>425</x:v>
+      </x:c>
+      <x:c r="D88" s="0" t="s">
+        <x:v>426</x:v>
+      </x:c>
+      <x:c r="E88" s="0" t="s">
+        <x:v>427</x:v>
+      </x:c>
+      <x:c r="F88" s="0" t="s">
+        <x:v>428</x:v>
+      </x:c>
+      <x:c r="G88" s="0" t="s">
+        <x:v>429</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:28">
+      <x:c r="A89" s="0" t="s">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>431</x:v>
+      </x:c>
+      <x:c r="C89" s="0" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="D89" s="0" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="E89" s="0" t="s">
+        <x:v>434</x:v>
+      </x:c>
+      <x:c r="F89" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="G89" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="H89" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="I89" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="J89" s="0" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="K89" s="0" t="s">
+        <x:v>439</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:28">
+      <x:c r="A90" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>442</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="F90" s="0" t="s">
+        <x:v>445</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:28">
+      <x:c r="A91" s="0" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="F91" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:28">
+      <x:c r="A92" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>453</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>454</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>455</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+      <x:c r="F92" s="0" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="G92" s="0" t="s">
+        <x:v>458</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:28">
+      <x:c r="A93" s="0" t="s">
+        <x:v>459</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>461</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>462</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="F93" s="0" t="s">
+        <x:v>463</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:28">
+      <x:c r="A94" s="0" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>465</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>466</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="F94" s="0" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="G94" s="0" t="s">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="H94" s="0" t="s">
+        <x:v>470</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:28">
+      <x:c r="A95" s="0" t="s">
+        <x:v>471</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>472</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>473</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>474</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>475</x:v>
+      </x:c>
+      <x:c r="F95" s="0" t="s">
+        <x:v>476</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:28">
+      <x:c r="A96" s="0" t="s">
+        <x:v>477</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>478</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>479</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="E96" s="0" t="s">
+        <x:v>481</x:v>
+      </x:c>
+      <x:c r="F96" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:28">
+      <x:c r="A97" s="0" t="s">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>484</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>485</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:28">
+      <x:c r="A98" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>488</x:v>
+      </x:c>
+      <x:c r="E98" s="0" t="s">
+        <x:v>489</x:v>
+      </x:c>
+      <x:c r="F98" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="G98" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="H98" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:28">
+      <x:c r="A99" s="0" t="s">
+        <x:v>492</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>493</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:28">
+      <x:c r="A100" s="0" t="s">
+        <x:v>494</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>495</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>496</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>488</x:v>
+      </x:c>
+      <x:c r="E100" s="0" t="s">
+        <x:v>497</x:v>
+      </x:c>
+      <x:c r="F100" s="0" t="s">
+        <x:v>498</x:v>
+      </x:c>
+      <x:c r="G100" s="0" t="s">
+        <x:v>499</x:v>
+      </x:c>
+      <x:c r="H100" s="0" t="s">
+        <x:v>500</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:28">
+      <x:c r="A101" s="0" t="s">
+        <x:v>501</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>502</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:28">
+      <x:c r="A102" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>503</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1609,7 +4685,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AE60"/>
+  <x:dimension ref="A1:AE98"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1617,15 +4693,15 @@
   <x:sheetData>
     <x:row r="1" spans="1:31">
       <x:c r="A1" s="1" t="s">
-        <x:v>101</x:v>
+        <x:v>504</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:31">
       <x:c r="A3" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>505</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>506</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
         <x:v>3</x:v>
@@ -1636,7 +4712,7 @@
     </x:row>
     <x:row r="5" spans="1:31">
       <x:c r="A5" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>507</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>6</x:v>
@@ -1645,7 +4721,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="R5" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>508</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:31">
@@ -1653,10 +4729,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>509</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>510</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:31">
@@ -1667,7 +4743,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>511</x:v>
       </x:c>
       <x:c r="R9" s="0" t="s">
         <x:v>8</x:v>
@@ -1678,50 +4754,50 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>512</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>513</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:31">
       <x:c r="A13" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>514</x:v>
       </x:c>
       <x:c r="N13" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>515</x:v>
       </x:c>
       <x:c r="Q13" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>516</x:v>
       </x:c>
       <x:c r="Z13" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>517</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:31">
       <x:c r="C14" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>518</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>519</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>520</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>521</x:v>
       </x:c>
       <x:c r="N14" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>522</x:v>
       </x:c>
       <x:c r="Q14" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>523</x:v>
       </x:c>
       <x:c r="V14" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>524</x:v>
       </x:c>
       <x:c r="Y14" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>525</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:31">
@@ -1729,37 +4805,37 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>123</x:v>
+        <x:v>526</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>124</x:v>
+        <x:v>527</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>125</x:v>
+        <x:v>528</x:v>
       </x:c>
       <x:c r="E15" s="1" t="s">
-        <x:v>126</x:v>
+        <x:v>529</x:v>
       </x:c>
       <x:c r="F15" s="1" t="s">
-        <x:v>127</x:v>
+        <x:v>530</x:v>
       </x:c>
       <x:c r="G15" s="1" t="s">
-        <x:v>128</x:v>
+        <x:v>531</x:v>
       </x:c>
       <x:c r="H15" s="1" t="s">
-        <x:v>129</x:v>
+        <x:v>532</x:v>
       </x:c>
       <x:c r="I15" s="1" t="s">
-        <x:v>130</x:v>
+        <x:v>533</x:v>
       </x:c>
       <x:c r="J15" s="1" t="s">
-        <x:v>131</x:v>
+        <x:v>534</x:v>
       </x:c>
       <x:c r="K15" s="1" t="s">
-        <x:v>132</x:v>
+        <x:v>535</x:v>
       </x:c>
       <x:c r="L15" s="1" t="s">
-        <x:v>133</x:v>
+        <x:v>536</x:v>
       </x:c>
       <x:c r="M15" s="1" t="s">
         <x:v>37</x:v>
@@ -1774,40 +4850,40 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="Q15" s="1" t="s">
-        <x:v>134</x:v>
+        <x:v>537</x:v>
       </x:c>
       <x:c r="R15" s="1" t="s">
-        <x:v>135</x:v>
+        <x:v>538</x:v>
       </x:c>
       <x:c r="S15" s="1" t="s">
-        <x:v>136</x:v>
+        <x:v>539</x:v>
       </x:c>
       <x:c r="T15" s="1" t="s">
-        <x:v>137</x:v>
+        <x:v>540</x:v>
       </x:c>
       <x:c r="U15" s="1" t="s">
         <x:v>46</x:v>
       </x:c>
       <x:c r="V15" s="1" t="s">
-        <x:v>138</x:v>
+        <x:v>541</x:v>
       </x:c>
       <x:c r="W15" s="1" t="s">
-        <x:v>139</x:v>
+        <x:v>542</x:v>
       </x:c>
       <x:c r="X15" s="1" t="s">
-        <x:v>140</x:v>
+        <x:v>543</x:v>
       </x:c>
       <x:c r="Y15" s="1" t="s">
-        <x:v>141</x:v>
+        <x:v>544</x:v>
       </x:c>
       <x:c r="Z15" s="1" t="s">
         <x:v>49</x:v>
       </x:c>
       <x:c r="AA15" s="1" t="s">
-        <x:v>142</x:v>
+        <x:v>545</x:v>
       </x:c>
       <x:c r="AB15" s="1" t="s">
-        <x:v>143</x:v>
+        <x:v>546</x:v>
       </x:c>
       <x:c r="AC15" s="1" t="s">
         <x:v>52</x:v>
@@ -1821,563 +4897,1071 @@
     </x:row>
     <x:row r="16" spans="1:31">
       <x:c r="A16" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>547</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>548</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>549</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>550</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>551</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>552</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>549</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>553</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>554</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:31">
       <x:c r="A17" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>555</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>556</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>557</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>558</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>559</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>560</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>561</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:31">
       <x:c r="A18" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>562</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>563</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>157</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
-      <x:c r="H18" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>564</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:31">
       <x:c r="A19" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>565</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>566</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>567</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>164</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-      <x:c r="F19" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-      <x:c r="G19" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>568</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:31">
       <x:c r="A20" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>569</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>570</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>571</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>171</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="F20" s="0" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="G20" s="0" t="s">
-        <x:v>173</x:v>
-      </x:c>
-      <x:c r="H20" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>572</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:31">
       <x:c r="A21" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>573</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>177</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>178</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="F21" s="0" t="s">
-        <x:v>179</x:v>
-      </x:c>
-      <x:c r="G21" s="0" t="s">
-        <x:v>180</x:v>
-      </x:c>
-      <x:c r="H21" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>574</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:31">
       <x:c r="A22" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>575</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>576</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>577</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>578</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>579</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>580</x:v>
+      </x:c>
+      <x:c r="H22" s="0" t="s">
+        <x:v>581</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:31">
       <x:c r="A23" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>582</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>583</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>584</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>585</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>586</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="s">
+        <x:v>587</x:v>
+      </x:c>
+      <x:c r="H23" s="0" t="s">
+        <x:v>588</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:31">
       <x:c r="A24" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>589</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>590</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>591</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>592</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>593</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="s">
+        <x:v>594</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:31">
       <x:c r="A25" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>595</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>596</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>597</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>598</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>599</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="s">
+        <x:v>600</x:v>
+      </x:c>
+      <x:c r="H25" s="0" t="s">
+        <x:v>601</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:31">
       <x:c r="A26" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>602</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>603</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>604</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>605</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>606</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="s">
+        <x:v>607</x:v>
+      </x:c>
+      <x:c r="H26" s="0" t="s">
+        <x:v>608</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:31">
       <x:c r="A27" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>609</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>610</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>611</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>612</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>613</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:31">
       <x:c r="A28" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>614</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>615</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>616</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>617</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>618</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:31">
       <x:c r="A29" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>619</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>620</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>621</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:31">
       <x:c r="A30" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>622</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>623</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>624</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:31">
       <x:c r="A31" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>625</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>626</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>627</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:31">
       <x:c r="A32" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>628</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>629</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>630</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:31">
       <x:c r="A33" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>631</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>632</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>633</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:31">
       <x:c r="A34" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>634</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>635</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>636</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>637</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:31">
       <x:c r="A35" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>638</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>639</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>640</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>641</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:31">
       <x:c r="A36" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>642</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>643</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>644</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>645</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:31">
       <x:c r="A37" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>646</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>647</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>648</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:31">
       <x:c r="A38" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>649</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>650</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>651</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:31">
       <x:c r="A39" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>652</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>653</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>654</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:31">
       <x:c r="A40" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>655</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>656</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>657</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>658</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:31">
       <x:c r="A41" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>659</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>660</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>661</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>662</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:31">
       <x:c r="A42" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>663</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>664</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>665</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>666</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:31">
       <x:c r="A43" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>667</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>668</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>669</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:31">
       <x:c r="A44" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>670</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>671</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>672</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>673</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:31">
       <x:c r="A45" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>674</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>675</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>676</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>677</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:31">
       <x:c r="A46" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>678</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>679</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>680</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:31">
       <x:c r="A47" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>681</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>682</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>683</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>684</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>685</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:31">
       <x:c r="A48" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>686</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>687</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>688</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:31">
       <x:c r="A49" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>689</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>690</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>691</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>692</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:31">
       <x:c r="A50" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>693</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>257</x:v>
+        <x:v>694</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>695</x:v>
       </x:c>
       <x:c r="D50" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>696</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:31">
       <x:c r="A51" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>697</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>698</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>699</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:31">
       <x:c r="A52" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>700</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="C52" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>701</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:31">
       <x:c r="A53" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>702</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>703</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>704</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:31">
       <x:c r="A54" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>705</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>254</x:v>
-      </x:c>
-      <x:c r="C54" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>706</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:31">
       <x:c r="A55" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>707</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>269</x:v>
-      </x:c>
-      <x:c r="C55" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>708</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:31">
       <x:c r="A56" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>709</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>272</x:v>
-      </x:c>
-      <x:c r="C56" s="0" t="s">
-        <x:v>254</x:v>
-      </x:c>
-      <x:c r="D56" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>710</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:31">
       <x:c r="A57" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>711</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>275</x:v>
-      </x:c>
-      <x:c r="C57" s="0" t="s">
-        <x:v>254</x:v>
-      </x:c>
-      <x:c r="D57" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>712</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:31">
       <x:c r="A58" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>713</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>714</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:31">
       <x:c r="A59" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>715</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>279</x:v>
-      </x:c>
-      <x:c r="C59" s="0" t="s">
-        <x:v>280</x:v>
-      </x:c>
-      <x:c r="D59" s="0" t="s">
-        <x:v>281</x:v>
-      </x:c>
-      <x:c r="E59" s="0" t="s">
-        <x:v>282</x:v>
-      </x:c>
-      <x:c r="F59" s="0" t="s">
-        <x:v>283</x:v>
-      </x:c>
-      <x:c r="G59" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="H59" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="I59" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>716</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:31">
       <x:c r="A60" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>717</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>285</x:v>
-      </x:c>
-      <x:c r="C60" s="0" t="s">
-        <x:v>286</x:v>
-      </x:c>
-      <x:c r="D60" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>718</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:31">
+      <x:c r="A61" s="0" t="s">
+        <x:v>719</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>720</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:31">
+      <x:c r="A62" s="0" t="s">
+        <x:v>721</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>722</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>723</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:31">
+      <x:c r="A63" s="0" t="s">
+        <x:v>724</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>725</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>726</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:31">
+      <x:c r="A64" s="0" t="s">
+        <x:v>727</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>728</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>729</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:31">
+      <x:c r="A65" s="0" t="s">
+        <x:v>730</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>731</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>732</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:31">
+      <x:c r="A66" s="0" t="s">
+        <x:v>733</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>734</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>735</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:31">
+      <x:c r="A67" s="0" t="s">
+        <x:v>736</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>737</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>738</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:31">
+      <x:c r="A68" s="0" t="s">
+        <x:v>739</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>740</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>741</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:31">
+      <x:c r="A69" s="0" t="s">
+        <x:v>742</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>743</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:31">
+      <x:c r="A70" s="0" t="s">
+        <x:v>744</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>745</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:31">
+      <x:c r="A71" s="0" t="s">
+        <x:v>746</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>747</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:31">
+      <x:c r="A72" s="0" t="s">
+        <x:v>748</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>749</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:31">
+      <x:c r="A73" s="0" t="s">
+        <x:v>750</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>751</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>752</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:31">
+      <x:c r="A74" s="0" t="s">
+        <x:v>753</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>754</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:31">
+      <x:c r="A75" s="0" t="s">
+        <x:v>755</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>756</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:31">
+      <x:c r="A76" s="0" t="s">
+        <x:v>757</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>758</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:31">
+      <x:c r="A77" s="0" t="s">
+        <x:v>759</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>760</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>761</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:31">
+      <x:c r="A78" s="0" t="s">
+        <x:v>762</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>763</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:31">
+      <x:c r="A79" s="0" t="s">
+        <x:v>764</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>765</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>766</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:31">
+      <x:c r="A80" s="0" t="s">
+        <x:v>767</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>768</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:31">
+      <x:c r="A81" s="0" t="s">
+        <x:v>769</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>770</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:31">
+      <x:c r="A82" s="0" t="s">
+        <x:v>771</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>772</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>773</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:31">
+      <x:c r="A83" s="0" t="s">
+        <x:v>774</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>775</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>776</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:31">
+      <x:c r="A84" s="0" t="s">
+        <x:v>777</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>778</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:31">
+      <x:c r="A85" s="0" t="s">
+        <x:v>779</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>780</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>781</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:31">
+      <x:c r="A86" s="0" t="s">
+        <x:v>782</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>765</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>783</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:31">
+      <x:c r="A87" s="0" t="s">
+        <x:v>784</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>785</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>786</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:31">
+      <x:c r="A88" s="0" t="s">
+        <x:v>787</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>788</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>789</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:31">
+      <x:c r="A89" s="0" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>791</x:v>
+      </x:c>
+      <x:c r="C89" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D89" s="0" t="s">
+        <x:v>792</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:31">
+      <x:c r="A90" s="0" t="s">
+        <x:v>793</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>794</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>795</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:31">
+      <x:c r="A91" s="0" t="s">
+        <x:v>796</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>797</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>798</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:31">
+      <x:c r="A92" s="0" t="s">
+        <x:v>799</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>800</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>801</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:31">
+      <x:c r="A93" s="0" t="s">
+        <x:v>802</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>803</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>804</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:31">
+      <x:c r="A94" s="0" t="s">
+        <x:v>805</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>806</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>807</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:31">
+      <x:c r="A95" s="0" t="s">
+        <x:v>808</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>809</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>810</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:31">
+      <x:c r="A96" s="0" t="s">
+        <x:v>492</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>811</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:31">
+      <x:c r="A97" s="0" t="s">
+        <x:v>812</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>813</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>814</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>815</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
+        <x:v>816</x:v>
+      </x:c>
+      <x:c r="F97" s="0" t="s">
+        <x:v>817</x:v>
+      </x:c>
+      <x:c r="G97" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="H97" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="I97" s="0" t="s">
+        <x:v>818</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:31">
+      <x:c r="A98" s="0" t="s">
+        <x:v>501</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>819</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>820</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>821</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement regex-based row splitting and improved filtering
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -149,52 +149,16 @@
     <x:t xml:space="preserve">PLC_MAPPING   OBJECT_NAME    </x:t>
   </x:si>
   <x:si>
-    <x:t>Noe POINT NAME 708 cont — IMTERPOSNG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INTERPOSING aie CRD ae RW NO: —— case No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>‘DIA INNNOON Noe POINT NAME 78 cont — TMTERPOGNE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INTERPOSING OIG a OUTPUT —— CASE NO.) DIAG. iNNOON</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DEC STATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 DSCRPT }0 DSCRIPT] RELAY NO.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RELAY NO.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>rwpuyr no.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>output No. (MoD-Priop-pr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“NOTE 3)) wc. Dec STATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>teem carp! TERM carp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MoD-PtiMoo-pr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NOTE 3)) owe.</x:t>
-  </x:si>
-  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
     <x:t>RTU MONITOR (JUMPER) CONTROL INHIBIT 0 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM — — [or t-t — = = = 81__</x:t>
+    <x:t>ALARM — — [or t-t — = = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81__</x:t>
   </x:si>
   <x:si>
     <x:t>{GATE ~\ 79 1C7 96-24T/C</x:t>
@@ -209,7 +173,10 @@
     <x:t>STINGER SWITCH 115KV 1 1 auto</x:t>
   </x:si>
   <x:si>
-    <x:t>SOLID = — [or 1-2 = 10 = 82</x:t>
+    <x:t>SOLID = — [or 1-2 = 10 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82</x:t>
   </x:si>
   <x:si>
     <x:t>FUPS TROUBLE F 80 1c8 DI 6-81 — W59</x:t>
@@ -233,7 +200,10 @@
     <x:t>[INYO 115KV CB 2 [3 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-2/AT RK Z — [or 1-4 [Rm 1-374 1B, 2A _ 84</x:t>
+    <x:t>95-2/AT RK Z — [or 1-4 [Rm 1-374 1B, 2A _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>84</x:t>
   </x:si>
   <x:si>
     <x:t>115KV RELAY BUS AL 82 95-2 DI 6-83 = W61</x:t>
@@ -275,7 +245,10 @@
     <x:t>95-7/AT RK 234 — [or t-7__ [RM 2-9/10 1B, 2A</x:t>
   </x:si>
   <x:si>
-    <x:t>5640030 = 87_</x:t>
+    <x:t>5640030 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>87_</x:t>
   </x:si>
   <x:si>
     <x:t>115KV ELECTRONIC BUS AL 85 95-5 = DI 6-86 = W64</x:t>
@@ -287,7 +260,10 @@
     <x:t>COSO-HAIWEE-INYOKERN 115KV CB 9 7 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-9/AT RK 235 — [or i-8 [RM 2-11712 1B, 24</x:t>
+    <x:t>95-9/AT RK 235 — [or i-8 [RM 2-11712 1B,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
   </x:si>
   <x:si>
     <x:t>5640034 = 88__</x:t>
@@ -305,7 +281,10 @@
     <x:t>8 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-15/AT RK Z —  fori-9 [RM 2-13/14 1B, 2A = 89_</x:t>
+    <x:t>95-15/AT RK Z —  fori-9 [RM 2-13/14 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>89_</x:t>
   </x:si>
   <x:si>
     <x:t>115KV _LBFB BUS 87 95-7 = DI 6-88 — W66</x:t>
@@ -314,7 +293,10 @@
     <x:t>10 [lOXBOW 115KV CB 17 lg 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-I7/AT RK Z — [or 1-10 [RM 2-15/16 1B, 2A = 90 __</x:t>
+    <x:t>95-I7/AT RK Z — [or 1-10 [RM 2-15/16 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>90 __</x:t>
   </x:si>
   <x:si>
     <x:t>115KV INTERFACE BUS 88 95-8 = DI 6-89 = W67</x:t>
@@ -326,7 +308,10 @@
     <x:t>/OXBOW CUST CB I} 10 1 CLOSE OPEN</x:t>
   </x:si>
   <x:si>
-    <x:t>95- X/AT RK Z = DI 1-11 [RM 3-17/18 1B, 2A = 91 __</x:t>
+    <x:t>95- X/AT RK Z = DI 1-11 [RM 3-17/18 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>91 __</x:t>
   </x:si>
   <x:si>
     <x:t>E115KVFMETER BUS F 89 95-9 = DI 6-90 = W68</x:t>
@@ -335,7 +320,10 @@
     <x:t>12 [WWIXIE VALLEY CUST CBF Tn 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A = 92_</x:t>
+    <x:t>95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>92_</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 90 = DI 6-91 = = W69</x:t>
@@ -347,7 +335,7 @@
     <x:t>BUS TIE 115KV CB 23 12 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B, 24</x:t>
+    <x:t>95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B,</x:t>
   </x:si>
   <x:si>
     <x:t>5640038 = 93__</x:t>
@@ -362,7 +350,10 @@
     <x:t>SPARE 3 [—</x:t>
   </x:si>
   <x:si>
-    <x:t>— = = = — [or 1-14 [RM 3-23/24 = = = 94 _</x:t>
+    <x:t>— = = = — [or 1-14 [RM 3-23/24 = = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>94 _</x:t>
   </x:si>
   <x:si>
     <x:t>(115KV W/BUS POT ALE 92 = DI 6-93 = Ww</x:t>
@@ -374,7 +365,10 @@
     <x:t>SPARE 4f{[—</x:t>
   </x:si>
   <x:si>
-    <x:t>[— = = = — [or 1-15 [RM 4-25/26 = = = 95 _</x:t>
+    <x:t>[— = = = — [or 1-15 [RM 4-25/26 = = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95 _</x:t>
   </x:si>
   <x:si>
     <x:t>LI5KV_E/BUS POT ALJ 93 = DI 6-94 = W712</x:t>
@@ -383,7 +377,10 @@
     <x:t>16 [fNO. 1 BANK T15KV CB 11) 15 1 CLOSE</x:t>
   </x:si>
   <x:si>
-    <x:t>95-1I/AT RK Z — [or 1-16 [RM 4-27/28 1B, 2A = 96 _</x:t>
+    <x:t>95-1I/AT RK Z — [or 1-16 [RM 4-27/28 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>96 _</x:t>
   </x:si>
   <x:si>
     <x:t>LOW DC VOLTAGE 94 1c-9 = DI 6-95 = W713</x:t>
@@ -395,7 +392,10 @@
     <x:t>95-13/AT RK Z _— DI 2-17</x:t>
   </x:si>
   <x:si>
-    <x:t>RM 4-29/30 1B, 2A _ 97</x:t>
+    <x:t>RM 4-29/30 1B, 2A _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>97</x:t>
   </x:si>
   <x:si>
     <x:t>BATT CHG FAIL FAIL LOSS OF AC 95 1C-10 _— DI 6-96 _— w74</x:t>
@@ -416,7 +416,10 @@
     <x:t>ENTRY ALARM 18 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM TAI — [or 2-19 = 8 = 99 _</x:t>
+    <x:t>ALARM TAI — [or 2-19 = 8 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>99 _</x:t>
   </x:si>
   <x:si>
     <x:t>NEGATIVE DC GRD 97 1C-12 = DI 7-98 = 4 W76</x:t>
@@ -428,7 +431,10 @@
     <x:t>fi1S5KV CB LOW GAS7AIR 19 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM TA2 — [pI 2-20 = 6C W1 100</x:t>
+    <x:t>ALARM TA2 — [pI 2-20 = 6C W1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100</x:t>
   </x:si>
   <x:si>
     <x:t>(SEL-2030 FAIL -—~—~~~~—~\({—«C98 1C-13 = DI 7-99 = 4 WT?</x:t>
@@ -482,7 +488,10 @@
     <x:t>23 o</x:t>
   </x:si>
   <x:si>
-    <x:t>NORMAL 1A6 — [pr 2-24 = 6B W4 104</x:t>
+    <x:t>NORMAL 1A6 — [pr 2-24 = 6B W4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>104</x:t>
   </x:si>
   <x:si>
     <x:t>INO. 3 BANK TAP RAISE/LOWER I</x:t>
@@ -500,7 +509,10 @@
     <x:t>24 o</x:t>
   </x:si>
   <x:si>
-    <x:t>NORMAL TAT — [or 2-25 — 6B W5 105 _</x:t>
+    <x:t>NORMAL TAT — [or 2-25 — 6B W5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>105 _</x:t>
   </x:si>
   <x:si>
     <x:t>ISPARE I] 103 = = DI 7-104 [RM 6-45/46 4 — W82</x:t>
@@ -515,7 +527,10 @@
     <x:t>25 o</x:t>
   </x:si>
   <x:si>
-    <x:t>NORMAL 1A8 — [or 2-26 — 6B W6 106</x:t>
+    <x:t>NORMAL 1A8 — [or 2-26 — 6B W6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>106</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE JI 104 = — DI 7-105 _ 4 W83</x:t>
@@ -611,7 +626,10 @@
     <x:t>— = = 1A14 —</x:t>
   </x:si>
   <x:si>
-    <x:t>or 2-32 = = = wi2 112</x:t>
+    <x:t>or 2-32 = = = wi2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>112</x:t>
   </x:si>
   <x:si>
     <x:t>110 ici? = DI ?-111 — 4 W88</x:t>
@@ -677,7 +695,7 @@
     <x:t>[NO. 3 BANKFITM FAI ) 36 0 [ ALARM</x:t>
   </x:si>
   <x:si>
-    <x:t>NORMAL TAS — [or 3-37 — 6B WI7 7</x:t>
+    <x:t>NORMAL TAS — [or 3-37 — 6B WI7</x:t>
   </x:si>
   <x:si>
     <x:t>I] 115 = DI 8-116 = =</x:t>
@@ -725,7 +743,10 @@
     <x:t>41</x:t>
   </x:si>
   <x:si>
-    <x:t>FTRANS BK SUDDENTPRESS RESET “1 - = = — [RM 5-33/34 28 = 121</x:t>
+    <x:t>FTRANS BK SUDDENTPRESS RESET “1 - = = — [RM 5-33/34 28 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>121</x:t>
   </x:si>
   <x:si>
     <x:t>F I] 119 1024 DI 8-120 = w96</x:t>
@@ -743,7 +764,10 @@
     <x:t>ALARM 1A23 —</x:t>
   </x:si>
   <x:si>
-    <x:t>or 3-41 — 6B W21 122</x:t>
+    <x:t>or 3-41 — 6B W21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>122</x:t>
   </x:si>
   <x:si>
     <x:t>120 = DI 8-121 = WoT</x:t>
@@ -755,7 +779,10 @@
     <x:t>INO. 1 BANK SEL-387 DIFF TRIP Ifa 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1A24 — [pr 3-42 = 6B W22 123</x:t>
+    <x:t>ALARM 1A24 — [pr 3-42 = 6B W22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123</x:t>
   </x:si>
   <x:si>
     <x:t>I 121 — DI 8-122 [RM 7-53/54 =</x:t>
@@ -770,7 +797,10 @@
     <x:t>42 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B1 — [or 3-43 = 6B W23 124</x:t>
+    <x:t>ALARM 1B1 — [or 3-43 = 6B W23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>124</x:t>
   </x:si>
   <x:si>
     <x:t>L RESERVED FOR 115KV LINE Pos. 1__l</x:t>
@@ -788,7 +818,10 @@
     <x:t>4 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B2 _— DI 3-44 _ 6B W24 125</x:t>
+    <x:t>ALARM 1B2 _— DI 3-44 _ 6B W24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>125</x:t>
   </x:si>
   <x:si>
     <x:t>[ PROTECTION RELAYS ALARMS I 123 1D-2 DI 8-124 — w99</x:t>
@@ -803,7 +836,10 @@
     <x:t>44 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B3 — [or 3-45 — 6B W25 126</x:t>
+    <x:t>ALARM 1B3 — [or 3-45 — 6B W25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>126</x:t>
   </x:si>
   <x:si>
     <x:t>I] 124 10-3 DI 8-125 = W100</x:t>
@@ -815,7 +851,10 @@
     <x:t>45 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B4 — [ol 3-46 = 6B W26 127</x:t>
+    <x:t>ALARM 1B4 — [ol 3-46 = 6B W26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>127</x:t>
   </x:si>
   <x:si>
     <x:t>I] 125 10-4 DI 8-126 _— W101</x:t>
@@ -830,7 +869,10 @@
     <x:t>47 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B6 — [or 3-48 — 6B W28 129</x:t>
+    <x:t>ALARM 1B6 — [or 3-48 — 6B W28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>129</x:t>
   </x:si>
   <x:si>
     <x:t>127 = DI 8-128 [RM 7-55/56 =</x:t>
@@ -845,7 +887,10 @@
     <x:t>48 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 187 — [or 4-49 — 6B W29 130</x:t>
+    <x:t>ALARM 187 — [or 4-49 — 6B W29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>130</x:t>
   </x:si>
   <x:si>
     <x:t>F[_ 128 10-5 DI 9-129 = W103 " ane SINE RO SSE TRIPPING RECS.</x:t>
@@ -860,7 +905,10 @@
     <x:t>49 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B8 —  [dI 4-50 = 6B W30 131</x:t>
+    <x:t>ALARM 1B8 —  [dI 4-50 = 6B W30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>131</x:t>
   </x:si>
   <x:si>
     <x:t>129 10-6 DI 9-130 — W104 AN INDICATION IS TAKEN FROM EACH</x:t>
@@ -887,7 +935,10 @@
     <x:t>53 NO. 3 BANK C30 FAIL I] 51 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B10 — [ol 4-52 = 6B W32 133</x:t>
+    <x:t>ALARM 1B10 — [ol 4-52 = 6B W32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>133</x:t>
   </x:si>
   <x:si>
     <x:t>I] 131 10-8 DI 9-132 = W106 .</x:t>
@@ -902,7 +953,10 @@
     <x:t>52 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B11 — DI 4-53 = 6B W33 134</x:t>
+    <x:t>ALARM 1B11 — DI 4-53 = 6B W33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>134</x:t>
   </x:si>
   <x:si>
     <x:t>I 132 = DI 9-133 — W107 2. OY IN A BLOCK INDICATES A VIRTUAL</x:t>
@@ -929,7 +983,10 @@
     <x:t>115KV_UNDERFREQ POT FAIL 54 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>74/AT RK Z58 —_ DI 4-55 a 3 5704102 W35 136_</x:t>
+    <x:t>74/AT RK Z58 —_ DI 4-55 a 3 5704102 W35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>136_</x:t>
   </x:si>
   <x:si>
     <x:t>_l RESERVED FOR 115KV LINE POS. 2_</x:t>
@@ -950,7 +1007,10 @@
     <x:t>or 4-56 = 6A</x:t>
   </x:si>
   <x:si>
-    <x:t>5704103 W36 137_</x:t>
+    <x:t>5704103 W36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>137_</x:t>
   </x:si>
   <x:si>
     <x:t>F [PROTECTION RELAYS ALARMS i135 10-10 DI 9-136</x:t>
@@ -968,7 +1028,10 @@
     <x:t>56 1 NORMAL</x:t>
   </x:si>
   <x:si>
-    <x:t>ALARM 1B15 — [ol 4-57 6A 5640043 W37 138</x:t>
+    <x:t>ALARM 1B15 — [ol 4-57 6A 5640043 W37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>138</x:t>
   </x:si>
   <x:si>
     <x:t>I! 136 10-11 DI 9-137 — WH10 "WA BLOCK MEANS THAT NO</x:t>
@@ -986,7 +1049,10 @@
     <x:t>ALARM 1B16 —</x:t>
   </x:si>
   <x:si>
-    <x:t>ol 4-58 = 6A 5640043 W438 139</x:t>
+    <x:t>ol 4-58 = 6A 5640043 W438</x:t>
+  </x:si>
+  <x:si>
+    <x:t>139</x:t>
   </x:si>
   <x:si>
     <x:t>137 10-12 DI 9-138 = Witt DATA IS APPLICABLE FOR THAT BLOCK.</x:t>
@@ -1004,7 +1070,10 @@
     <x:t>ALARM 1B17 — [oI 459 = 6A</x:t>
   </x:si>
   <x:si>
-    <x:t>5640046 W39 140</x:t>
+    <x:t>5640046 W39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>140</x:t>
   </x:si>
   <x:si>
     <x:t>138 = DI 9-139 = Wi12</x:t>
@@ -1067,7 +1136,10 @@
     <x:t>ALARM = — [di 4-63 = 6A</x:t>
   </x:si>
   <x:si>
-    <x:t>5640046 W43 144</x:t>
+    <x:t>5640046 W43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>144</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-INYOKERN 115KVID6O</x:t>
@@ -1127,7 +1199,10 @@
     <x:t>dI 5-65 = 6B</x:t>
   </x:si>
   <x:si>
-    <x:t>5640062 W45 146</x:t>
+    <x:t>5640062 W45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>146</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
@@ -1148,7 +1223,10 @@
     <x:t>oI 5-66 = 6B</x:t>
   </x:si>
   <x:si>
-    <x:t>5640062 Ww46 147</x:t>
+    <x:t>5640062 Ww46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>147</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL[ 145 1 NORMAL</x:t>
@@ -1190,7 +1268,10 @@
     <x:t>ALARM 1822 — [br 5-68 = 6B</x:t>
   </x:si>
   <x:si>
-    <x:t>5704103 w48 149</x:t>
+    <x:t>5704103 w48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>149</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
@@ -1208,7 +1289,10 @@
     <x:t>FCASA DIABLO REACTOR CS 7} 68 95-21/AT RK Z —</x:t>
   </x:si>
   <x:si>
-    <x:t>or 5-69 = 1B, 2A = 150</x:t>
+    <x:t>or 5-69 = 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>150</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
@@ -1235,7 +1319,7 @@
     <x:t>69 1C1 = DI 5-70 = 6A wag</x:t>
   </x:si>
   <x:si>
-    <x:t>904562794 “Ts 7</x:t>
+    <x:t>904562794 “Ts</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN T15KV{D60) TRIP</x:t>
@@ -1259,7 +1343,10 @@
     <x:t>ICASA DIABLO REACTOR UV ] 70 1¢2 —</x:t>
   </x:si>
   <x:si>
-    <x:t>[ors-71 = 6A W50 152</x:t>
+    <x:t>[ors-71 = 6A W50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>152</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV(D60[RLY FAIL 150 1 NORMAL</x:t>
@@ -1283,7 +1370,10 @@
     <x:t>— __</x:t>
   </x:si>
   <x:si>
-    <x:t>DI 5-72 = 1B, 2A = 153</x:t>
+    <x:t>DI 5-72 = 1B, 2A =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>153</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV[D60/A/S</x:t>
@@ -1310,7 +1400,10 @@
     <x:t>ICASA D-SHERWIN REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>72 1C3 — [or 5-73 = 6A W51 154</x:t>
+    <x:t>72 1C3 — [or 5-73 = 6A W51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>154</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
@@ -1328,7 +1421,10 @@
     <x:t>FCASA D-SHERWIN REACTOR UV ] 3 1c4 —</x:t>
   </x:si>
   <x:si>
-    <x:t>or 5-74 = 6A W52 155</x:t>
+    <x:t>or 5-74 = 6A W52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>155</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
@@ -1349,7 +1445,10 @@
     <x:t>— _—‘</x:t>
   </x:si>
   <x:si>
-    <x:t>DI 5-75 = 4 W53 156</x:t>
+    <x:t>DI 5-75 = 4 W53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>156</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
@@ -1364,7 +1463,10 @@
     <x:t>77</x:t>
   </x:si>
   <x:si>
-    <x:t>REACTOR DC BACK-UP BUS AL ] 15 95-8 AT C3 — [ol 5-76 = 4 W54 157</x:t>
+    <x:t>REACTOR DC BACK-UP BUS AL ] 15 95-8 AT C3 — [ol 5-76 = 4 W54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>157</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
@@ -1379,7 +1481,10 @@
     <x:t>78</x:t>
   </x:si>
   <x:si>
-    <x:t>REACTOR OPERATING BUS AL F 16 95-9 AT C3 — [or 5-7 = 4 W55 158</x:t>
+    <x:t>REACTOR OPERATING BUS AL F 16 95-9 AT C3 — [or 5-7 = 4 W55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>158</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
@@ -1403,7 +1508,10 @@
     <x:t>TT 105 —</x:t>
   </x:si>
   <x:si>
-    <x:t>p 5-78 = 6A W56 159</x:t>
+    <x:t>p 5-78 = 6A W56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>159</x:t>
   </x:si>
   <x:si>
     <x:t>HATWEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
@@ -1421,7 +1529,10 @@
     <x:t>[CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>78 1C6 — [or 5-79 = 6A W57 160</x:t>
+    <x:t>78 1C6 — [or 5-79 = 6A W57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>160</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
@@ -1583,24 +1694,6 @@
     <x:t>ANNUNCTATOR</x:t>
   </x:si>
   <x:si>
-    <x:t>NUMBER Bee CONT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NORIML) 1 DscRPT 0 DSCRIPT] RELAY NO.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RELAY NO. TNT NO ouPUy NO. MODPT alee (NOTE 3)] we. WINDOW NUMBER Fee PCONT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NORMAL)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DscRPT 0 DSCRIPT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RELAY NO. TNT NS oupuy io. MPT MOT (NOTE 3)} pwc. WINDOW</x:t>
-  </x:si>
-  <x:si>
     <x:t>161</x:t>
   </x:si>
   <x:si>
@@ -1775,7 +1868,10 @@
     <x:t>172 [i RESERVED FOR 115KV LINE Pos. 7_[</x:t>
   </x:si>
   <x:si>
-    <x:t>170 1 1E9 DI 11-171 W138 252 _</x:t>
+    <x:t>170 1 1E9 DI 11-171 W138</x:t>
+  </x:si>
+  <x:si>
+    <x:t>252 _</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 250 16-22 DI 15-235 W199</x:t>
@@ -1784,7 +1880,10 @@
     <x:t>173_</x:t>
   </x:si>
   <x:si>
-    <x:t>I_{ PROTECTION RELAYS ALARMS FY a7 1 1E10 DI 11-172 W139 253_</x:t>
+    <x:t>I_{ PROTECTION RELAYS ALARMS FY a7 1 1E10 DI 11-172 W139</x:t>
+  </x:si>
+  <x:si>
+    <x:t>253_</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 251 16-23 DI 15-236 W200</x:t>
@@ -1910,7 +2009,10 @@
     <x:t>{ PROTECTION RELAYS ALARMS</x:t>
   </x:si>
   <x:si>
-    <x:t>183 1 1E18 DI 12-184 149 265 _</x:t>
+    <x:t>183 1 1E18 DI 12-184 149</x:t>
+  </x:si>
+  <x:si>
+    <x:t>265 _</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 263 = DI 16-248]RM 10-79/80 =</x:t>
@@ -1976,7 +2078,10 @@
     <x:t>191</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV LBFB ARMED 189 1 1F1 DI 12-190 NOTE 4 W154 271</x:t>
+    <x:t>115KV LBFB ARMED 189 1 1F1 DI 12-190 NOTE 4 W154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>271</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 269 _ DI 16-254]RM 12-91/92 _</x:t>
@@ -1985,7 +2090,10 @@
     <x:t>192</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV LBFB TRIP 190 1 1F2 DI 12-191 NOTE 4 W155 272_</x:t>
+    <x:t>115KV LBFB TRIP 190 1 1F2 DI 12-191 NOTE 4 W155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>272_</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 270 = DI 16-255</x:t>
@@ -2000,7 +2108,10 @@
     <x:t>(15KV CB I'LBFB RELAY PS % FAIL \</x:t>
   </x:si>
   <x:si>
-    <x:t>191 1 1F3 DI 12-192 W156 273</x:t>
+    <x:t>191 1 1F3 DI 12-192 W156</x:t>
+  </x:si>
+  <x:si>
+    <x:t>273</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE on = DI 16-256]/RM 12-95/96 =</x:t>
@@ -2693,7 +2804,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:W96"/>
+  <x:dimension ref="A1:W147"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -2857,1572 +2968,1788 @@
       <x:c r="C16" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
     </x:row>
     <x:row r="17" spans="1:23">
       <x:c r="A17" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
+      <x:c r="C17" s="0" t="s">
         <x:v>49</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="F17" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="G17" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="I17" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="J17" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="K17" s="0" t="s">
-        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:23">
       <x:c r="A18" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:23">
       <x:c r="A19" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:23">
       <x:c r="A20" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:23">
       <x:c r="A21" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:23">
       <x:c r="A22" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="E22" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:23">
       <x:c r="A23" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
         <x:v>68</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="E23" s="0" t="s">
-        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:23">
       <x:c r="A24" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="F24" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:23">
       <x:c r="A25" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="F25" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:23">
       <x:c r="A26" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="F26" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:23">
       <x:c r="A27" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:23">
       <x:c r="A28" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:23">
       <x:c r="A29" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:23">
       <x:c r="A30" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>109</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="E30" s="0" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="F30" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:23">
       <x:c r="A31" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>115</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:23">
       <x:c r="A32" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="C32" s="0" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:23">
       <x:c r="A33" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>122</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:23">
       <x:c r="A34" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>125</x:v>
-      </x:c>
-      <x:c r="C34" s="0" t="s">
-        <x:v>126</x:v>
-      </x:c>
-      <x:c r="D34" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:23">
       <x:c r="A35" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:23">
       <x:c r="A36" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>132</x:v>
-      </x:c>
-      <x:c r="C36" s="0" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="D36" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:23">
       <x:c r="A37" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:23">
       <x:c r="A38" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>141</x:v>
-      </x:c>
-      <x:c r="D38" s="0" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="E38" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:23">
       <x:c r="A39" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="D39" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:23">
       <x:c r="A40" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>149</x:v>
-      </x:c>
-      <x:c r="C40" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="D40" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:23">
       <x:c r="A41" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="D41" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="E41" s="0" t="s">
-        <x:v>155</x:v>
-      </x:c>
-      <x:c r="F41" s="0" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="G41" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:23">
       <x:c r="A42" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
-      <x:c r="C42" s="0" t="s">
-        <x:v>160</x:v>
-      </x:c>
-      <x:c r="D42" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="E42" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="F42" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:23">
       <x:c r="A43" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-      <x:c r="D43" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="E43" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-      <x:c r="F43" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:23">
       <x:c r="A44" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="C44" s="0" t="s">
-        <x:v>169</x:v>
-      </x:c>
-      <x:c r="D44" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
-      <x:c r="E44" s="0" t="s">
-        <x:v>171</x:v>
-      </x:c>
-      <x:c r="F44" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:23">
       <x:c r="A45" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
-        <x:v>175</x:v>
-      </x:c>
-      <x:c r="D45" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="E45" s="0" t="s">
-        <x:v>176</x:v>
-      </x:c>
-      <x:c r="F45" s="0" t="s">
-        <x:v>177</x:v>
-      </x:c>
-      <x:c r="G45" s="0" t="s">
-        <x:v>178</x:v>
-      </x:c>
-      <x:c r="H45" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:23">
       <x:c r="A46" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>181</x:v>
-      </x:c>
-      <x:c r="C46" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="D46" s="0" t="s">
-        <x:v>182</x:v>
-      </x:c>
-      <x:c r="E46" s="0" t="s">
-        <x:v>183</x:v>
-      </x:c>
-      <x:c r="F46" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="G46" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:23">
       <x:c r="A47" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="D47" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:23">
       <x:c r="A48" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="D48" s="0" t="s">
-        <x:v>192</x:v>
-      </x:c>
-      <x:c r="E48" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="F48" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:23">
       <x:c r="A49" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>196</x:v>
-      </x:c>
-      <x:c r="C49" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="D49" s="0" t="s">
-        <x:v>197</x:v>
-      </x:c>
-      <x:c r="E49" s="0" t="s">
-        <x:v>198</x:v>
-      </x:c>
-      <x:c r="F49" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="G49" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:23">
       <x:c r="A50" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="D50" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-      <x:c r="E50" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:23">
       <x:c r="A51" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>205</x:v>
-      </x:c>
-      <x:c r="C51" s="0" t="s">
-        <x:v>206</x:v>
-      </x:c>
-      <x:c r="D51" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:23">
       <x:c r="A52" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D52" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="E52" s="0" t="s">
-        <x:v>211</x:v>
-      </x:c>
-      <x:c r="F52" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="G52" s="0" t="s">
-        <x:v>213</x:v>
-      </x:c>
-      <x:c r="H52" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:23">
       <x:c r="A53" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D53" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:23">
       <x:c r="A54" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D54" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:23">
       <x:c r="A55" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D55" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="s">
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:23">
       <x:c r="A56" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="D56" s="0" t="s">
-        <x:v>228</x:v>
-      </x:c>
-      <x:c r="E56" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:23">
       <x:c r="A57" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D57" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="E57" s="0" t="s">
-        <x:v>233</x:v>
-      </x:c>
-      <x:c r="F57" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:23">
       <x:c r="A58" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>236</x:v>
-      </x:c>
-      <x:c r="C58" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:23">
       <x:c r="A59" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D59" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="E59" s="0" t="s">
-        <x:v>242</x:v>
-      </x:c>
-      <x:c r="F59" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="G59" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:23">
       <x:c r="A60" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>245</x:v>
-      </x:c>
-      <x:c r="C60" s="0" t="s">
-        <x:v>246</x:v>
-      </x:c>
-      <x:c r="D60" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:23">
       <x:c r="A61" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="D61" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="E61" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F61" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:23">
       <x:c r="A62" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="D62" s="0" t="s">
-        <x:v>257</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="E62" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="F62" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="G62" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="H62" s="0" t="s">
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:23">
       <x:c r="A63" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D63" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="E63" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="F63" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="G63" s="0" t="s">
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:23">
       <x:c r="A64" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D64" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:23">
       <x:c r="A65" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D65" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E65" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="F65" s="0" t="s">
+        <x:v>199</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:23">
       <x:c r="A66" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
-        <x:v>275</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D66" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="E66" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:23">
       <x:c r="A67" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>279</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
-        <x:v>280</x:v>
-      </x:c>
-      <x:c r="D67" s="0" t="s">
-        <x:v>281</x:v>
-      </x:c>
-      <x:c r="E67" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="F67" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>205</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:23">
       <x:c r="A68" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D68" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E68" s="0" t="s">
-        <x:v>287</x:v>
-      </x:c>
-      <x:c r="F68" s="0" t="s">
-        <x:v>288</x:v>
+        <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:23">
       <x:c r="A69" s="0" t="s">
-        <x:v>289</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>290</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:23">
       <x:c r="A70" s="0" t="s">
-        <x:v>292</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>293</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
-        <x:v>294</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D70" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="E70" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="F70" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="G70" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="H70" s="0" t="s">
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:23">
       <x:c r="A71" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
-        <x:v>299</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="D71" s="0" t="s">
-        <x:v>300</x:v>
-      </x:c>
-      <x:c r="E71" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:23">
       <x:c r="A72" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="D72" s="0" t="s">
-        <x:v>304</x:v>
-      </x:c>
-      <x:c r="E72" s="0" t="s">
-        <x:v>305</x:v>
-      </x:c>
-      <x:c r="F72" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:23">
       <x:c r="A73" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>308</x:v>
-      </x:c>
-      <x:c r="C73" s="0" t="s">
-        <x:v>309</x:v>
-      </x:c>
-      <x:c r="D73" s="0" t="s">
-        <x:v>310</x:v>
-      </x:c>
-      <x:c r="E73" s="0" t="s">
-        <x:v>311</x:v>
-      </x:c>
-      <x:c r="F73" s="0" t="s">
-        <x:v>312</x:v>
-      </x:c>
-      <x:c r="G73" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:23">
       <x:c r="A74" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="D74" s="0" t="s">
-        <x:v>317</x:v>
-      </x:c>
-      <x:c r="E74" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>231</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:23">
       <x:c r="A75" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D75" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="E75" s="0" t="s">
-        <x:v>323</x:v>
-      </x:c>
-      <x:c r="F75" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="G75" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>235</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:23">
       <x:c r="A76" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D76" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="E76" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F76" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:23">
       <x:c r="A77" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>332</x:v>
-      </x:c>
-      <x:c r="C77" s="0" t="s">
-        <x:v>333</x:v>
-      </x:c>
-      <x:c r="D77" s="0" t="s">
-        <x:v>334</x:v>
-      </x:c>
-      <x:c r="E77" s="0" t="s">
-        <x:v>335</x:v>
-      </x:c>
-      <x:c r="F77" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:23">
       <x:c r="A78" s="0" t="s">
-        <x:v>337</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>338</x:v>
-      </x:c>
-      <x:c r="C78" s="0" t="s">
-        <x:v>339</x:v>
-      </x:c>
-      <x:c r="D78" s="0" t="s">
-        <x:v>340</x:v>
-      </x:c>
-      <x:c r="E78" s="0" t="s">
-        <x:v>341</x:v>
-      </x:c>
-      <x:c r="F78" s="0" t="s">
-        <x:v>342</x:v>
-      </x:c>
-      <x:c r="G78" s="0" t="s">
-        <x:v>343</x:v>
-      </x:c>
-      <x:c r="H78" s="0" t="s">
-        <x:v>344</x:v>
-      </x:c>
-      <x:c r="I78" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:23">
       <x:c r="A79" s="0" t="s">
-        <x:v>346</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>347</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
-        <x:v>348</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="D79" s="0" t="s">
-        <x:v>349</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="E79" s="0" t="s">
-        <x:v>350</x:v>
-      </x:c>
-      <x:c r="F79" s="0" t="s">
-        <x:v>351</x:v>
-      </x:c>
-      <x:c r="G79" s="0" t="s">
-        <x:v>352</x:v>
-      </x:c>
-      <x:c r="H79" s="0" t="s">
-        <x:v>353</x:v>
-      </x:c>
-      <x:c r="I79" s="0" t="s">
-        <x:v>354</x:v>
-      </x:c>
-      <x:c r="J79" s="0" t="s">
-        <x:v>355</x:v>
-      </x:c>
-      <x:c r="K79" s="0" t="s">
-        <x:v>356</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:23">
       <x:c r="A80" s="0" t="s">
-        <x:v>357</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>358</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>359</x:v>
-      </x:c>
-      <x:c r="D80" s="0" t="s">
-        <x:v>286</x:v>
-      </x:c>
-      <x:c r="E80" s="0" t="s">
-        <x:v>360</x:v>
-      </x:c>
-      <x:c r="F80" s="0" t="s">
-        <x:v>361</x:v>
-      </x:c>
-      <x:c r="G80" s="0" t="s">
-        <x:v>362</x:v>
-      </x:c>
-      <x:c r="H80" s="0" t="s">
-        <x:v>363</x:v>
-      </x:c>
-      <x:c r="I80" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="J80" s="0" t="s">
-        <x:v>364</x:v>
-      </x:c>
-      <x:c r="K80" s="0" t="s">
-        <x:v>365</x:v>
-      </x:c>
-      <x:c r="L80" s="0" t="s">
-        <x:v>366</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:23">
       <x:c r="A81" s="0" t="s">
-        <x:v>367</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>368</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>369</x:v>
-      </x:c>
-      <x:c r="D81" s="0" t="s">
-        <x:v>370</x:v>
-      </x:c>
-      <x:c r="E81" s="0" t="s">
-        <x:v>371</x:v>
-      </x:c>
-      <x:c r="F81" s="0" t="s">
-        <x:v>372</x:v>
-      </x:c>
-      <x:c r="G81" s="0" t="s">
-        <x:v>373</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:23">
       <x:c r="A82" s="0" t="s">
-        <x:v>374</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>375</x:v>
-      </x:c>
-      <x:c r="C82" s="0" t="s">
-        <x:v>376</x:v>
-      </x:c>
-      <x:c r="D82" s="0" t="s">
-        <x:v>377</x:v>
-      </x:c>
-      <x:c r="E82" s="0" t="s">
-        <x:v>378</x:v>
-      </x:c>
-      <x:c r="F82" s="0" t="s">
-        <x:v>379</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:23">
       <x:c r="A83" s="0" t="s">
-        <x:v>380</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>381</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
-        <x:v>382</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="D83" s="0" t="s">
-        <x:v>383</x:v>
-      </x:c>
-      <x:c r="E83" s="0" t="s">
-        <x:v>384</x:v>
-      </x:c>
-      <x:c r="F83" s="0" t="s">
-        <x:v>385</x:v>
-      </x:c>
-      <x:c r="G83" s="0" t="s">
-        <x:v>386</x:v>
-      </x:c>
-      <x:c r="H83" s="0" t="s">
-        <x:v>387</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:23">
       <x:c r="A84" s="0" t="s">
-        <x:v>388</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>389</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>390</x:v>
-      </x:c>
-      <x:c r="D84" s="0" t="s">
-        <x:v>391</x:v>
-      </x:c>
-      <x:c r="E84" s="0" t="s">
-        <x:v>392</x:v>
-      </x:c>
-      <x:c r="F84" s="0" t="s">
-        <x:v>393</x:v>
-      </x:c>
-      <x:c r="G84" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="H84" s="0" t="s">
-        <x:v>394</x:v>
+        <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:23">
       <x:c r="A85" s="0" t="s">
-        <x:v>395</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>396</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>397</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="D85" s="0" t="s">
-        <x:v>398</x:v>
-      </x:c>
-      <x:c r="E85" s="0" t="s">
-        <x:v>399</x:v>
-      </x:c>
-      <x:c r="F85" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="G85" s="0" t="s">
-        <x:v>400</x:v>
-      </x:c>
-      <x:c r="H85" s="0" t="s">
-        <x:v>401</x:v>
-      </x:c>
-      <x:c r="I85" s="0" t="s">
-        <x:v>402</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:23">
       <x:c r="A86" s="0" t="s">
-        <x:v>403</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>404</x:v>
-      </x:c>
-      <x:c r="C86" s="0" t="s">
-        <x:v>405</x:v>
-      </x:c>
-      <x:c r="D86" s="0" t="s">
-        <x:v>406</x:v>
-      </x:c>
-      <x:c r="E86" s="0" t="s">
-        <x:v>407</x:v>
-      </x:c>
-      <x:c r="F86" s="0" t="s">
-        <x:v>408</x:v>
-      </x:c>
-      <x:c r="G86" s="0" t="s">
-        <x:v>409</x:v>
-      </x:c>
-      <x:c r="H86" s="0" t="s">
-        <x:v>410</x:v>
-      </x:c>
-      <x:c r="I86" s="0" t="s">
-        <x:v>411</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:23">
       <x:c r="A87" s="0" t="s">
-        <x:v>412</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>413</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>414</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="D87" s="0" t="s">
-        <x:v>415</x:v>
-      </x:c>
-      <x:c r="E87" s="0" t="s">
-        <x:v>416</x:v>
-      </x:c>
-      <x:c r="F87" s="0" t="s">
-        <x:v>417</x:v>
-      </x:c>
-      <x:c r="G87" s="0" t="s">
-        <x:v>418</x:v>
+        <x:v>273</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:23">
       <x:c r="A88" s="0" t="s">
-        <x:v>419</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>420</x:v>
-      </x:c>
-      <x:c r="C88" s="0" t="s">
-        <x:v>421</x:v>
-      </x:c>
-      <x:c r="D88" s="0" t="s">
-        <x:v>422</x:v>
-      </x:c>
-      <x:c r="E88" s="0" t="s">
-        <x:v>423</x:v>
-      </x:c>
-      <x:c r="F88" s="0" t="s">
-        <x:v>424</x:v>
-      </x:c>
-      <x:c r="G88" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="H88" s="0" t="s">
-        <x:v>425</x:v>
-      </x:c>
-      <x:c r="I88" s="0" t="s">
-        <x:v>426</x:v>
-      </x:c>
-      <x:c r="J88" s="0" t="s">
-        <x:v>427</x:v>
-      </x:c>
-      <x:c r="K88" s="0" t="s">
-        <x:v>428</x:v>
+        <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:23">
       <x:c r="A89" s="0" t="s">
-        <x:v>429</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>430</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
-        <x:v>431</x:v>
-      </x:c>
-      <x:c r="D89" s="0" t="s">
-        <x:v>432</x:v>
-      </x:c>
-      <x:c r="E89" s="0" t="s">
-        <x:v>433</x:v>
-      </x:c>
-      <x:c r="F89" s="0" t="s">
-        <x:v>434</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:23">
       <x:c r="A90" s="0" t="s">
-        <x:v>435</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>436</x:v>
-      </x:c>
-      <x:c r="C90" s="0" t="s">
-        <x:v>437</x:v>
-      </x:c>
-      <x:c r="D90" s="0" t="s">
-        <x:v>438</x:v>
-      </x:c>
-      <x:c r="E90" s="0" t="s">
-        <x:v>439</x:v>
-      </x:c>
-      <x:c r="F90" s="0" t="s">
-        <x:v>440</x:v>
+        <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:23">
       <x:c r="A91" s="0" t="s">
-        <x:v>441</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>442</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>443</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D91" s="0" t="s">
-        <x:v>444</x:v>
-      </x:c>
-      <x:c r="E91" s="0" t="s">
-        <x:v>445</x:v>
-      </x:c>
-      <x:c r="F91" s="0" t="s">
-        <x:v>446</x:v>
-      </x:c>
-      <x:c r="G91" s="0" t="s">
-        <x:v>447</x:v>
+        <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:23">
       <x:c r="A92" s="0" t="s">
-        <x:v>448</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>449</x:v>
-      </x:c>
-      <x:c r="C92" s="0" t="s">
-        <x:v>450</x:v>
-      </x:c>
-      <x:c r="D92" s="0" t="s">
-        <x:v>451</x:v>
-      </x:c>
-      <x:c r="E92" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="F92" s="0" t="s">
-        <x:v>452</x:v>
+        <x:v>286</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:23">
       <x:c r="A93" s="0" t="s">
-        <x:v>453</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>454</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
-        <x:v>455</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="D93" s="0" t="s">
-        <x:v>456</x:v>
-      </x:c>
-      <x:c r="E93" s="0" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="F93" s="0" t="s">
-        <x:v>457</x:v>
-      </x:c>
-      <x:c r="G93" s="0" t="s">
-        <x:v>458</x:v>
-      </x:c>
-      <x:c r="H93" s="0" t="s">
-        <x:v>459</x:v>
+        <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:23">
       <x:c r="A94" s="0" t="s">
-        <x:v>460</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>461</x:v>
-      </x:c>
-      <x:c r="C94" s="0" t="s">
-        <x:v>462</x:v>
-      </x:c>
-      <x:c r="D94" s="0" t="s">
-        <x:v>463</x:v>
-      </x:c>
-      <x:c r="E94" s="0" t="s">
-        <x:v>464</x:v>
-      </x:c>
-      <x:c r="F94" s="0" t="s">
-        <x:v>465</x:v>
+        <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:23">
       <x:c r="A95" s="0" t="s">
-        <x:v>466</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>467</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
-        <x:v>468</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="D95" s="0" t="s">
-        <x:v>469</x:v>
-      </x:c>
-      <x:c r="E95" s="0" t="s">
-        <x:v>470</x:v>
-      </x:c>
-      <x:c r="F95" s="0" t="s">
-        <x:v>471</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:23">
       <x:c r="A96" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:23">
+      <x:c r="A97" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="F97" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:23">
+      <x:c r="A98" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:23">
+      <x:c r="A99" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:23">
+      <x:c r="A100" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:23">
+      <x:c r="A101" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:23">
+      <x:c r="A102" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="C102" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="D102" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="E102" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:23">
+      <x:c r="A103" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="C103" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:23">
+      <x:c r="A104" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="C104" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:23">
+      <x:c r="A105" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="D105" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="E105" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:23">
+      <x:c r="A106" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="C106" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:23">
+      <x:c r="A107" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="C107" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:23">
+      <x:c r="A108" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:23">
+      <x:c r="A109" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="C109" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="E109" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:23">
+      <x:c r="A110" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="C110" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:23">
+      <x:c r="A111" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="E111" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:23">
+      <x:c r="A112" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:23">
+      <x:c r="A113" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C113" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="D113" s="0" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="E113" s="0" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="F113" s="0" t="s">
+        <x:v>359</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:23">
+      <x:c r="A114" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="C114" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="D114" s="0" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="E114" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="F114" s="0" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="G114" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="H114" s="0" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="I114" s="0" t="s">
+        <x:v>368</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:23">
+      <x:c r="A115" s="0" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="C115" s="0" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="D115" s="0" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="E115" s="0" t="s">
+        <x:v>373</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:23">
+      <x:c r="A116" s="0" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="C116" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="D116" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="E116" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="F116" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="G116" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:23">
+      <x:c r="A117" s="0" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="C117" s="0" t="s">
+        <x:v>383</x:v>
+      </x:c>
+      <x:c r="D117" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="E117" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="F117" s="0" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="G117" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="H117" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="I117" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="J117" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="K117" s="0" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="L117" s="0" t="s">
+        <x:v>390</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:23">
+      <x:c r="A118" s="0" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="C118" s="0" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="D118" s="0" t="s">
+        <x:v>394</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:23">
+      <x:c r="A119" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="C119" s="0" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="D119" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:23">
+      <x:c r="A120" s="0" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="C120" s="0" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="D120" s="0" t="s">
+        <x:v>402</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:23">
+      <x:c r="A121" s="0" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>404</x:v>
+      </x:c>
+      <x:c r="C121" s="0" t="s">
+        <x:v>405</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122" spans="1:23">
+      <x:c r="A122" s="0" t="s">
+        <x:v>406</x:v>
+      </x:c>
+      <x:c r="B122" s="0" t="s">
+        <x:v>407</x:v>
+      </x:c>
+      <x:c r="C122" s="0" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="D122" s="0" t="s">
+        <x:v>409</x:v>
+      </x:c>
+      <x:c r="E122" s="0" t="s">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="F122" s="0" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="G122" s="0" t="s">
+        <x:v>412</x:v>
+      </x:c>
+      <x:c r="H122" s="0" t="s">
+        <x:v>413</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:23">
+      <x:c r="A123" s="0" t="s">
+        <x:v>414</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>415</x:v>
+      </x:c>
+      <x:c r="C123" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="D123" s="0" t="s">
+        <x:v>417</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:23">
+      <x:c r="A124" s="0" t="s">
+        <x:v>418</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>419</x:v>
+      </x:c>
+      <x:c r="C124" s="0" t="s">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="D124" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="E124" s="0" t="s">
+        <x:v>421</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:23">
+      <x:c r="A125" s="0" t="s">
+        <x:v>422</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>423</x:v>
+      </x:c>
+      <x:c r="C125" s="0" t="s">
+        <x:v>424</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:23">
+      <x:c r="A126" s="0" t="s">
+        <x:v>425</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>426</x:v>
+      </x:c>
+      <x:c r="C126" s="0" t="s">
+        <x:v>427</x:v>
+      </x:c>
+      <x:c r="D126" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="E126" s="0" t="s">
+        <x:v>428</x:v>
+      </x:c>
+      <x:c r="F126" s="0" t="s">
+        <x:v>429</x:v>
+      </x:c>
+      <x:c r="G126" s="0" t="s">
+        <x:v>430</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:23">
+      <x:c r="A127" s="0" t="s">
+        <x:v>431</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="C127" s="0" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="D127" s="0" t="s">
+        <x:v>434</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:23">
+      <x:c r="A128" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="C128" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="D128" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="E128" s="0" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="F128" s="0" t="s">
+        <x:v>439</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:23">
+      <x:c r="A129" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="C129" s="0" t="s">
+        <x:v>442</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:23">
+      <x:c r="A130" s="0" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="C130" s="0" t="s">
+        <x:v>445</x:v>
+      </x:c>
+      <x:c r="D130" s="0" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="E130" s="0" t="s">
+        <x:v>447</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:23">
+      <x:c r="A131" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="C131" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="D131" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:23">
+      <x:c r="A132" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>453</x:v>
+      </x:c>
+      <x:c r="C132" s="0" t="s">
+        <x:v>454</x:v>
+      </x:c>
+      <x:c r="D132" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="E132" s="0" t="s">
+        <x:v>455</x:v>
+      </x:c>
+      <x:c r="F132" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+      <x:c r="G132" s="0" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="H132" s="0" t="s">
+        <x:v>458</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:23">
+      <x:c r="A133" s="0" t="s">
+        <x:v>459</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="C133" s="0" t="s">
+        <x:v>461</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:23">
+      <x:c r="A134" s="0" t="s">
+        <x:v>462</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>463</x:v>
+      </x:c>
+      <x:c r="C134" s="0" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="D134" s="0" t="s">
+        <x:v>465</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:23">
+      <x:c r="A135" s="0" t="s">
+        <x:v>466</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="C135" s="0" t="s">
+        <x:v>468</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:23">
+      <x:c r="A136" s="0" t="s">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
+        <x:v>470</x:v>
+      </x:c>
+      <x:c r="C136" s="0" t="s">
+        <x:v>471</x:v>
+      </x:c>
+      <x:c r="D136" s="0" t="s">
         <x:v>472</x:v>
       </x:c>
-      <x:c r="C96" s="0" t="s">
+    </x:row>
+    <x:row r="137" spans="1:23">
+      <x:c r="A137" s="0" t="s">
         <x:v>473</x:v>
       </x:c>
-      <x:c r="D96" s="0" t="s">
+      <x:c r="B137" s="0" t="s">
         <x:v>474</x:v>
       </x:c>
-      <x:c r="E96" s="0" t="s">
+      <x:c r="C137" s="0" t="s">
         <x:v>475</x:v>
       </x:c>
-      <x:c r="F96" s="0" t="s">
+      <x:c r="D137" s="0" t="s">
         <x:v>476</x:v>
       </x:c>
-      <x:c r="G96" s="0" t="s">
-        <x:v>476</x:v>
-      </x:c>
-      <x:c r="H96" s="0" t="s">
+    </x:row>
+    <x:row r="138" spans="1:23">
+      <x:c r="A138" s="0" t="s">
         <x:v>477</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>478</x:v>
+      </x:c>
+      <x:c r="C138" s="0" t="s">
+        <x:v>479</x:v>
+      </x:c>
+      <x:c r="D138" s="0" t="s">
+        <x:v>480</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:23">
+      <x:c r="A139" s="0" t="s">
+        <x:v>481</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:23">
+      <x:c r="A140" s="0" t="s">
+        <x:v>483</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>484</x:v>
+      </x:c>
+      <x:c r="C140" s="0" t="s">
+        <x:v>485</x:v>
+      </x:c>
+      <x:c r="D140" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="E140" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:23">
+      <x:c r="A141" s="0" t="s">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>488</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:23">
+      <x:c r="A142" s="0" t="s">
+        <x:v>489</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="C142" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+      <x:c r="D142" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="E142" s="0" t="s">
+        <x:v>492</x:v>
+      </x:c>
+      <x:c r="F142" s="0" t="s">
+        <x:v>493</x:v>
+      </x:c>
+      <x:c r="G142" s="0" t="s">
+        <x:v>494</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:23">
+      <x:c r="A143" s="0" t="s">
+        <x:v>495</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>496</x:v>
+      </x:c>
+      <x:c r="C143" s="0" t="s">
+        <x:v>497</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:23">
+      <x:c r="A144" s="0" t="s">
+        <x:v>498</x:v>
+      </x:c>
+      <x:c r="B144" s="0" t="s">
+        <x:v>499</x:v>
+      </x:c>
+      <x:c r="C144" s="0" t="s">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="D144" s="0" t="s">
+        <x:v>501</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:23">
+      <x:c r="A145" s="0" t="s">
+        <x:v>502</x:v>
+      </x:c>
+      <x:c r="B145" s="0" t="s">
+        <x:v>503</x:v>
+      </x:c>
+      <x:c r="C145" s="0" t="s">
+        <x:v>504</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:23">
+      <x:c r="A146" s="0" t="s">
+        <x:v>505</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="s">
+        <x:v>506</x:v>
+      </x:c>
+      <x:c r="C146" s="0" t="s">
+        <x:v>507</x:v>
+      </x:c>
+      <x:c r="D146" s="0" t="s">
+        <x:v>508</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:23">
+      <x:c r="A147" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>509</x:v>
+      </x:c>
+      <x:c r="C147" s="0" t="s">
+        <x:v>510</x:v>
+      </x:c>
+      <x:c r="D147" s="0" t="s">
+        <x:v>511</x:v>
+      </x:c>
+      <x:c r="E147" s="0" t="s">
+        <x:v>512</x:v>
+      </x:c>
+      <x:c r="F147" s="0" t="s">
+        <x:v>513</x:v>
+      </x:c>
+      <x:c r="G147" s="0" t="s">
+        <x:v>513</x:v>
+      </x:c>
+      <x:c r="H147" s="0" t="s">
+        <x:v>514</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4439,7 +4766,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:T94"/>
+  <x:dimension ref="A1:T99"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -4447,15 +4774,15 @@
   <x:sheetData>
     <x:row r="1" spans="1:20">
       <x:c r="A1" s="1" t="s">
-        <x:v>478</x:v>
+        <x:v>515</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:20">
       <x:c r="A3" s="0" t="s">
-        <x:v>479</x:v>
+        <x:v>516</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>480</x:v>
+        <x:v>517</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
         <x:v>3</x:v>
@@ -4466,7 +4793,7 @@
     </x:row>
     <x:row r="5" spans="1:20">
       <x:c r="A5" s="0" t="s">
-        <x:v>481</x:v>
+        <x:v>518</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>6</x:v>
@@ -4475,7 +4802,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="R5" s="0" t="s">
-        <x:v>482</x:v>
+        <x:v>519</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:20">
@@ -4483,10 +4810,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>483</x:v>
+        <x:v>520</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>484</x:v>
+        <x:v>521</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:20">
@@ -4497,7 +4824,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>485</x:v>
+        <x:v>522</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:20">
@@ -4505,41 +4832,41 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>486</x:v>
+        <x:v>523</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>487</x:v>
+        <x:v>524</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:20">
       <x:c r="A13" s="0" t="s">
-        <x:v>488</x:v>
+        <x:v>525</x:v>
       </x:c>
       <x:c r="N13" s="0" t="s">
-        <x:v>489</x:v>
+        <x:v>526</x:v>
       </x:c>
       <x:c r="Q13" s="0" t="s">
-        <x:v>490</x:v>
+        <x:v>527</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:20">
       <x:c r="C14" s="0" t="s">
-        <x:v>491</x:v>
+        <x:v>528</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>492</x:v>
+        <x:v>529</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>493</x:v>
+        <x:v>530</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>494</x:v>
+        <x:v>531</x:v>
       </x:c>
       <x:c r="N14" s="0" t="s">
-        <x:v>495</x:v>
+        <x:v>532</x:v>
       </x:c>
       <x:c r="Q14" s="0" t="s">
-        <x:v>496</x:v>
+        <x:v>533</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:20">
@@ -4547,37 +4874,37 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>497</x:v>
+        <x:v>534</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>498</x:v>
+        <x:v>535</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>499</x:v>
+        <x:v>536</x:v>
       </x:c>
       <x:c r="E15" s="1" t="s">
-        <x:v>500</x:v>
+        <x:v>537</x:v>
       </x:c>
       <x:c r="F15" s="1" t="s">
-        <x:v>501</x:v>
+        <x:v>538</x:v>
       </x:c>
       <x:c r="G15" s="1" t="s">
-        <x:v>502</x:v>
+        <x:v>539</x:v>
       </x:c>
       <x:c r="H15" s="1" t="s">
-        <x:v>503</x:v>
+        <x:v>540</x:v>
       </x:c>
       <x:c r="I15" s="1" t="s">
-        <x:v>504</x:v>
+        <x:v>541</x:v>
       </x:c>
       <x:c r="J15" s="1" t="s">
-        <x:v>505</x:v>
+        <x:v>542</x:v>
       </x:c>
       <x:c r="K15" s="1" t="s">
-        <x:v>506</x:v>
+        <x:v>543</x:v>
       </x:c>
       <x:c r="L15" s="1" t="s">
-        <x:v>507</x:v>
+        <x:v>544</x:v>
       </x:c>
       <x:c r="M15" s="1" t="s">
         <x:v>34</x:v>
@@ -4592,1017 +4919,1024 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="Q15" s="1" t="s">
-        <x:v>508</x:v>
+        <x:v>545</x:v>
       </x:c>
       <x:c r="R15" s="1" t="s">
-        <x:v>509</x:v>
+        <x:v>546</x:v>
       </x:c>
       <x:c r="S15" s="1" t="s">
-        <x:v>510</x:v>
+        <x:v>547</x:v>
       </x:c>
       <x:c r="T15" s="1" t="s">
-        <x:v>511</x:v>
+        <x:v>548</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:20">
       <x:c r="A16" s="0" t="s">
-        <x:v>512</x:v>
+        <x:v>549</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>513</x:v>
+        <x:v>550</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:20">
       <x:c r="A17" s="0" t="s">
-        <x:v>514</x:v>
+        <x:v>551</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>515</x:v>
+        <x:v>552</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>516</x:v>
+        <x:v>553</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>517</x:v>
+        <x:v>554</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>518</x:v>
+        <x:v>555</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>519</x:v>
+        <x:v>556</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>516</x:v>
+        <x:v>553</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>520</x:v>
+        <x:v>557</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
-        <x:v>521</x:v>
+        <x:v>558</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:20">
       <x:c r="A18" s="0" t="s">
-        <x:v>522</x:v>
+        <x:v>559</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>523</x:v>
+        <x:v>560</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>524</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>525</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>526</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>527</x:v>
+        <x:v>561</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:20">
       <x:c r="A19" s="0" t="s">
-        <x:v>528</x:v>
+        <x:v>562</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>529</x:v>
+        <x:v>563</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>530</x:v>
+        <x:v>564</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>565</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:20">
       <x:c r="A20" s="0" t="s">
-        <x:v>531</x:v>
+        <x:v>566</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>532</x:v>
+        <x:v>567</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>533</x:v>
+        <x:v>568</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>534</x:v>
+        <x:v>569</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:20">
       <x:c r="A21" s="0" t="s">
-        <x:v>535</x:v>
+        <x:v>570</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>536</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>537</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>538</x:v>
+        <x:v>571</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:20">
       <x:c r="A22" s="0" t="s">
-        <x:v>539</x:v>
+        <x:v>572</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>573</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>540</x:v>
+        <x:v>574</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>575</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>576</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>577</x:v>
+      </x:c>
+      <x:c r="H22" s="0" t="s">
+        <x:v>578</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:20">
       <x:c r="A23" s="0" t="s">
-        <x:v>541</x:v>
+        <x:v>579</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>542</x:v>
+        <x:v>580</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>543</x:v>
+        <x:v>581</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>544</x:v>
+        <x:v>582</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>545</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>583</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>546</x:v>
+        <x:v>584</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>547</x:v>
+        <x:v>585</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:20">
       <x:c r="A24" s="0" t="s">
-        <x:v>548</x:v>
+        <x:v>586</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>549</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>550</x:v>
+        <x:v>587</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>551</x:v>
+        <x:v>588</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>589</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>552</x:v>
+        <x:v>590</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>553</x:v>
-      </x:c>
-      <x:c r="H24" s="0" t="s">
-        <x:v>554</x:v>
+        <x:v>591</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:20">
       <x:c r="A25" s="0" t="s">
-        <x:v>555</x:v>
+        <x:v>592</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>593</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>556</x:v>
+        <x:v>594</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>557</x:v>
+        <x:v>595</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>558</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>559</x:v>
+        <x:v>596</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>560</x:v>
+        <x:v>597</x:v>
+      </x:c>
+      <x:c r="H25" s="0" t="s">
+        <x:v>598</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:20">
       <x:c r="A26" s="0" t="s">
-        <x:v>561</x:v>
+        <x:v>599</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>562</x:v>
+        <x:v>600</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>563</x:v>
+        <x:v>601</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>564</x:v>
+        <x:v>602</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>565</x:v>
+        <x:v>603</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>566</x:v>
+        <x:v>604</x:v>
       </x:c>
       <x:c r="H26" s="0" t="s">
-        <x:v>567</x:v>
+        <x:v>605</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:20">
       <x:c r="A27" s="0" t="s">
-        <x:v>568</x:v>
+        <x:v>606</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>569</x:v>
+        <x:v>607</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>570</x:v>
+        <x:v>608</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>571</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>609</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>572</x:v>
-      </x:c>
-      <x:c r="G27" s="0" t="s">
-        <x:v>573</x:v>
-      </x:c>
-      <x:c r="H27" s="0" t="s">
-        <x:v>574</x:v>
+        <x:v>610</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:20">
       <x:c r="A28" s="0" t="s">
-        <x:v>575</x:v>
+        <x:v>611</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>576</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>577</x:v>
+        <x:v>612</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>613</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>578</x:v>
+        <x:v>614</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>579</x:v>
+        <x:v>615</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:20">
       <x:c r="A29" s="0" t="s">
-        <x:v>580</x:v>
+        <x:v>616</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="C29" s="0" t="s">
-        <x:v>581</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>582</x:v>
-      </x:c>
-      <x:c r="E29" s="0" t="s">
-        <x:v>583</x:v>
-      </x:c>
-      <x:c r="F29" s="0" t="s">
-        <x:v>584</x:v>
+        <x:v>617</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:20">
       <x:c r="A30" s="0" t="s">
-        <x:v>585</x:v>
+        <x:v>618</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>586</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>587</x:v>
+        <x:v>619</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:20">
       <x:c r="A31" s="0" t="s">
-        <x:v>588</x:v>
+        <x:v>620</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>589</x:v>
-      </x:c>
-      <x:c r="C31" s="0" t="s">
-        <x:v>590</x:v>
+        <x:v>621</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:20">
       <x:c r="A32" s="0" t="s">
-        <x:v>591</x:v>
+        <x:v>622</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="C32" s="0" t="s">
-        <x:v>592</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>593</x:v>
+        <x:v>623</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:20">
       <x:c r="A33" s="0" t="s">
-        <x:v>594</x:v>
+        <x:v>624</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>595</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>596</x:v>
+        <x:v>625</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>626</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:20">
       <x:c r="A34" s="0" t="s">
-        <x:v>597</x:v>
+        <x:v>627</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>598</x:v>
+        <x:v>628</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>599</x:v>
+        <x:v>629</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:20">
       <x:c r="A35" s="0" t="s">
-        <x:v>600</x:v>
+        <x:v>630</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>601</x:v>
+        <x:v>631</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>602</x:v>
-      </x:c>
-      <x:c r="D35" s="0" t="s">
-        <x:v>603</x:v>
+        <x:v>632</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:20">
       <x:c r="A36" s="0" t="s">
-        <x:v>604</x:v>
+        <x:v>633</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>605</x:v>
+        <x:v>634</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>606</x:v>
+        <x:v>635</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
-        <x:v>607</x:v>
+        <x:v>636</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:20">
       <x:c r="A37" s="0" t="s">
-        <x:v>608</x:v>
+        <x:v>637</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>609</x:v>
+        <x:v>638</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>610</x:v>
+        <x:v>639</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>611</x:v>
+        <x:v>640</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:20">
       <x:c r="A38" s="0" t="s">
-        <x:v>612</x:v>
+        <x:v>641</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>613</x:v>
+        <x:v>642</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>614</x:v>
+        <x:v>643</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>644</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:20">
       <x:c r="A39" s="0" t="s">
-        <x:v>615</x:v>
+        <x:v>645</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>616</x:v>
+        <x:v>646</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>617</x:v>
+        <x:v>647</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:20">
       <x:c r="A40" s="0" t="s">
-        <x:v>618</x:v>
+        <x:v>648</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>619</x:v>
+        <x:v>649</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>620</x:v>
+        <x:v>650</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:20">
       <x:c r="A41" s="0" t="s">
-        <x:v>621</x:v>
+        <x:v>651</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>622</x:v>
+        <x:v>652</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>623</x:v>
-      </x:c>
-      <x:c r="D41" s="0" t="s">
-        <x:v>624</x:v>
+        <x:v>653</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:20">
       <x:c r="A42" s="0" t="s">
-        <x:v>625</x:v>
+        <x:v>654</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>626</x:v>
+        <x:v>655</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>627</x:v>
+        <x:v>656</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
-        <x:v>628</x:v>
+        <x:v>657</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:20">
       <x:c r="A43" s="0" t="s">
-        <x:v>629</x:v>
+        <x:v>658</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>630</x:v>
+        <x:v>659</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>631</x:v>
+        <x:v>660</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>632</x:v>
+        <x:v>661</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:20">
       <x:c r="A44" s="0" t="s">
-        <x:v>633</x:v>
+        <x:v>662</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>663</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>634</x:v>
-      </x:c>
-      <x:c r="D44" s="0" t="s">
-        <x:v>635</x:v>
+        <x:v>664</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:20">
       <x:c r="A45" s="0" t="s">
-        <x:v>636</x:v>
+        <x:v>665</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>637</x:v>
-      </x:c>
-      <x:c r="C45" s="0" t="s">
-        <x:v>638</x:v>
-      </x:c>
-      <x:c r="D45" s="0" t="s">
-        <x:v>639</x:v>
+        <x:v>666</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:20">
       <x:c r="A46" s="0" t="s">
-        <x:v>640</x:v>
+        <x:v>667</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>641</x:v>
+        <x:v>668</x:v>
       </x:c>
       <x:c r="D46" s="0" t="s">
-        <x:v>642</x:v>
-      </x:c>
-      <x:c r="E46" s="0" t="s">
-        <x:v>643</x:v>
+        <x:v>669</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:20">
       <x:c r="A47" s="0" t="s">
-        <x:v>644</x:v>
+        <x:v>670</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>645</x:v>
+        <x:v>671</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>646</x:v>
+        <x:v>672</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>673</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:20">
       <x:c r="A48" s="0" t="s">
-        <x:v>647</x:v>
+        <x:v>674</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>648</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>649</x:v>
+        <x:v>675</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>650</x:v>
+        <x:v>676</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
-        <x:v>651</x:v>
+        <x:v>677</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:20">
       <x:c r="A49" s="0" t="s">
-        <x:v>652</x:v>
+        <x:v>678</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>653</x:v>
+        <x:v>679</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
-        <x:v>654</x:v>
+        <x:v>680</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:20">
       <x:c r="A50" s="0" t="s">
-        <x:v>655</x:v>
+        <x:v>681</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>656</x:v>
+        <x:v>682</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>657</x:v>
+        <x:v>683</x:v>
       </x:c>
       <x:c r="D50" s="0" t="s">
-        <x:v>658</x:v>
+        <x:v>684</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>685</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:20">
       <x:c r="A51" s="0" t="s">
-        <x:v>659</x:v>
+        <x:v>686</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>660</x:v>
-      </x:c>
-      <x:c r="C51" s="0" t="s">
-        <x:v>661</x:v>
-      </x:c>
-      <x:c r="D51" s="0" t="s">
-        <x:v>662</x:v>
+        <x:v>687</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:20">
       <x:c r="A52" s="0" t="s">
-        <x:v>663</x:v>
+        <x:v>688</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>664</x:v>
-      </x:c>
-      <x:c r="C52" s="0" t="s">
-        <x:v>665</x:v>
+        <x:v>689</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:20">
       <x:c r="A53" s="0" t="s">
-        <x:v>666</x:v>
+        <x:v>690</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>667</x:v>
+        <x:v>691</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:20">
       <x:c r="A54" s="0" t="s">
-        <x:v>668</x:v>
+        <x:v>692</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>669</x:v>
+        <x:v>693</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>670</x:v>
+        <x:v>694</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:20">
       <x:c r="A55" s="0" t="s">
-        <x:v>671</x:v>
+        <x:v>695</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>672</x:v>
+        <x:v>696</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>697</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:20">
       <x:c r="A56" s="0" t="s">
-        <x:v>673</x:v>
+        <x:v>698</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>674</x:v>
+        <x:v>699</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:20">
       <x:c r="A57" s="0" t="s">
-        <x:v>675</x:v>
+        <x:v>700</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>676</x:v>
+        <x:v>701</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>702</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:20">
       <x:c r="A58" s="0" t="s">
-        <x:v>677</x:v>
+        <x:v>703</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>678</x:v>
+        <x:v>704</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:20">
       <x:c r="A59" s="0" t="s">
-        <x:v>679</x:v>
+        <x:v>705</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>680</x:v>
+        <x:v>706</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>707</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:20">
       <x:c r="A60" s="0" t="s">
-        <x:v>681</x:v>
+        <x:v>708</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>682</x:v>
+        <x:v>709</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:20">
       <x:c r="A61" s="0" t="s">
-        <x:v>683</x:v>
+        <x:v>710</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>684</x:v>
+        <x:v>711</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:20">
       <x:c r="A62" s="0" t="s">
-        <x:v>685</x:v>
+        <x:v>712</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>686</x:v>
+        <x:v>713</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:20">
       <x:c r="A63" s="0" t="s">
-        <x:v>687</x:v>
+        <x:v>714</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>688</x:v>
-      </x:c>
-      <x:c r="C63" s="0" t="s">
-        <x:v>689</x:v>
+        <x:v>715</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:20">
       <x:c r="A64" s="0" t="s">
-        <x:v>690</x:v>
+        <x:v>716</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>691</x:v>
-      </x:c>
-      <x:c r="C64" s="0" t="s">
-        <x:v>692</x:v>
+        <x:v>717</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:20">
       <x:c r="A65" s="0" t="s">
-        <x:v>693</x:v>
+        <x:v>718</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>694</x:v>
-      </x:c>
-      <x:c r="C65" s="0" t="s">
-        <x:v>695</x:v>
+        <x:v>719</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:20">
       <x:c r="A66" s="0" t="s">
-        <x:v>696</x:v>
+        <x:v>720</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>697</x:v>
-      </x:c>
-      <x:c r="C66" s="0" t="s">
-        <x:v>698</x:v>
+        <x:v>721</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:20">
       <x:c r="A67" s="0" t="s">
-        <x:v>699</x:v>
+        <x:v>722</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>700</x:v>
-      </x:c>
-      <x:c r="C67" s="0" t="s">
-        <x:v>701</x:v>
+        <x:v>723</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:20">
       <x:c r="A68" s="0" t="s">
-        <x:v>702</x:v>
+        <x:v>724</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>703</x:v>
+        <x:v>725</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>704</x:v>
+        <x:v>726</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:20">
       <x:c r="A69" s="0" t="s">
-        <x:v>705</x:v>
+        <x:v>727</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>706</x:v>
+        <x:v>728</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
-        <x:v>707</x:v>
+        <x:v>729</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:20">
       <x:c r="A70" s="0" t="s">
-        <x:v>708</x:v>
+        <x:v>730</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>709</x:v>
+        <x:v>731</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>732</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:20">
       <x:c r="A71" s="0" t="s">
-        <x:v>710</x:v>
+        <x:v>733</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>711</x:v>
+        <x:v>734</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>735</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:20">
       <x:c r="A72" s="0" t="s">
-        <x:v>712</x:v>
+        <x:v>736</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>713</x:v>
+        <x:v>737</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>738</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:20">
       <x:c r="A73" s="0" t="s">
-        <x:v>714</x:v>
+        <x:v>739</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>715</x:v>
+        <x:v>740</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>741</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:20">
       <x:c r="A74" s="0" t="s">
-        <x:v>716</x:v>
+        <x:v>742</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>717</x:v>
+        <x:v>743</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>744</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:20">
       <x:c r="A75" s="0" t="s">
-        <x:v>718</x:v>
+        <x:v>745</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>719</x:v>
+        <x:v>746</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:20">
       <x:c r="A76" s="0" t="s">
-        <x:v>720</x:v>
+        <x:v>747</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="C76" s="0" t="s">
-        <x:v>721</x:v>
+        <x:v>748</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:20">
       <x:c r="A77" s="0" t="s">
-        <x:v>722</x:v>
+        <x:v>749</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>723</x:v>
-      </x:c>
-      <x:c r="C77" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="D77" s="0" t="s">
-        <x:v>724</x:v>
+        <x:v>750</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:20">
       <x:c r="A78" s="0" t="s">
-        <x:v>725</x:v>
+        <x:v>751</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>726</x:v>
+        <x:v>752</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:20">
       <x:c r="A79" s="0" t="s">
-        <x:v>727</x:v>
+        <x:v>753</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>728</x:v>
-      </x:c>
-      <x:c r="C79" s="0" t="s">
-        <x:v>729</x:v>
+        <x:v>754</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:20">
       <x:c r="A80" s="0" t="s">
-        <x:v>730</x:v>
+        <x:v>755</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="C80" s="0" t="s">
-        <x:v>731</x:v>
+        <x:v>756</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:20">
       <x:c r="A81" s="0" t="s">
-        <x:v>732</x:v>
+        <x:v>757</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>733</x:v>
+        <x:v>758</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:20">
       <x:c r="A82" s="0" t="s">
-        <x:v>734</x:v>
+        <x:v>759</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>735</x:v>
+        <x:v>760</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>736</x:v>
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D82" s="0" t="s">
+        <x:v>761</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:20">
       <x:c r="A83" s="0" t="s">
-        <x:v>737</x:v>
+        <x:v>762</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>738</x:v>
-      </x:c>
-      <x:c r="C83" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="D83" s="0" t="s">
-        <x:v>739</x:v>
+        <x:v>763</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:20">
       <x:c r="A84" s="0" t="s">
-        <x:v>740</x:v>
+        <x:v>764</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>741</x:v>
+        <x:v>765</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>766</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:20">
       <x:c r="A85" s="0" t="s">
-        <x:v>742</x:v>
+        <x:v>767</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>728</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>743</x:v>
+        <x:v>768</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:20">
       <x:c r="A86" s="0" t="s">
-        <x:v>744</x:v>
+        <x:v>769</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>745</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="D86" s="0" t="s">
-        <x:v>746</x:v>
+        <x:v>770</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:20">
       <x:c r="A87" s="0" t="s">
-        <x:v>747</x:v>
+        <x:v>771</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>748</x:v>
+        <x:v>772</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>749</x:v>
+        <x:v>773</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:20">
       <x:c r="A88" s="0" t="s">
-        <x:v>750</x:v>
+        <x:v>774</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>751</x:v>
+        <x:v>775</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="D88" s="0" t="s">
-        <x:v>752</x:v>
+        <x:v>776</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:20">
       <x:c r="A89" s="0" t="s">
-        <x:v>753</x:v>
+        <x:v>777</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>754</x:v>
-      </x:c>
-      <x:c r="C89" s="0" t="s">
-        <x:v>755</x:v>
+        <x:v>778</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:20">
       <x:c r="A90" s="0" t="s">
-        <x:v>756</x:v>
+        <x:v>779</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>757</x:v>
+        <x:v>765</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
-        <x:v>758</x:v>
+        <x:v>780</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:20">
       <x:c r="A91" s="0" t="s">
-        <x:v>759</x:v>
+        <x:v>781</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>760</x:v>
+        <x:v>782</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>761</x:v>
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>783</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:20">
       <x:c r="A92" s="0" t="s">
-        <x:v>762</x:v>
+        <x:v>784</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>763</x:v>
+        <x:v>785</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>212</x:v>
-      </x:c>
-      <x:c r="D92" s="0" t="s">
-        <x:v>764</x:v>
+        <x:v>786</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:20">
       <x:c r="A93" s="0" t="s">
-        <x:v>765</x:v>
+        <x:v>787</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>766</x:v>
+        <x:v>788</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
-        <x:v>767</x:v>
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>789</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:20">
       <x:c r="A94" s="0" t="s">
-        <x:v>768</x:v>
+        <x:v>790</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>769</x:v>
+        <x:v>791</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
-        <x:v>770</x:v>
+        <x:v>792</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:20">
+      <x:c r="A95" s="0" t="s">
+        <x:v>793</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>794</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>795</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:20">
+      <x:c r="A96" s="0" t="s">
+        <x:v>796</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>797</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>798</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:20">
+      <x:c r="A97" s="0" t="s">
+        <x:v>799</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>800</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>801</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:20">
+      <x:c r="A98" s="0" t="s">
+        <x:v>802</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>803</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>804</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:20">
+      <x:c r="A99" s="0" t="s">
+        <x:v>805</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>806</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>807</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add dual-column table parsing and improve filtering for cleaner output
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -89,6 +89,12 @@
     <x:t>STINGER SWITCH 115KV 1</x:t>
   </x:si>
   <x:si>
+    <x:t>82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FUPS TROUBLE F 80</x:t>
+  </x:si>
+  <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
@@ -101,12 +107,24 @@
     <x:t>INYO 115KV CB 2</x:t>
   </x:si>
   <x:si>
+    <x:t>84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV RELAY BUS AL 82</x:t>
+  </x:si>
+  <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO-SHERWIN 115KV CB 5</x:t>
   </x:si>
   <x:si>
+    <x:t>86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV OPERATING BUS AL 84</x:t>
+  </x:si>
+  <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
@@ -161,6 +179,12 @@
     <x:t>fi1S5KV CB LOW GAS7AIR 19</x:t>
   </x:si>
   <x:si>
+    <x:t>100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
+  </x:si>
+  <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
@@ -248,6 +272,12 @@
     <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
   </x:si>
   <x:si>
+    <x:t>144</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KVID6O</x:t>
+  </x:si>
+  <x:si>
     <x:t>65</x:t>
   </x:si>
   <x:si>
@@ -260,12 +290,24 @@
     <x:t>115KV DFR FAIL 64</x:t>
   </x:si>
   <x:si>
+    <x:t>146</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>67</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR OPERATION 65</x:t>
   </x:si>
   <x:si>
+    <x:t>147</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>68</x:t>
   </x:si>
   <x:si>
@@ -278,36 +320,81 @@
     <x:t>115KV UNDERFREQ RELAY FAIL 67</x:t>
   </x:si>
   <x:si>
+    <x:t>149</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
     <x:t>71</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA DIABLO REACTOR OV</x:t>
   </x:si>
   <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN T15KVD60 TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>72</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA DIABLO REACTOR UV</x:t>
   </x:si>
   <x:si>
+    <x:t>152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KVD60RLY FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>73</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA D-SHERWIN REACTOR CSF 71</x:t>
   </x:si>
   <x:si>
+    <x:t>153</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KVD60/A/S</x:t>
+  </x:si>
+  <x:si>
     <x:t>74</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA D-SHERWIN REACTOR OV</x:t>
   </x:si>
   <x:si>
+    <x:t>154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>75</x:t>
   </x:si>
   <x:si>
     <x:t>FCASA D-SHERWIN REACTOR UV</x:t>
   </x:si>
   <x:si>
+    <x:t>155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>157</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>158</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
     <x:t>79</x:t>
   </x:si>
   <x:si>
@@ -320,31 +407,16 @@
     <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
+    <x:t>160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
     <x:t>ADDED POINT FOR 115KV LINE POS. 4</x:t>
   </x:si>
   <x:si>
-    <x:t>5640067</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5640066</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM T15KV SH. 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5640064</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>585409</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONE LINE FOR CONSTRUCTION 3</x:t>
+    <x:t>REPL'D RLY SEL-311C WITH D60 FOR 115KV LINE POS. 3.</x:t>
   </x:si>
   <x:si>
     <x:t>CONTRL_D  DNP Analog Point List</x:t>
@@ -377,16 +449,28 @@
     <x:t xml:space="preserve">TESTMAN: </x:t>
   </x:si>
   <x:si>
+    <x:t>241</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK A A ToT ' \</x:t>
+  </x:si>
+  <x:si>
     <x:t>166</x:t>
   </x:si>
   <x:si>
     <x:t>fF F</x:t>
   </x:si>
   <x:si>
-    <x:t>167</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I</x:t>
+    <x:t>247</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV D60 OPD TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>248</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV D60 OPD A/S</x:t>
   </x:si>
   <x:si>
     <x:t>172</x:t>
@@ -395,15 +479,6 @@
     <x:t>i RESERVED FOR 115KV LINE Pos. 7</x:t>
   </x:si>
   <x:si>
-    <x:t>174</x:t>
-  </x:si>
-  <x:si>
-    <x:t>178</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F</x:t>
-  </x:si>
-  <x:si>
     <x:t>184</x:t>
   </x:si>
   <x:si>
@@ -587,19 +662,16 @@
     <x:t>ISILVERPEAK C C TCT</x:t>
   </x:si>
   <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5640065</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM 115KV SH. 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ED RTU SYSTEM 115-55KV —— ADDED OPD ALARMS FOR D60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONE LINE FOR CONSTRUCTION 0</x:t>
+    <x:t>ADDED OPD ALARMS FOR D60 115KV LINE POS. 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>————</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISSUED FOR CONSTRUCTION 08-31-20</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -965,7 +1037,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:W61"/>
+  <x:dimension ref="A1:W74"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1234,39 +1306,39 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:23">
       <x:c r="A40" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:23">
       <x:c r="A41" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:23">
       <x:c r="A42" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:23">
       <x:c r="A43" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
         <x:v>73</x:v>
-      </x:c>
-      <x:c r="B43" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:23">
@@ -1375,23 +1447,23 @@
     </x:row>
     <x:row r="57" spans="1:23">
       <x:c r="A57" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:23">
       <x:c r="A58" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:23">
       <x:c r="A59" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
         <x:v>105</x:v>
@@ -1411,6 +1483,110 @@
       </x:c>
       <x:c r="B61" s="0" t="s">
         <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:23">
+      <x:c r="A62" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:23">
+      <x:c r="A63" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:23">
+      <x:c r="A64" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:23">
+      <x:c r="A65" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:23">
+      <x:c r="A66" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:23">
+      <x:c r="A67" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:23">
+      <x:c r="A68" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:23">
+      <x:c r="A69" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:23">
+      <x:c r="A70" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:23">
+      <x:c r="A71" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:23">
+      <x:c r="A72" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:23">
+      <x:c r="A73" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:23">
+      <x:c r="A74" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>133</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1427,7 +1603,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:R58"/>
+  <x:dimension ref="A1:R57"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1435,15 +1611,15 @@
   <x:sheetData>
     <x:row r="1" spans="1:18">
       <x:c r="A1" s="1" t="s">
-        <x:v>110</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:18">
       <x:c r="A3" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
         <x:v>3</x:v>
@@ -1454,7 +1630,7 @@
     </x:row>
     <x:row r="5" spans="1:18">
       <x:c r="A5" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>6</x:v>
@@ -1463,7 +1639,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="R5" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:18">
@@ -1471,10 +1647,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:18">
@@ -1485,7 +1661,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:18">
@@ -1493,10 +1669,10 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:18">
@@ -1509,346 +1685,338 @@
     </x:row>
     <x:row r="16" spans="1:18">
       <x:c r="A16" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:18">
       <x:c r="A17" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:18">
       <x:c r="A18" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:18">
       <x:c r="A19" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:18">
       <x:c r="A20" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:18">
       <x:c r="A21" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:18">
       <x:c r="A22" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:18">
       <x:c r="A23" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:18">
       <x:c r="A24" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:18">
       <x:c r="A25" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:18">
       <x:c r="A26" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:18">
       <x:c r="A27" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:18">
       <x:c r="A28" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:18">
       <x:c r="A29" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:18">
       <x:c r="A30" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:18">
       <x:c r="A31" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:18">
       <x:c r="A32" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:18">
       <x:c r="A33" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:18">
       <x:c r="A34" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:18">
       <x:c r="A35" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:18">
       <x:c r="A36" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:18">
       <x:c r="A37" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:18">
       <x:c r="A38" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:18">
       <x:c r="A39" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:18">
       <x:c r="A40" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:18">
       <x:c r="A41" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:18">
       <x:c r="A42" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:18">
       <x:c r="A43" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:18">
       <x:c r="A44" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:18">
       <x:c r="A45" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:18">
       <x:c r="A46" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:18">
       <x:c r="A47" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:18">
       <x:c r="A48" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:18">
       <x:c r="A49" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:18">
       <x:c r="A50" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:18">
       <x:c r="A51" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>208</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:18">
       <x:c r="A52" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>210</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:18">
       <x:c r="A53" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:18">
       <x:c r="A54" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>214</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:18">
       <x:c r="A55" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:18">
       <x:c r="A56" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:18">
       <x:c r="A57" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>193</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58" spans="1:18">
-      <x:c r="A58" s="0" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="B58" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement two-column parsing and improve point name extraction logic
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -26,289 +26,373 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
-    <x:t>RTU MONITOR JUMPER CONTROL INHIBIT 0</x:t>
+    <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>STINGER SWITCH 115KV 1</x:t>
+    <x:t>STINGER SWITCH 115KV</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>ftnyo 115KV CB 1</x:t>
+    <x:t>FUPS TROUBLE</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>INYO 115KV CB 2</x:t>
+    <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA DIABLO-SHERWIN 115KV CB 5</x:t>
+    <x:t>NYO 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV CB 7</x:t>
+    <x:t>115KV RELAY BUS AL</x:t>
   </x:si>
   <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV CB 9</x:t>
+    <x:t>115KV BACK-UP BUS AL</x:t>
   </x:si>
   <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
-    <x:t>BISHOP CREEK PLANT NO. 3 &amp; 4 115KV CB E</x:t>
+    <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW 115KV CB 17</x:t>
+    <x:t>115KV OPERATING BUS AL</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW CUST CB I 10</x:t>
+    <x:t>HAIWEE-INYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>WWIXIE VALLEY CUST CBF Tn 1</x:t>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>fNO. 1</x:t>
+    <x:t>BISHOP CREEK PLANT NO.</x:t>
   </x:si>
   <x:si>
     <x:t>12</x:t>
   </x:si>
   <x:si>
+    <x:t>OXBOW 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW CUST CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIXIE VALLEY CUST CBF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
     <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fi1S5KV CB LOW GAS7AIR 19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14</x:t>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1155KV CB LOW GAS7AIR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB GEN</x:t>
   </x:si>
   <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FTRANS BK SUDDENTPRESS RESET “1 -</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INO. 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FNO. 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 1 BANK 63X FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF FAIL I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
-  </x:si>
-  <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
-  </x:si>
-  <x:si>
     <x:t>22</x:t>
   </x:si>
   <x:si>
-    <x:t>INO. 3</x:t>
+    <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>23</x:t>
   </x:si>
   <x:si>
+    <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>24</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ POT FAIL 54</x:t>
+    <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
   </x:si>
   <x:si>
     <x:t>25</x:t>
   </x:si>
   <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ POT FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
     <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
+    <x:t>35</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>27</x:t>
+    <x:t>36</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
+    <x:t>37</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>29</x:t>
+    <x:t>38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KVID6O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>39</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV DFR FAIL 64</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV DFR OPERATION 65</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY PICK UP 66</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY FAIL 67</x:t>
-  </x:si>
-  <x:si>
-    <x:t>34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ICASA DIABLO REACTOR OV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ICASA DIABLO REACTOR UV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ICASA D-SHERWIN REACTOR CSF 71</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ICASA D-SHERWIN REACTOR OV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>38</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FCASA D-SHERWIN REACTOR UV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cD SHUNT REACTOR TROUBLE AL</x:t>
-  </x:si>
-  <x:si>
     <x:t>40</x:t>
   </x:si>
   <x:si>
+    <x:t>HAIWEE-INYOKERN 115KVD60JA/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR OPERATION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KVD60RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR CSF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KVD60/A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HATWEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63</x:t>
+  </x:si>
+  <x:si>
     <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADDED POINT FOR 115KV LINE POS. 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM T15KV SH. 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>44</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONE LINE FOR CONSTRUCTION 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fF F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos. 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fF L RESERVED FOR 115KV LINE POs. 8</x:t>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK A C TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
   </x:si>
   <x:si>
     <x:t>115KV LBFB ARMED</x:t>
@@ -320,58 +404,25 @@
     <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
   </x:si>
   <x:si>
-    <x:t>I115KV CB 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f115KV CB 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TS5KV CB 11" LBFB RELAY PS 16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB 11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN15KV CB 13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB 15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN15KV CB 17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV cB 11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115K CB 15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 23</x:t>
+    <x:t>I115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV cB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115K CB</x:t>
   </x:si>
   <x:si>
     <x:t>SEL-2020 COM</x:t>
@@ -386,19 +437,7 @@
     <x:t>lcoso HWE GRD TGT</x:t>
   </x:si>
   <x:si>
-    <x:t>ISILVERPEAK C C TCT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM 115KV SH. 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ED RTU SYSTEM 115-55KV —— ADDED OPD ALARMS FOR D60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONE LINE FOR CONSTRUCTION 0</x:t>
+    <x:t>SILVERPEAK C C TCT</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -764,7 +803,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B47"/>
+  <x:dimension ref="A1:B66"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -951,23 +990,23 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
         <x:v>48</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -983,167 +1022,319 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
       <x:c r="A47" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:2">
+      <x:c r="A48" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:2">
+      <x:c r="A49" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:2">
+      <x:c r="A50" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:2">
+      <x:c r="A51" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="B47" s="0" t="s">
+      <x:c r="B51" s="0" t="s">
         <x:v>92</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:2">
+      <x:c r="A52" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:2">
+      <x:c r="A53" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:2">
+      <x:c r="A54" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:2">
+      <x:c r="A55" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:2">
+      <x:c r="A56" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:2">
+      <x:c r="A57" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:2">
+      <x:c r="A59" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:2">
+      <x:c r="A60" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:2">
+      <x:c r="A61" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:2">
+      <x:c r="A62" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:2">
+      <x:c r="A63" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:2">
+      <x:c r="A64" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:2">
+      <x:c r="A65" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:2">
+      <x:c r="A66" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>122</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1160,7 +1351,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B44"/>
+  <x:dimension ref="A1:B37"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1179,7 +1370,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1187,7 +1378,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1195,7 +1386,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1203,7 +1394,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1211,7 +1402,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1219,7 +1410,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1227,7 +1418,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1235,7 +1426,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1243,7 +1434,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1251,7 +1442,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1259,7 +1450,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1267,7 +1458,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1275,7 +1466,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1283,7 +1474,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1291,7 +1482,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1299,7 +1490,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1307,7 +1498,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1315,7 +1506,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1323,7 +1514,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1331,7 +1522,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1339,7 +1530,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1347,23 +1538,23 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1371,7 +1562,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1379,143 +1570,87 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>120</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:2">
-      <x:c r="A38" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="B38" s="0" t="s">
-        <x:v>121</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:2">
-      <x:c r="A39" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="B39" s="0" t="s">
-        <x:v>122</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:2">
-      <x:c r="A40" s="0" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="B40" s="0" t="s">
-        <x:v>123</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:2">
-      <x:c r="A41" s="0" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="B41" s="0" t="s">
-        <x:v>124</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:2">
-      <x:c r="A42" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="B42" s="0" t="s">
-        <x:v>125</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:2">
-      <x:c r="A43" s="0" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="B43" s="0" t="s">
-        <x:v>126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:2">
-      <x:c r="A44" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="B44" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
WIP: Implementing dual-column parsing for PDF tables
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -26,7 +26,7 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
-    <x:t>RTU MONITOR JUMPER CONTROL INHIBIT 0</x:t>
+    <x:t>RTU MONITOR JUMPER CONTROL INHIBIT</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
@@ -50,7 +50,7 @@
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA DIABLO-SHERWIN 115KV CB 5</x:t>
+    <x:t>CASA</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
@@ -68,31 +68,31 @@
     <x:t>7</x:t>
   </x:si>
   <x:si>
-    <x:t>BISHOP CREEK PLANT NO. 3 &amp; 4 115KV CB E</x:t>
+    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW 115KV CB 17</x:t>
+    <x:t>OXBOW 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW CUST CB I 10</x:t>
+    <x:t>OXBOW CUST CB</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>WWIXIE VALLEY CUST CBF Tn 1</x:t>
+    <x:t>WWIXIE VALLEY CUST CB</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>fNO. 1</x:t>
+    <x:t>fNO. 1 BANK T15KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>12</x:t>
@@ -104,7 +104,7 @@
     <x:t>13</x:t>
   </x:si>
   <x:si>
-    <x:t>fi1S5KV CB LOW GAS7AIR 19</x:t>
+    <x:t>fi1S5KV CB LOW GAS7AIR</x:t>
   </x:si>
   <x:si>
     <x:t>14</x:t>
@@ -122,13 +122,13 @@
     <x:t>16</x:t>
   </x:si>
   <x:si>
-    <x:t>INO. 1</x:t>
+    <x:t>INO. 1 BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>17</x:t>
   </x:si>
   <x:si>
-    <x:t>FNO. 1</x:t>
+    <x:t>FNO. 1 BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>18</x:t>
@@ -140,15 +140,12 @@
     <x:t>19</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF FAIL I</x:t>
+    <x:t>NO. 3 BANK SEL-387</x:t>
   </x:si>
   <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
-  </x:si>
-  <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
@@ -158,88 +155,79 @@
     <x:t>22</x:t>
   </x:si>
   <x:si>
-    <x:t>INO. 3</x:t>
+    <x:t>INO. 3 BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>23</x:t>
   </x:si>
   <x:si>
+    <x:t>INO. 3 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>24</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ POT FAIL 54</x:t>
+    <x:t>115KV UNDERFREQ POT FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>25</x:t>
   </x:si>
   <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
+    <x:t>EAST 115KV BUS</x:t>
   </x:si>
   <x:si>
     <x:t>26</x:t>
   </x:si>
   <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
-  </x:si>
-  <x:si>
     <x:t>27</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+    <x:t>WEST 115KV BUS</x:t>
   </x:si>
   <x:si>
     <x:t>28</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
-  </x:si>
-  <x:si>
     <x:t>29</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
-  </x:si>
-  <x:si>
     <x:t>30</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV DFR FAIL 64</x:t>
+    <x:t>115KV DFR FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>31</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV DFR OPERATION 65</x:t>
+    <x:t>115KV DFR OPERATION</x:t>
   </x:si>
   <x:si>
     <x:t>32</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ RELAY PICK UP 66</x:t>
+    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
   </x:si>
   <x:si>
     <x:t>33</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ RELAY FAIL 67</x:t>
+    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>34</x:t>
   </x:si>
   <x:si>
-    <x:t>ICASA DIABLO REACTOR OV</x:t>
+    <x:t>ICASA</x:t>
   </x:si>
   <x:si>
     <x:t>35</x:t>
   </x:si>
   <x:si>
-    <x:t>ICASA DIABLO REACTOR UV</x:t>
-  </x:si>
-  <x:si>
     <x:t>36</x:t>
   </x:si>
   <x:si>
-    <x:t>ICASA D-SHERWIN REACTOR CSF 71</x:t>
+    <x:t>ICASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
     <x:t>37</x:t>
@@ -269,7 +257,7 @@
     <x:t>41</x:t>
   </x:si>
   <x:si>
-    <x:t>ADDED POINT FOR 115KV LINE POS. 4</x:t>
+    <x:t>ADDED POINT FOR 115KV LINE POS.</x:t>
   </x:si>
   <x:si>
     <x:t>42</x:t>
@@ -281,34 +269,22 @@
     <x:t>43</x:t>
   </x:si>
   <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM T15KV SH. 2</x:t>
+    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS.</x:t>
   </x:si>
   <x:si>
     <x:t>44</x:t>
   </x:si>
   <x:si>
-    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>45</x:t>
-  </x:si>
-  <x:si>
     <x:t>ONE LINE FOR CONSTRUCTION 3</x:t>
   </x:si>
   <x:si>
-    <x:t>fF F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos. 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fF L RESERVED FOR 115KV LINE POs. 8</x:t>
+    <x:t>f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fF L RESERVED FOR 115KV LINE POs.</x:t>
   </x:si>
   <x:si>
     <x:t>115KV LBFB ARMED</x:t>
@@ -320,58 +296,64 @@
     <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
   </x:si>
   <x:si>
-    <x:t>I115KV CB 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f115KV CB 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TS5KV CB 11" LBFB RELAY PS 16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB 11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN15KV CB 13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB 15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN15KV CB 17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV cB 11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115K CB 15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB 23</x:t>
+    <x:t>I115KV CB 1 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f115KV CB 2 LBFB RELAY PS % FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB 2 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 3 LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 3 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 5 LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 5 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 7 LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 7 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 9 LBFB RELAY PS 1% FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 9 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TS5KV CB 11" LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IN15KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 5 TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB 9 TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV cB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115K CB</x:t>
   </x:si>
   <x:si>
     <x:t>SEL-2020 COM</x:t>
@@ -389,10 +371,7 @@
     <x:t>ISILVERPEAK C C TCT</x:t>
   </x:si>
   <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM 115KV SH. 1</x:t>
+    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV</x:t>
   </x:si>
   <x:si>
     <x:t>ED RTU SYSTEM 115-55KV —— ADDED OPD ALARMS FOR D60</x:t>
@@ -764,7 +743,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B47"/>
+  <x:dimension ref="A1:B46"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -943,31 +922,31 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
         <x:v>48</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -991,159 +970,151 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
         <x:v>55</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47" spans="1:2">
-      <x:c r="A47" s="0" t="s">
-        <x:v>91</x:v>
-      </x:c>
-      <x:c r="B47" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1160,7 +1131,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B44"/>
+  <x:dimension ref="A1:B40"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1179,7 +1150,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1187,7 +1158,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1195,7 +1166,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1203,7 +1174,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1211,7 +1182,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1219,7 +1190,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1227,7 +1198,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1235,7 +1206,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1243,7 +1214,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1251,7 +1222,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1259,7 +1230,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1267,7 +1238,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1275,7 +1246,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1283,7 +1254,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1291,7 +1262,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1299,7 +1270,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1307,7 +1278,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1315,7 +1286,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1323,7 +1294,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1331,7 +1302,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1339,31 +1310,31 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1371,7 +1342,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1379,7 +1350,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1387,135 +1358,103 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>123</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:2">
-      <x:c r="A41" s="0" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="B41" s="0" t="s">
-        <x:v>124</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:2">
-      <x:c r="A42" s="0" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="B42" s="0" t="s">
-        <x:v>125</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:2">
-      <x:c r="A43" s="0" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="B43" s="0" t="s">
-        <x:v>126</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:2">
-      <x:c r="A44" s="0" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="B44" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Improved dual-column parsing with better filtering
- Added length checks (> 3 chars) to filter out junk entries
- Skip sections with state keywords (OPEN, CLOSE, ALARM, etc.)
- Added validation for multi-word point names
- Currently extracting 66 Status rows (target 196) and 45 Analog rows (target 90)
- Filtering out "Spare" entries correctly

Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -32,15 +32,15 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
+    <x:t>GATE ~\</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
     <x:t>STINGER SWITCH 115KV 1</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ftnyo 115KV CB 1</x:t>
-  </x:si>
-  <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
@@ -50,112 +50,112 @@
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA</x:t>
+    <x:t>HAIWEE-INYOKERN 115KV CB 7</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV CB 7</x:t>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV CB 9</x:t>
   </x:si>
   <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV CB 9</x:t>
+    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
   </x:si>
   <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
-    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
+    <x:t>OXBOW CUST CB</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW 115KV CB</x:t>
+    <x:t>BUS TIE 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW CUST CB</x:t>
+    <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>WWIXIE VALLEY CUST CB</x:t>
+    <x:t>fi1S5KV CB LOW GAS7AIR</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>fNO. 1 BANK T15KV CB</x:t>
+    <x:t>115KV CB GEN</x:t>
   </x:si>
   <x:si>
     <x:t>12</x:t>
   </x:si>
   <x:si>
-    <x:t>ENTRY</x:t>
+    <x:t>or 3-34</x:t>
   </x:si>
   <x:si>
     <x:t>13</x:t>
   </x:si>
   <x:si>
-    <x:t>fi1S5KV CB LOW GAS7AIR</x:t>
+    <x:t>oI 3-38</x:t>
   </x:si>
   <x:si>
     <x:t>14</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV CB GEN</x:t>
+    <x:t>FTRANS BK SUDDENTPRESS RESET “1 -</x:t>
   </x:si>
   <x:si>
     <x:t>15</x:t>
   </x:si>
   <x:si>
-    <x:t>FTRANS BK SUDDENTPRESS RESET “1 -</x:t>
+    <x:t>INO. 1 BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>16</x:t>
   </x:si>
   <x:si>
-    <x:t>INO. 1 BANK SEL-351 0C TRIP</x:t>
+    <x:t>FNO. 1 BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>17</x:t>
   </x:si>
   <x:si>
-    <x:t>FNO. 1 BANK C30 FAIL</x:t>
+    <x:t>NO. 1 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>18</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 1 BANK 63X FAIL</x:t>
+    <x:t>NO. 3 BANK SEL-387</x:t>
   </x:si>
   <x:si>
     <x:t>19</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-387</x:t>
-  </x:si>
-  <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+    <x:t>INO. 3 BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>22</x:t>
   </x:si>
   <x:si>
-    <x:t>INO. 3 BANK SEL-351 OC TRIP</x:t>
+    <x:t>NO. 3 BANK C30 TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>23</x:t>
@@ -173,118 +173,253 @@
     <x:t>25</x:t>
   </x:si>
   <x:si>
+    <x:t>l RESERVED FOR 115KV LINE POS.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
     <x:t>EAST 115KV BUS</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
     <x:t>27</x:t>
   </x:si>
   <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ol 4-58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
     <x:t>WEST 115KV BUS</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
     <x:t>30</x:t>
   </x:si>
   <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5640046 W43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 4-64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
     <x:t>115KV DFR FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>31</x:t>
+    <x:t>35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dI 5-65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR OPERATION</x:t>
   </x:si>
   <x:si>
-    <x:t>32</x:t>
+    <x:t>37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 5-66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
   </x:si>
   <x:si>
-    <x:t>33</x:t>
+    <x:t>39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oI 5-67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
+    <x:t>41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5704103 w48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA</x:t>
   </x:si>
   <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36</x:t>
+    <x:t>43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>904562794 “Ts 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
-    <x:t>37</x:t>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KVD60/A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47</x:t>
   </x:si>
   <x:si>
     <x:t>ICASA D-SHERWIN REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>38</x:t>
+    <x:t>48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49</x:t>
   </x:si>
   <x:si>
     <x:t>FCASA D-SHERWIN REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cD SHUNT REACTOR TROUBLE AL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40</x:t>
+    <x:t>50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>or 5-74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TT 105</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p 5-78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56</x:t>
   </x:si>
   <x:si>
     <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
+    <x:t>57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58</x:t>
   </x:si>
   <x:si>
     <x:t>ADDED POINT FOR 115KV LINE POS.</x:t>
   </x:si>
   <x:si>
-    <x:t>42</x:t>
+    <x:t>59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VM VM ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
   </x:si>
   <x:si>
     <x:t>ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROOED,POINTS FOR TTSKV LINE POS. 3, BUS TIE POS. 1X,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VM vM ve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63</x:t>
   </x:si>
   <x:si>
     <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS.</x:t>
   </x:si>
   <x:si>
-    <x:t>44</x:t>
+    <x:t>64</x:t>
   </x:si>
   <x:si>
     <x:t>ONE LINE FOR CONSTRUCTION 3</x:t>
   </x:si>
   <x:si>
-    <x:t>f</x:t>
-  </x:si>
-  <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fF L RESERVED FOR 115KV LINE POs.</x:t>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REPL'D RLY SEL-311C WITH D60 FOR 115KV LINE POS. 3.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK A A ToT ' \</x:t>
+  </x:si>
+  <x:si>
+    <x:t>164 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV D60 OPD TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV D60 OPD A/S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>248 Lt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>170 1</x:t>
   </x:si>
   <x:si>
     <x:t>115KV LBFB ARMED</x:t>
@@ -299,7 +434,7 @@
     <x:t>I115KV CB 1 LBFB RELAY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>f115KV CB 2 LBFB RELAY PS % FAIL</x:t>
+    <x:t>193 1</x:t>
   </x:si>
   <x:si>
     <x:t>l115KV CB 2 LBFB RELAY FAIL</x:t>
@@ -344,7 +479,7 @@
     <x:t>115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV CB 5 TCM</x:t>
+    <x:t>218 166</x:t>
   </x:si>
   <x:si>
     <x:t>l115KV CB 9 TCM</x:t>
@@ -353,9 +488,6 @@
     <x:t>l115KV cB</x:t>
   </x:si>
   <x:si>
-    <x:t>115K CB</x:t>
-  </x:si>
-  <x:si>
     <x:t>SEL-2020 COM</x:t>
   </x:si>
   <x:si>
@@ -371,13 +503,25 @@
     <x:t>ISILVERPEAK C C TCT</x:t>
   </x:si>
   <x:si>
+    <x:t>SILVERPEAK C GRD TcT ps</x:t>
+  </x:si>
+  <x:si>
     <x:t>ANALOG PT LISTING RTU SYSTEM 115KV</x:t>
   </x:si>
   <x:si>
+    <x:t>VM vM SS</x:t>
+  </x:si>
+  <x:si>
     <x:t>ED RTU SYSTEM 115-55KV —— ADDED OPD ALARMS FOR D60</x:t>
   </x:si>
   <x:si>
+    <x:t>904562794 SH. 2</x:t>
+  </x:si>
+  <x:si>
     <x:t>ONE LINE FOR CONSTRUCTION 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISSUED FOR CONSTRUCTION 08-31-20</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -743,7 +887,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B46"/>
+  <x:dimension ref="A1:B67"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -914,15 +1058,15 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
         <x:v>42</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -970,15 +1114,15 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
         <x:v>54</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -986,20 +1130,20 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
         <x:v>59</x:v>
@@ -1007,18 +1151,18 @@
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1042,79 +1186,247 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>83</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:2">
+      <x:c r="A47" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:2">
+      <x:c r="A48" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:2">
+      <x:c r="A49" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:2">
+      <x:c r="A50" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:2">
+      <x:c r="A51" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:2">
+      <x:c r="A52" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:2">
+      <x:c r="A53" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:2">
+      <x:c r="A54" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:2">
+      <x:c r="A55" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:2">
+      <x:c r="A56" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:2">
+      <x:c r="A57" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:2">
+      <x:c r="A59" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:2">
+      <x:c r="A60" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:2">
+      <x:c r="A61" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:2">
+      <x:c r="A62" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:2">
+      <x:c r="A63" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:2">
+      <x:c r="A64" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:2">
+      <x:c r="A65" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:2">
+      <x:c r="A66" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>128</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1131,7 +1443,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B40"/>
+  <x:dimension ref="A1:B46"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1150,7 +1462,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1158,7 +1470,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1166,7 +1478,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1174,7 +1486,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1182,7 +1494,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1190,7 +1502,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1198,7 +1510,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1206,7 +1518,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1214,7 +1526,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1222,7 +1534,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1230,7 +1542,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1238,7 +1550,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1246,7 +1558,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1254,7 +1566,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1262,7 +1574,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1270,7 +1582,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1278,7 +1590,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1286,7 +1598,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1294,7 +1606,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1302,15 +1614,15 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1318,7 +1630,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1326,7 +1638,7 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -1334,7 +1646,7 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1342,7 +1654,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1350,7 +1662,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1358,15 +1670,15 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -1374,39 +1686,39 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1414,7 +1726,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -1422,7 +1734,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -1430,31 +1742,79 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:2">
+      <x:c r="A41" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:2">
+      <x:c r="A42" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:2">
+      <x:c r="A43" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:2">
+      <x:c r="A44" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:2">
+      <x:c r="A45" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:2">
+      <x:c r="A46" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>168</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Changes before error encountered
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -44,15 +44,15 @@
     <x:t>3</x:t>
   </x:si>
   <x:si>
+    <x:t>IINYO 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
     <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NYO 115KV CB</x:t>
-  </x:si>
-  <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
@@ -80,19 +80,19 @@
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV CB</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV CB</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>BISHOP CREEK PLANT NO.</x:t>
+    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
   </x:si>
   <x:si>
     <x:t>12</x:t>
@@ -110,13 +110,13 @@
     <x:t>14</x:t>
   </x:si>
   <x:si>
-    <x:t>DIXIE VALLEY CUST CBF</x:t>
+    <x:t>DIXIE VALLEY CUST CB</x:t>
   </x:si>
   <x:si>
     <x:t>15</x:t>
   </x:si>
   <x:si>
-    <x:t>NO.</x:t>
+    <x:t>NO. 1 BANK 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>16</x:t>
@@ -134,7 +134,7 @@
     <x:t>18</x:t>
   </x:si>
   <x:si>
-    <x:t>1155KV CB LOW GAS7AIR</x:t>
+    <x:t>115KV CB LOW GAS/AIR</x:t>
   </x:si>
   <x:si>
     <x:t>19</x:t>
@@ -152,6 +152,9 @@
     <x:t>21</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
+  </x:si>
+  <x:si>
     <x:t>22</x:t>
   </x:si>
   <x:si>
@@ -173,27 +176,51 @@
     <x:t>25</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>26</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 1 BANK C30 FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>27</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 1 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>28</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>29</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>30</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>31</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
+  </x:si>
+  <x:si>
     <x:t>32</x:t>
   </x:si>
   <x:si>
+    <x:t>NO. 3 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
     <x:t>33</x:t>
   </x:si>
   <x:si>
@@ -227,7 +254,7 @@
     <x:t>38</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KVID6O</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KVID6O</x:t>
   </x:si>
   <x:si>
     <x:t>39</x:t>
@@ -239,7 +266,7 @@
     <x:t>40</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KVD60JA/S</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KVD60JA/S</x:t>
   </x:si>
   <x:si>
     <x:t>41</x:t>
@@ -251,7 +278,7 @@
     <x:t>42</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>43</x:t>
@@ -263,7 +290,7 @@
     <x:t>44</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>45</x:t>
@@ -281,13 +308,13 @@
     <x:t>47</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
     <x:t>48</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
     <x:t>49</x:t>
@@ -305,19 +332,19 @@
     <x:t>51</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KVD60RLY FAIL</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KVD60RLY FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>52</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA D-SHERWIN REACTOR CSF</x:t>
+    <x:t>CASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
     <x:t>53</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KVD60/A/S</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KVD60/A/S</x:t>
   </x:si>
   <x:si>
     <x:t>54</x:t>
@@ -329,7 +356,7 @@
     <x:t>55</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
     <x:t>56</x:t>
@@ -341,25 +368,25 @@
     <x:t>57</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL</x:t>
+    <x:t>COSO-HATNEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>58</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L CHAN FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>59</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S</x:t>
+    <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
     <x:t>60</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S</x:t>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
     <x:t>61</x:t>
@@ -371,7 +398,7 @@
     <x:t>62</x:t>
   </x:si>
   <x:si>
-    <x:t>HATWEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+    <x:t>HATWEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
     <x:t>63</x:t>
@@ -383,7 +410,7 @@
     <x:t>64</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD</x:t>
+    <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
     <x:t>SILVERPEAK A C TCT</x:t>
@@ -990,351 +1017,351 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
       <x:c r="A47" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
       <x:c r="A48" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:2">
       <x:c r="A49" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:2">
       <x:c r="A50" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:2">
       <x:c r="A51" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:2">
       <x:c r="A52" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:2">
       <x:c r="A53" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:2">
       <x:c r="A54" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:2">
       <x:c r="A55" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:2">
       <x:c r="A56" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:2">
       <x:c r="A57" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:2">
       <x:c r="A58" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:2">
       <x:c r="A59" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:2">
       <x:c r="A60" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:2">
       <x:c r="A61" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:2">
       <x:c r="A62" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:2">
       <x:c r="A63" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:2">
       <x:c r="A64" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:2">
       <x:c r="A65" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:2">
       <x:c r="A66" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1370,7 +1397,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1378,7 +1405,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1386,7 +1413,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1394,7 +1421,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1402,7 +1429,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1410,7 +1437,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1418,7 +1445,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1426,7 +1453,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1434,7 +1461,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1442,7 +1469,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1450,7 +1477,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1458,7 +1485,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1466,7 +1493,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1474,7 +1501,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1482,7 +1509,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1490,7 +1517,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1498,7 +1525,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1506,7 +1533,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1514,7 +1541,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1522,7 +1549,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1530,7 +1557,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1538,119 +1565,119 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement processing of all tables in PDF files regardless of type
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -26,216 +26,270 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
+    <x:t>SILVERPEAK A C TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB ARMED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV cB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115K CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEL-2020 COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE A TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE B TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE GRD TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK C C TCT</x:t>
+  </x:si>
+  <x:si>
     <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
   </x:si>
   <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
     <x:t>STINGER SWITCH 115KV</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
     <x:t>FUPS TROUBLE</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
     <x:t>IINYO 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
     <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV RELAY BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV BACK-UP BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
     <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV OPERATING BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
     <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
   </x:si>
   <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
     <x:t>OXBOW 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
     <x:t>OXBOW CUST CB</x:t>
   </x:si>
   <x:si>
-    <x:t>14</x:t>
-  </x:si>
-  <x:si>
     <x:t>DIXIE VALLEY CUST CB</x:t>
   </x:si>
   <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 1 BANK 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
     <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
     <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV CB LOW GAS/AIR</x:t>
   </x:si>
   <x:si>
-    <x:t>19</x:t>
-  </x:si>
-  <x:si>
     <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
   </x:si>
   <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV CB GEN</x:t>
   </x:si>
   <x:si>
-    <x:t>21</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
   </x:si>
   <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>23</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>24</x:t>
-  </x:si>
-  <x:si>
     <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
   </x:si>
   <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 1 BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>27</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 1 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>31</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
     <x:t>NO. 3 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
     <x:t>115KV UNDERFREQ POT FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
-  </x:si>
-  <x:si>
     <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
     <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
@@ -411,60 +465,6 @@
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SILVERPEAK A C TCT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB ARMED</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV cB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115K CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEL-2020 COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE A TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE B TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE GRD TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SILVERPEAK C C TCT</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -830,7 +830,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B66"/>
+  <x:dimension ref="A1:B102"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -929,439 +929,727 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
       <x:c r="A13" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
       <x:c r="A14" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
       <x:c r="A15" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
       <x:c r="A16" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
       <x:c r="A18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
       <x:c r="A19" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
       <x:c r="A20" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
       <x:c r="A21" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
       <x:c r="A47" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
       <x:c r="A48" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:2">
       <x:c r="A49" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:2">
       <x:c r="A50" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:2">
       <x:c r="A51" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:2">
       <x:c r="A52" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:2">
       <x:c r="A53" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:2">
       <x:c r="A54" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:2">
       <x:c r="A55" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:2">
       <x:c r="A56" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:2">
       <x:c r="A57" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:2">
       <x:c r="A58" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:2">
       <x:c r="A59" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:2">
       <x:c r="A60" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:2">
       <x:c r="A61" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:2">
       <x:c r="A62" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:2">
       <x:c r="A63" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:2">
       <x:c r="A64" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:2">
       <x:c r="A65" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:2">
       <x:c r="A66" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:2">
+      <x:c r="A76" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:2">
+      <x:c r="A77" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:2">
+      <x:c r="A78" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:2">
+      <x:c r="A79" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:2">
+      <x:c r="A80" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:2">
+      <x:c r="A81" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:2">
+      <x:c r="A82" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:2">
+      <x:c r="A83" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:2">
+      <x:c r="A84" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:2">
+      <x:c r="A85" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:2">
+      <x:c r="A86" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:2">
+      <x:c r="A87" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:2">
+      <x:c r="A88" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:2">
+      <x:c r="A89" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:2">
+      <x:c r="A90" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:2">
+      <x:c r="A91" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:2">
+      <x:c r="A92" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:2">
+      <x:c r="A93" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="B66" s="0" t="s">
+      <x:c r="B93" s="0" t="s">
         <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:2">
+      <x:c r="A94" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:2">
+      <x:c r="A95" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:2">
+      <x:c r="A96" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:2">
+      <x:c r="A97" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:2">
+      <x:c r="A98" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:2">
+      <x:c r="A99" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:2">
+      <x:c r="A100" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:2">
+      <x:c r="A101" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:2">
+      <x:c r="A102" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>149</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1378,7 +1666,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B37"/>
+  <x:dimension ref="A1:B102"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1397,7 +1685,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1405,7 +1693,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1413,7 +1701,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1421,7 +1709,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1429,7 +1717,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1437,7 +1725,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1445,7 +1733,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1453,7 +1741,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1461,7 +1749,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1469,7 +1757,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1477,206 +1765,726 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
       <x:c r="A13" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
       <x:c r="A14" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
       <x:c r="A15" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
       <x:c r="A16" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
       <x:c r="A18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
       <x:c r="A19" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
       <x:c r="A20" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
       <x:c r="A21" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:2">
+      <x:c r="A38" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:2">
+      <x:c r="A39" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:2">
+      <x:c r="A40" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:2">
+      <x:c r="A41" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:2">
+      <x:c r="A42" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:2">
+      <x:c r="A43" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:2">
+      <x:c r="A44" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:2">
+      <x:c r="A45" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:2">
+      <x:c r="A46" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:2">
+      <x:c r="A47" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:2">
+      <x:c r="A48" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:2">
+      <x:c r="A49" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:2">
+      <x:c r="A50" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:2">
+      <x:c r="A51" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:2">
+      <x:c r="A52" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:2">
+      <x:c r="A53" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:2">
+      <x:c r="A54" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="B37" s="0" t="s">
+    </x:row>
+    <x:row r="55" spans="1:2">
+      <x:c r="A55" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:2">
+      <x:c r="A56" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:2">
+      <x:c r="A57" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:2">
+      <x:c r="A59" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:2">
+      <x:c r="A60" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:2">
+      <x:c r="A61" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:2">
+      <x:c r="A62" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:2">
+      <x:c r="A63" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:2">
+      <x:c r="A64" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:2">
+      <x:c r="A65" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:2">
+      <x:c r="A66" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:2">
+      <x:c r="A76" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:2">
+      <x:c r="A77" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:2">
+      <x:c r="A78" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:2">
+      <x:c r="A79" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:2">
+      <x:c r="A80" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:2">
+      <x:c r="A81" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:2">
+      <x:c r="A82" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:2">
+      <x:c r="A83" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:2">
+      <x:c r="A84" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:2">
+      <x:c r="A85" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:2">
+      <x:c r="A86" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:2">
+      <x:c r="A87" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:2">
+      <x:c r="A88" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:2">
+      <x:c r="A89" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:2">
+      <x:c r="A90" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:2">
+      <x:c r="A91" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:2">
+      <x:c r="A92" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:2">
+      <x:c r="A93" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:2">
+      <x:c r="A94" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:2">
+      <x:c r="A95" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:2">
+      <x:c r="A96" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:2">
+      <x:c r="A97" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:2">
+      <x:c r="A98" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:2">
+      <x:c r="A99" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:2">
+      <x:c r="A100" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:2">
+      <x:c r="A101" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:2">
+      <x:c r="A102" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
         <x:v>149</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Fix multi-table parsing for PDFs with side-by-side column layouts
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -116,298 +116,334 @@
     <x:t>15</x:t>
   </x:si>
   <x:si>
+    <x:t>BUS TIE 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
     <x:t>NO. 1 BANK 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>16</x:t>
+    <x:t>17</x:t>
   </x:si>
   <x:si>
     <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
+    <x:t>18</x:t>
   </x:si>
   <x:si>
     <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
-    <x:t>18</x:t>
+    <x:t>19</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB LOW GAS/AIR</x:t>
   </x:si>
   <x:si>
-    <x:t>19</x:t>
+    <x:t>20</x:t>
   </x:si>
   <x:si>
     <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
   </x:si>
   <x:si>
-    <x:t>20</x:t>
+    <x:t>21</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB GEN</x:t>
   </x:si>
   <x:si>
-    <x:t>21</x:t>
+    <x:t>22</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
   </x:si>
   <x:si>
-    <x:t>22</x:t>
+    <x:t>23</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>23</x:t>
+    <x:t>24</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>24</x:t>
+    <x:t>25</x:t>
   </x:si>
   <x:si>
     <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
   </x:si>
   <x:si>
-    <x:t>25</x:t>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L RESERVED FOR 115KV LINE Pos. 1 l</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
+    <x:t>28</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>27</x:t>
+    <x:t>29</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
+    <x:t>30</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>29</x:t>
+    <x:t>31</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>30</x:t>
+    <x:t>32</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>31</x:t>
+    <x:t>33</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>32</x:t>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK C30 TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>33</x:t>
+    <x:t>36</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ POT FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
+    <x:t>37</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>35</x:t>
+    <x:t>38</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>36</x:t>
+    <x:t>39</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>37</x:t>
+    <x:t>40</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>38</x:t>
+    <x:t>41</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVID6O</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
+    <x:t>42</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>40</x:t>
+    <x:t>43</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVD60JA/S</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
+    <x:t>44</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>42</x:t>
+    <x:t>45</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
+    <x:t>46</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR OPERATION</x:t>
   </x:si>
   <x:si>
-    <x:t>44</x:t>
+    <x:t>47</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>45</x:t>
+    <x:t>48</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
   </x:si>
   <x:si>
-    <x:t>46</x:t>
+    <x:t>49</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>47</x:t>
+    <x:t>50</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>48</x:t>
+    <x:t>51</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>49</x:t>
+    <x:t>52</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>50</x:t>
+    <x:t>53</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>51</x:t>
+    <x:t>54</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>52</x:t>
+    <x:t>55</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
-    <x:t>53</x:t>
+    <x:t>56</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60/A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>54</x:t>
+    <x:t>57</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>55</x:t>
+    <x:t>58</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>56</x:t>
+    <x:t>59</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>57</x:t>
+    <x:t>60</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HATNEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>58</x:t>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR OC RELAY BUS AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L CHAN FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>59</x:t>
+    <x:t>63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR DC BACK-UP BUS AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>60</x:t>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REACTOR OPERATING BUS AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>61</x:t>
+    <x:t>67</x:t>
   </x:si>
   <x:si>
     <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>62</x:t>
+    <x:t>68</x:t>
   </x:si>
   <x:si>
     <x:t>HATWEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
-    <x:t>63</x:t>
+    <x:t>69</x:t>
   </x:si>
   <x:si>
     <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>64</x:t>
+    <x:t>70</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
@@ -416,6 +452,9 @@
     <x:t>SILVERPEAK A C TCT</x:t>
   </x:si>
   <x:si>
+    <x:t>PROTECTION RELAYS ALARMS</x:t>
+  </x:si>
+  <x:si>
     <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
   </x:si>
   <x:si>
@@ -465,6 +504,9 @@
   </x:si>
   <x:si>
     <x:t>SILVERPEAK C C TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK C GRD TcT ps</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -830,7 +872,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B66"/>
+  <x:dimension ref="A1:B72"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1362,6 +1404,54 @@
       </x:c>
       <x:c r="B66" s="0" t="s">
         <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>143</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1378,7 +1468,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B37"/>
+  <x:dimension ref="A1:B40"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1397,7 +1487,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1405,7 +1495,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1413,7 +1503,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1421,7 +1511,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1429,7 +1519,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1437,7 +1527,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1445,7 +1535,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1453,7 +1543,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1461,7 +1551,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1469,7 +1559,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1477,7 +1567,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1485,7 +1575,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1493,7 +1583,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1501,7 +1591,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1509,7 +1599,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1517,7 +1607,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1525,7 +1615,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1533,7 +1623,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1541,7 +1631,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1549,7 +1639,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1557,7 +1647,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1565,7 +1655,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1573,7 +1663,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -1581,7 +1671,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1589,7 +1679,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1597,7 +1687,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1605,7 +1695,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -1613,7 +1703,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -1621,7 +1711,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -1629,7 +1719,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -1637,7 +1727,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -1645,7 +1735,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -1653,7 +1743,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1661,7 +1751,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -1669,7 +1759,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -1677,7 +1767,31 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>160</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:2">
+      <x:c r="A38" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:2">
+      <x:c r="A39" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:2">
+      <x:c r="A40" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>163</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement simplified PDF point extraction with two-column output
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -6,8 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Status" sheetId="1" r:id="rId2"/>
-    <x:sheet name="Analog" sheetId="2" r:id="rId3"/>
+    <x:sheet name="Points" sheetId="1" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -21,6 +20,225 @@
   </x:si>
   <x:si>
     <x:t>Point Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ADDED POINT FOR 115KV LINE POS. RELAY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tnyo 115KV CB F———-~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NYO 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-INYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BISHOP CREEK PLANT NO. 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW 115KV CB 17 lg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW CUST CB I} 10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WWIXIE VALLEY CUST CBF Tn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK T15KV CB 11 15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ENTRY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>i1S5KV CB LOW GAS7AIR 19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV_CB GEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FTRANS BK SUDDENTPRESS RESET “1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK SEL-351 0C TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FNO. BANK C30 FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK SEL-387 DIFF FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK SEL-387 DIFF TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK SEL-351 OC TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV_UNDERFREQ POT FAIL 54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR FAIL 64 1B19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR OPERATION 65 1820</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY PICK UP 66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY FAIL 67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR CSF 71</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FCASA D-SHERWIN REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cD SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB ARMED 189 1F1 DI 12-190 NOTE W154 271</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB TRIP 190 1F2 DI 12-191 NOTE W155 272_</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15KV CB I'LBFB RELAY PS FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY PS FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY PS FAIL 195 1F7 DI 13-196 5640022 W160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY FAIL 196 1F8 DI 13-197 5640022 W161</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY PS FAIL 197 1F9 DI 13-198 5640026 wi62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY FAIL 198 1F10 DI 13-199 5640026 W163</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY PS FAIL 199 Tal DI 13-200 5640030 W164</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY FAIL 200 1F12 DI 13-201 5640030 W165</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY PS 1% FAIL 201 1F13 DI 13-202 5640034 W166</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LBFB RELAY FAIL 202 1F14 DI 13-203 5640034 W167</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TS5KV CB 11" LBFB RELAY PS 16 FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 11 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>N15KV CB 13 LBFB RELAY PS FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 15 LBFB RELAY PS FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 15 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>N15KV CB 17 LBFB RELAY PS FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 17 LBFB RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 23 LBFB RELAY PS FAIL 2u1 1F23 DI 14-212 5640038 W176</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 23 LBFB RELAY FAIL 212 1F24 DI 14-213 5640038 WI77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV cB 11 TCM 221 169 DI 14-222 W186 2. "Vv" BLOCK NDICATES VIRTUAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115K CB 15 TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 23 TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEL-2020 COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>coso HWE TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>coso HWE GRD TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK TCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ONE LINE FOR CONSTRUCTION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. RLY'S 903536612 SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIG PT LISTING RTU SYSTEM 115KV SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIG PT LISTING RTU SYSTEM T15KV SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV LINE POS. RELAY 903536612 DIGITAL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -386,11 +604,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B1"/>
+  <x:dimension ref="A1:B80"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="13.567768" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="92.282054" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">
@@ -400,32 +622,636 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:B1"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:2">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0">
         <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:2">
+      <x:c r="A17" s="0">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="0">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:2">
+      <x:c r="A19" s="0">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:2">
+      <x:c r="A20" s="0">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:2">
+      <x:c r="A21" s="0">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:2">
+      <x:c r="A22" s="0">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:2">
+      <x:c r="A23" s="0">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:2">
+      <x:c r="A24" s="0">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:2">
+      <x:c r="A25" s="0">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:2">
+      <x:c r="A26" s="0">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:2">
+      <x:c r="A27" s="0">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:2">
+      <x:c r="A28" s="0">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:2">
+      <x:c r="A29" s="0">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:2">
+      <x:c r="A30" s="0">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:2">
+      <x:c r="A31" s="0">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:2">
+      <x:c r="A32" s="0">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:2">
+      <x:c r="A33" s="0">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:2">
+      <x:c r="A34" s="0">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:2">
+      <x:c r="A35" s="0">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:2">
+      <x:c r="A36" s="0">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:2">
+      <x:c r="A37" s="0">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:2">
+      <x:c r="A38" s="0">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:2">
+      <x:c r="A39" s="0">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:2">
+      <x:c r="A40" s="0">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:2">
+      <x:c r="A41" s="0">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:2">
+      <x:c r="A42" s="0">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:2">
+      <x:c r="A43" s="0">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:2">
+      <x:c r="A44" s="0">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:2">
+      <x:c r="A45" s="0">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:2">
+      <x:c r="A46" s="0">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:2">
+      <x:c r="A47" s="0">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:2">
+      <x:c r="A48" s="0">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:2">
+      <x:c r="A49" s="0">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:2">
+      <x:c r="A50" s="0">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:2">
+      <x:c r="A51" s="0">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:2">
+      <x:c r="A52" s="0">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:2">
+      <x:c r="A53" s="0">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:2">
+      <x:c r="A54" s="0">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:2">
+      <x:c r="A55" s="0">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:2">
+      <x:c r="A56" s="0">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:2">
+      <x:c r="A57" s="0">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="0">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:2">
+      <x:c r="A59" s="0">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:2">
+      <x:c r="A60" s="0">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:2">
+      <x:c r="A61" s="0">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:2">
+      <x:c r="A62" s="0">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:2">
+      <x:c r="A63" s="0">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:2">
+      <x:c r="A64" s="0">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:2">
+      <x:c r="A65" s="0">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:2">
+      <x:c r="A66" s="0">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0">
+        <x:v>223</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0">
+        <x:v>239</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:2">
+      <x:c r="A76" s="0">
+        <x:v>585409</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:2">
+      <x:c r="A77" s="0">
+        <x:v>5640064</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:2">
+      <x:c r="A78" s="0">
+        <x:v>5640065</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:2">
+      <x:c r="A79" s="0">
+        <x:v>5640066</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:2">
+      <x:c r="A80" s="0">
+        <x:v>5640067</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>74</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement sequential point numbering and filtering
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -23,448 +23,481 @@
     <x:t>Point Name</x:t>
   </x:si>
   <x:si>
-    <x:t>0</x:t>
+    <x:t>1</x:t>
   </x:si>
   <x:si>
     <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
   </x:si>
   <x:si>
-    <x:t>1</x:t>
+    <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>STINGER SWITCH 115KV</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IINYO 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INYO 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW CUST CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIXIE VALLEY CUST CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 4f—</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ENTRY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB LOW GAS/AIR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB GEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE 2a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SPARE x f—i—</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK C30 FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 1 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. 3 BANK 63X FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ POT FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR OPERATION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA DIABLO REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR CS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR OV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CASA D-SHERWIN REACTOR UV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49</x:t>
   </x:si>
   <x:si>
     <x:t>FUPS TROUBLE</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IINYO 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INYO 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
+    <x:t>50</x:t>
   </x:si>
   <x:si>
     <x:t>115KV RELAY BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>6</x:t>
+    <x:t>51</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BACK-UP BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
+    <x:t>52</x:t>
   </x:si>
   <x:si>
     <x:t>115KV OPERATING BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OXBOW 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OXBOW CUST CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIXIE VALLEY CUST CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 1 BANK 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16</x:t>
+    <x:t>53</x:t>
   </x:si>
   <x:si>
     <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ENTRY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB LOW GAS/AIR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19</x:t>
+    <x:t>54</x:t>
   </x:si>
   <x:si>
     <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
   </x:si>
   <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB GEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21</x:t>
+    <x:t>55</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
   </x:si>
   <x:si>
-    <x:t>22</x:t>
+    <x:t>56</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>23</x:t>
+    <x:t>57</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 1 BANK C30 FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 1 BANK 63X FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. 3 BANK 63X FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ POT FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>38</x:t>
+    <x:t>58</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVID6O</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40</x:t>
+    <x:t>59</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVD60JA/S</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV DFR FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>42</x:t>
+    <x:t>60</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV DFR OPERATION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>44</x:t>
+    <x:t>61</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>47</x:t>
+    <x:t>62</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>48</x:t>
+    <x:t>63</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>49</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA DIABLO REACTOR OV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA DIABLO REACTOR UV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>51</x:t>
+    <x:t>64</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA D-SHERWIN REACTOR CS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>53</x:t>
+    <x:t>65</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60/A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>54</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA D-SHERWIN REACTOR OV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>55</x:t>
+    <x:t>66</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CASA D-SHERWIN REACTOR UV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>57</x:t>
+    <x:t>67</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HATNEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>58</x:t>
+    <x:t>68</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L CHAN FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>59</x:t>
+    <x:t>69</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>60</x:t>
+    <x:t>70</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>61</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>62</x:t>
+    <x:t>71</x:t>
   </x:si>
   <x:si>
     <x:t>HATWEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
-    <x:t>63</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64</x:t>
+    <x:t>72</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
+    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB ARMED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV LBFB TRIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l115KV cB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115K CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEL-2020 COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE A TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE B TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lcoso HWE GRD TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SILVERPEAK C C TCT</x:t>
+  </x:si>
+  <x:si>
     <x:t>SILVERPEAK A C TCT</x:t>
   </x:si>
   <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB ARMED</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV cB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115K CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEL-2020 COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE A TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE B TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE GRD TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SILVERPEAK C C TCT</x:t>
+    <x:t>SPARE on</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -830,7 +863,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B66"/>
+  <x:dimension ref="A1:B73"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -961,407 +994,463 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>32</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
       <x:c r="A18" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
       <x:c r="A19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
         <x:v>36</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
       <x:c r="A20" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
       <x:c r="A21" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
       <x:c r="A47" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
       <x:c r="A48" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:2">
       <x:c r="A49" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:2">
       <x:c r="A50" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:2">
       <x:c r="A51" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:2">
       <x:c r="A52" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:2">
       <x:c r="A53" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:2">
       <x:c r="A54" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:2">
       <x:c r="A55" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:2">
       <x:c r="A56" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:2">
       <x:c r="A57" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:2">
       <x:c r="A58" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:2">
       <x:c r="A59" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:2">
       <x:c r="A60" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:2">
       <x:c r="A61" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:2">
       <x:c r="A62" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:2">
       <x:c r="A63" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:2">
       <x:c r="A64" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:2">
       <x:c r="A65" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:2">
       <x:c r="A66" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="B66" s="0" t="s">
+      <x:c r="B68" s="0" t="s">
         <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>141</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1378,7 +1467,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B37"/>
+  <x:dimension ref="A1:B41"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1397,7 +1486,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1405,7 +1494,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1413,7 +1502,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1421,7 +1510,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1429,7 +1518,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1437,7 +1526,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1445,7 +1534,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1453,7 +1542,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1461,7 +1550,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1469,7 +1558,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1477,7 +1566,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1485,7 +1574,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1493,7 +1582,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1501,7 +1590,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1509,175 +1598,207 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
       <x:c r="A18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
       <x:c r="A19" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
       <x:c r="A20" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
       <x:c r="A21" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:2">
+      <x:c r="A38" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:2">
+      <x:c r="A39" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="B37" s="0" t="s">
-        <x:v>149</x:v>
+      <x:c r="B39" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:2">
+      <x:c r="A40" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:2">
+      <x:c r="A41" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>160</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Improve OCR artifact cleaning and filtering
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -22,58 +22,58 @@
     <x:t>Point Name</x:t>
   </x:si>
   <x:si>
-    <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADDED POINT FOR 115KV LINE POS. RELAY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tnyo 115KV CB F———-~</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NYO 115KV CB</x:t>
+    <x:t>RTU MONITOR JUMPER CONTROL INHIBIT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STINGER SWITCH 115KV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IINYO 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-INYOKERN 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COSO-HAIWEE-INYOKERN 115KV CB</x:t>
+    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>BISHOP CREEK PLANT NO. 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW 115KV CB 17 lg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OXBOW CUST CB I} 10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WWIXIE VALLEY CUST CBF Tn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO. BANK T15KV CB 11 15</x:t>
+    <x:t>OXBOW 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OXBOW CUST CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DIXIE VALLEY CUST CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
-    <x:t>i1S5KV CB LOW GAS7AIR 19</x:t>
+    <x:t>115KV CB LOW GAS/AIR</x:t>
   </x:si>
   <x:si>
     <x:t>115KV_CB GEN</x:t>
   </x:si>
   <x:si>
-    <x:t>FTRANS BK SUDDENTPRESS RESET “1</x:t>
+    <x:t>TRANS BK SUDDENTPRESS RESET “1</x:t>
   </x:si>
   <x:si>
     <x:t>NO. BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>FNO. BANK C30 FAIL</x:t>
+    <x:t>NO. BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>NO. BANK 63X FAIL</x:t>
@@ -91,7 +91,7 @@
     <x:t>NO. BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV_UNDERFREQ POT FAIL 54</x:t>
+    <x:t>115KV_UNDERFREQ POT FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS RLY FAIL</x:t>
@@ -103,16 +103,16 @@
     <x:t>WEST 115KV BUS DIFF SYS RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV DFR FAIL 64 1B19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV DFR OPERATION 65 1820</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY PICK UP 66</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV UNDERFREQ RELAY FAIL 67</x:t>
+    <x:t>115KV DFR FAIL 1B19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV DFR OPERATION 1820</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO REACTOR OV</x:t>
@@ -121,7 +121,7 @@
     <x:t>CASA DIABLO REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA D-SHERWIN REACTOR CSF 71</x:t>
+    <x:t>CASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR OV</x:t>
@@ -175,7 +175,7 @@
     <x:t>115KV CB LBFB RELAY FAIL 202 1F14 DI 13-203 5640034 W167</x:t>
   </x:si>
   <x:si>
-    <x:t>TS5KV CB 11" LBFB RELAY PS 16 FAIL</x:t>
+    <x:t>TS5KV CB 11" LBFB RELAY PS FAIL</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB 11 LBFB RELAY FAIL</x:t>
@@ -217,28 +217,13 @@
     <x:t>SEL-2020 COM</x:t>
   </x:si>
   <x:si>
-    <x:t>coso HWE TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>coso HWE GRD TGT</x:t>
+    <x:t>COSO HWE TGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO HWE GRD TGT</x:t>
   </x:si>
   <x:si>
     <x:t>SILVERPEAK TCT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONE LINE FOR CONSTRUCTION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. RLY'S 903536612 SH.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM 115KV SH.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DIG PT LISTING RTU SYSTEM T15KV SH.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV LINE POS. RELAY 903536612 DIGITAL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -604,14 +589,14 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B80"/>
+  <x:dimension ref="A1:B75"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="92.282054" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="68.567768" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
@@ -1212,46 +1197,6 @@
       </x:c>
       <x:c r="B75" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="76" spans="1:2">
-      <x:c r="A76" s="0">
-        <x:v>585409</x:v>
-      </x:c>
-      <x:c r="B76" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="77" spans="1:2">
-      <x:c r="A77" s="0">
-        <x:v>5640064</x:v>
-      </x:c>
-      <x:c r="B77" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="78" spans="1:2">
-      <x:c r="A78" s="0">
-        <x:v>5640065</x:v>
-      </x:c>
-      <x:c r="B78" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="79" spans="1:2">
-      <x:c r="A79" s="0">
-        <x:v>5640066</x:v>
-      </x:c>
-      <x:c r="B79" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="80" spans="1:2">
-      <x:c r="A80" s="0">
-        <x:v>5640067</x:v>
-      </x:c>
-      <x:c r="B80" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Address code review feedback - add constants and improve exception handling
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -28,19 +28,16 @@
     <x:t>STINGER SWITCH 115KV</x:t>
   </x:si>
   <x:si>
-    <x:t>IINYO 115KV CB</x:t>
-  </x:si>
-  <x:si>
     <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
+    <x:t>HAIWEE-INYOKERN 115KV CB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
     <x:t>BISHOP CREEK PLANT NO. 115KV CB</x:t>
@@ -636,7 +633,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -644,7 +641,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -652,7 +649,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -660,7 +657,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -668,7 +665,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -676,7 +673,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -684,7 +681,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -692,7 +689,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -700,7 +697,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -708,7 +705,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -716,7 +713,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -724,7 +721,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -732,7 +729,7 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -740,7 +737,7 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -748,7 +745,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -756,7 +753,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -764,7 +761,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -772,7 +769,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -780,7 +777,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -788,7 +785,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -796,7 +793,7 @@
         <x:v>55</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -804,7 +801,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -812,7 +809,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -820,7 +817,7 @@
         <x:v>59</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -828,7 +825,7 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -836,7 +833,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -844,7 +841,7 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -852,7 +849,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -860,7 +857,7 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -868,7 +865,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -876,7 +873,7 @@
         <x:v>69</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -884,7 +881,7 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -892,7 +889,7 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
@@ -900,7 +897,7 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
@@ -908,7 +905,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
@@ -916,7 +913,7 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
@@ -924,7 +921,7 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
@@ -932,7 +929,7 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
@@ -940,7 +937,7 @@
         <x:v>191</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
@@ -948,7 +945,7 @@
         <x:v>192</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
@@ -956,7 +953,7 @@
         <x:v>193</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
@@ -964,7 +961,7 @@
         <x:v>194</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
@@ -972,7 +969,7 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
@@ -980,7 +977,7 @@
         <x:v>196</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:2">
@@ -988,7 +985,7 @@
         <x:v>197</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:2">
@@ -996,7 +993,7 @@
         <x:v>198</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:2">
@@ -1004,7 +1001,7 @@
         <x:v>199</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:2">
@@ -1012,7 +1009,7 @@
         <x:v>200</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:2">
@@ -1020,7 +1017,7 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:2">
@@ -1028,7 +1025,7 @@
         <x:v>202</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:2">
@@ -1036,7 +1033,7 @@
         <x:v>203</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:2">
@@ -1044,7 +1041,7 @@
         <x:v>204</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:2">
@@ -1052,7 +1049,7 @@
         <x:v>205</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:2">
@@ -1060,7 +1057,7 @@
         <x:v>206</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:2">
@@ -1068,7 +1065,7 @@
         <x:v>207</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:2">
@@ -1076,7 +1073,7 @@
         <x:v>209</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:2">
@@ -1084,7 +1081,7 @@
         <x:v>210</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:2">
@@ -1092,7 +1089,7 @@
         <x:v>211</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:2">
@@ -1100,7 +1097,7 @@
         <x:v>212</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:2">
@@ -1108,7 +1105,7 @@
         <x:v>213</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:2">
@@ -1116,7 +1113,7 @@
         <x:v>214</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:2">
@@ -1124,7 +1121,7 @@
         <x:v>220</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:2">
@@ -1132,7 +1129,7 @@
         <x:v>222</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:2">
@@ -1140,7 +1137,7 @@
         <x:v>223</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:2">
@@ -1148,7 +1145,7 @@
         <x:v>226</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:2">
@@ -1156,7 +1153,7 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:2">
@@ -1164,7 +1161,7 @@
         <x:v>228</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:2">
@@ -1172,7 +1169,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:2">
@@ -1180,7 +1177,7 @@
         <x:v>234</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:2">
@@ -1188,7 +1185,7 @@
         <x:v>236</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:2">
@@ -1196,7 +1193,7 @@
         <x:v>239</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Address code review feedback - use nullable int and regex for document references
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -38,406 +38,418 @@
     <x:t>3</x:t>
   </x:si>
   <x:si>
+    <x:t>ADDED POINT FOR 115KV LINE POS.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
     <x:t>IINYO 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
+    <x:t>5</x:t>
   </x:si>
   <x:si>
     <x:t>INYO 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>5</x:t>
+    <x:t>6</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>6</x:t>
+    <x:t>7</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>7</x:t>
+    <x:t>8</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>8</x:t>
+    <x:t>9</x:t>
   </x:si>
   <x:si>
     <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
   </x:si>
   <x:si>
-    <x:t>9</x:t>
+    <x:t>10</x:t>
   </x:si>
   <x:si>
     <x:t>OXBOW 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>10</x:t>
+    <x:t>11</x:t>
   </x:si>
   <x:si>
     <x:t>OXBOW CUST CB</x:t>
   </x:si>
   <x:si>
-    <x:t>11</x:t>
+    <x:t>12</x:t>
   </x:si>
   <x:si>
     <x:t>DIXIE VALLEY CUST CB</x:t>
   </x:si>
   <x:si>
-    <x:t>12</x:t>
+    <x:t>13</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE</x:t>
   </x:si>
   <x:si>
-    <x:t>13</x:t>
+    <x:t>14</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 4f—</x:t>
   </x:si>
   <x:si>
-    <x:t>14</x:t>
+    <x:t>15</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK 115KV CB</x:t>
   </x:si>
   <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
     <x:t>16</x:t>
   </x:si>
   <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
     <x:t>ENTRY</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
+    <x:t>18</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB LOW GAS/AIR</x:t>
   </x:si>
   <x:si>
-    <x:t>18</x:t>
+    <x:t>19</x:t>
   </x:si>
   <x:si>
     <x:t>115KV CB GEN</x:t>
   </x:si>
   <x:si>
-    <x:t>19</x:t>
+    <x:t>20</x:t>
   </x:si>
   <x:si>
     <x:t>SPARE 2a</x:t>
   </x:si>
   <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
     <x:t>22</x:t>
   </x:si>
   <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
     <x:t>SPARE x f—i—</x:t>
   </x:si>
   <x:si>
-    <x:t>23</x:t>
-  </x:si>
-  <x:si>
     <x:t>24</x:t>
   </x:si>
   <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
     <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
   </x:si>
   <x:si>
-    <x:t>25</x:t>
+    <x:t>26</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
+    <x:t>27</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK C30 FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>27</x:t>
+    <x:t>28</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 1 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
+    <x:t>29</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>29</x:t>
+    <x:t>30</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>30</x:t>
+    <x:t>31</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>31</x:t>
+    <x:t>32</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>32</x:t>
+    <x:t>33</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK 63X FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>33</x:t>
+    <x:t>34</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ POT FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
+    <x:t>35</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>35</x:t>
+    <x:t>36</x:t>
   </x:si>
   <x:si>
     <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>36</x:t>
+    <x:t>37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>37</x:t>
+    <x:t>39</x:t>
   </x:si>
   <x:si>
     <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>38</x:t>
+    <x:t>40</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
+    <x:t>41</x:t>
   </x:si>
   <x:si>
     <x:t>115KV DFR OPERATION</x:t>
   </x:si>
   <x:si>
-    <x:t>40</x:t>
+    <x:t>42</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
+    <x:t>43</x:t>
   </x:si>
   <x:si>
     <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>42</x:t>
+    <x:t>44</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
+    <x:t>45</x:t>
   </x:si>
   <x:si>
     <x:t>CASA DIABLO REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>44</x:t>
+    <x:t>46</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR CS</x:t>
   </x:si>
   <x:si>
-    <x:t>45</x:t>
+    <x:t>47</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR OV</x:t>
   </x:si>
   <x:si>
-    <x:t>46</x:t>
+    <x:t>48</x:t>
   </x:si>
   <x:si>
     <x:t>CASA D-SHERWIN REACTOR UV</x:t>
   </x:si>
   <x:si>
-    <x:t>47</x:t>
+    <x:t>49</x:t>
   </x:si>
   <x:si>
     <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>48</x:t>
+    <x:t>50</x:t>
   </x:si>
   <x:si>
     <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
   </x:si>
   <x:si>
-    <x:t>49</x:t>
+    <x:t>51</x:t>
   </x:si>
   <x:si>
     <x:t>FUPS TROUBLE</x:t>
   </x:si>
   <x:si>
-    <x:t>50</x:t>
+    <x:t>52</x:t>
   </x:si>
   <x:si>
     <x:t>115KV RELAY BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>51</x:t>
+    <x:t>53</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BACK-UP BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>52</x:t>
+    <x:t>54</x:t>
   </x:si>
   <x:si>
     <x:t>115KV OPERATING BUS AL</x:t>
   </x:si>
   <x:si>
-    <x:t>53</x:t>
+    <x:t>55</x:t>
   </x:si>
   <x:si>
     <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
   </x:si>
   <x:si>
-    <x:t>54</x:t>
+    <x:t>56</x:t>
   </x:si>
   <x:si>
     <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
   </x:si>
   <x:si>
-    <x:t>55</x:t>
+    <x:t>57</x:t>
   </x:si>
   <x:si>
     <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
   </x:si>
   <x:si>
-    <x:t>56</x:t>
+    <x:t>58</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>57</x:t>
+    <x:t>59</x:t>
   </x:si>
   <x:si>
     <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>58</x:t>
+    <x:t>60</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVID6O</x:t>
   </x:si>
   <x:si>
-    <x:t>59</x:t>
+    <x:t>61</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KVD60JA/S</x:t>
   </x:si>
   <x:si>
-    <x:t>60</x:t>
+    <x:t>62</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>61</x:t>
+    <x:t>63</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>62</x:t>
+    <x:t>64</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>63</x:t>
+    <x:t>65</x:t>
   </x:si>
   <x:si>
     <x:t>HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>64</x:t>
+    <x:t>66</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>65</x:t>
+    <x:t>67</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KVD60/A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>66</x:t>
+    <x:t>68</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
   </x:si>
   <x:si>
-    <x:t>67</x:t>
+    <x:t>69</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HATNEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>68</x:t>
+    <x:t>70</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L CHAN FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>69</x:t>
+    <x:t>71</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>70</x:t>
+    <x:t>72</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
   </x:si>
   <x:si>
-    <x:t>71</x:t>
+    <x:t>73</x:t>
   </x:si>
   <x:si>
     <x:t>HATWEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
   </x:si>
   <x:si>
-    <x:t>72</x:t>
+    <x:t>74</x:t>
   </x:si>
   <x:si>
     <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
@@ -863,7 +875,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B73"/>
+  <x:dimension ref="A1:B75"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -994,15 +1006,15 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1034,23 +1046,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1058,15 +1070,15 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1451,6 +1463,22 @@
       </x:c>
       <x:c r="B73" s="0" t="s">
         <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>145</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1486,7 +1514,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1494,7 +1522,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1502,7 +1530,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1510,7 +1538,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1518,7 +1546,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1526,7 +1554,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1534,7 +1562,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1542,7 +1570,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1550,7 +1578,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1558,7 +1586,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1566,7 +1594,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1574,7 +1602,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1582,7 +1610,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1590,7 +1618,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1598,15 +1626,15 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1614,7 +1642,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1622,7 +1650,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1630,7 +1658,7 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1638,23 +1666,23 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1662,15 +1690,15 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1678,7 +1706,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1686,7 +1714,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1694,7 +1722,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -1702,7 +1730,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -1710,7 +1738,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -1718,7 +1746,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -1726,7 +1754,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -1734,7 +1762,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -1742,7 +1770,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1750,7 +1778,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -1758,7 +1786,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -1766,7 +1794,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
@@ -1774,7 +1802,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
@@ -1782,7 +1810,7 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
@@ -1790,7 +1818,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
@@ -1798,7 +1826,7 @@
         <x:v>76</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement OCR+Geometry parser with header detection and row extraction
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -26,445 +26,763 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
-    <x:t>RTU MONITOR JUMPER CONTROL NHIBIT</x:t>
+    <x:t>DSCRPT }0 DSCRIPT] RELAY NO. RELAY NO. “NOTE 3)) wc. DSCRPT }0 DSCRIPT] RELAY NO. RELAY NO. NOTE 3)) owe.</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>STINGER SWITCH 115KV</x:t>
+    <x:t>| RTU MONITOR (JUMPER) CONTROL INHIBIT NORMAL | ALARM — — [or t-t — = = = 81__| {GATE ~\ 1C7 96-24T/C | DI 5-80 [RM 5-35/36 W58</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>FUPS TROUBLE</x:t>
+    <x:t>|FUPS TROUBLE F 1c8 DI 6-81 — W59</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>IINYO 115KV CB</x:t>
+    <x:t>[UI15KV CONTROL BUS AL) 95-1 DI 6-82 = W60</x:t>
   </x:si>
   <x:si>
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>INYO 115KV CB</x:t>
+    <x:t>| 115KV RELAY BUS AL 95-2 DI 6-83 = W61</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV RELAY BUS AL</x:t>
+    <x:t>| 115KV BACK-UP BUS AL 95-3 DI 6-84 = W62</x:t>
   </x:si>
   <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV BACK-UP BUS AL</x:t>
+    <x:t>| 115KV OPERATING BUS AL 95-4 DI 6-85 = W63</x:t>
   </x:si>
   <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA DIABLO-SHERWIN 115KV CB</x:t>
+    <x:t>| HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-7/AT RK — [or t-7__ [RM 2-9/10 1B, 2A | = 87_| 115KV ELECTRONIC BUS AL 95-5 = DI 6-86 = W64</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV OPERATING BUS AL</x:t>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-9/AT RK — [or i-8 [RM 2-11712 1B, | = 88__| 115KV DUPLICATE ELECTRONIC BUS 95-6 = DI 6-87 = W65</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV CB</x:t>
+    <x:t>|(BISHOP CREEK PLANT NO. &amp; 115KV CB CLOSE | OPEN | 95-15/AT RK Z — fori-9 [RM 2-13/14 1B, 2A = 89_| 115KV _LBFB BUS 95-7 = DI 6-88 — W66</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV CB</x:t>
+    <x:t>__| 115KV INTERFACE BUS 95-8 = DI 6-89 = W67</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>BISHOP CREEK PLANT NO. 3 &amp;</x:t>
+    <x:t>__|E115KVFMETER BUS F 95-9 = DI 6-90 = W68</x:t>
   </x:si>
   <x:si>
     <x:t>12</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW 115KV CB</x:t>
+    <x:t>[WWIXIE VALLEY CUST CBF Tn CLOSE | OPEN | 95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A = 92_| SPARE = DI 6-91 = = W69</x:t>
   </x:si>
   <x:si>
     <x:t>13</x:t>
   </x:si>
   <x:si>
-    <x:t>OXBOW CUST CB</x:t>
+    <x:t>[| BUS TIE 115KV CB CLOSE | OPEN | 95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B, | = 93__| SPARE = DI 6-92 = = W70</x:t>
   </x:si>
   <x:si>
     <x:t>14</x:t>
   </x:si>
   <x:si>
-    <x:t>DIXIE VALLEY CUST CB</x:t>
+    <x:t>_|(115KV W/BUS POT ALE = DI 6-93 = Ww</x:t>
   </x:si>
   <x:si>
     <x:t>15</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 1 BANK 115KV CB</x:t>
+    <x:t>_|LI5KV_E/BUS POT ALJ = DI 6-94 = W712</x:t>
   </x:si>
   <x:si>
     <x:t>16</x:t>
   </x:si>
   <x:si>
-    <x:t>BATT CHG FAIL FAIL LOSS OF AC</x:t>
+    <x:t>_| LOW DC VOLTAGE 1c-9 = DI 6-95 = W713</x:t>
   </x:si>
   <x:si>
     <x:t>17</x:t>
   </x:si>
   <x:si>
-    <x:t>ENTRY</x:t>
+    <x:t>| BATT CHG FAIL FAIL LOSS OF AC 1C-10 _— DI 6-96 _— w74</x:t>
   </x:si>
   <x:si>
     <x:t>18</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV CB LOW GAS/AIR</x:t>
+    <x:t>__| POSITIVE DC GRD 1c-11 = DI 7-97 = W75</x:t>
   </x:si>
   <x:si>
     <x:t>19</x:t>
   </x:si>
   <x:si>
-    <x:t>SEL-2030 FAIL -—~—~~~~—~\—«C98 1C-13</x:t>
+    <x:t>_| NEGATIVE DC GRD 1C-12 = DI 7-98 = W76</x:t>
   </x:si>
   <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV CB GEN</x:t>
+    <x:t>|(SEL-2030 FAIL -—~—~~~~—~\({—«C98 1C-13 = DI 7-99 = WT?</x:t>
   </x:si>
   <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK TAP RAISE/LOWER</x:t>
+    <x:t>INO. BANK LTC AUTO/MAN I| = — DI 7-100 |RM 5-37/38 Ww78</x:t>
   </x:si>
   <x:si>
     <x:t>22</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV BUS TIE POS. 1X SEL-311C TRIP</x:t>
+    <x:t>INO. BANK LTC AUTO/MAN || = = DI 7-101 [RM 5-39/40 w79</x:t>
   </x:si>
   <x:si>
     <x:t>23</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV BUS TIE POS. 1X SEL-31IC RLY FAIL</x:t>
+    <x:t>INO. BANK TAP RATSE/LOWER I] = = DI 7-102 [RM 6-41/42 W80</x:t>
   </x:si>
   <x:si>
     <x:t>24</x:t>
   </x:si>
   <x:si>
-    <x:t>TRANS BK SUDDENTPRESS RESET “1 -</x:t>
+    <x:t>|INO. BANK TAP RAISE/LOWER I| — = DI 7-103 [RM 6-43/44 W81</x:t>
   </x:si>
   <x:si>
     <x:t>25</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 1 BANK SEL-351 0C TRIP</x:t>
+    <x:t>_|ISPARE I] = = DI 7-104 [RM 6-45/46 — W82</x:t>
   </x:si>
   <x:si>
     <x:t>26</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 1 BANK C30 FAIL</x:t>
+    <x:t>||SPARE JI = — DI 7-105 _ W83</x:t>
   </x:si>
   <x:si>
     <x:t>27</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 1 BANK 63X FAIL</x:t>
+    <x:t>| 115KV BUS TIE POS. 1X SEL-311C TRIP | ALARM | NORMAL — DI 7-106 = 6B Ww84</x:t>
   </x:si>
   <x:si>
     <x:t>28</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF FAIL</x:t>
+    <x:t>| 115KV BUS TIE POS. 1X SEL-31IC RLY FAIL| NORMAL | ALARM 1C15 = DI 7-107 = 6B W85</x:t>
   </x:si>
   <x:si>
     <x:t>29</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-387 DIFF TRIP</x:t>
+    <x:t>[115KV BUS TIE POS. 1X SEL-311C A/S [| AuTO | SOLID | 8-1/AT RK Z51 = DI 7-108 = =</x:t>
   </x:si>
   <x:si>
     <x:t>30</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC FAIL</x:t>
+    <x:t>[f- F[ 1C16 = DI 7-109 = W86</x:t>
   </x:si>
   <x:si>
     <x:t>31</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK SEL-351 OC TRIP</x:t>
+    <x:t>| SPARE | — | — = = 1A13 — [or 2-31 — = = Wi mt | I| = = DI 7-110 [RM 7-49/50 W87</x:t>
   </x:si>
   <x:si>
     <x:t>32</x:t>
   </x:si>
   <x:si>
-    <x:t>NO. 3 BANK 63X FAIL</x:t>
+    <x:t>| I| ici? = DI ?-111 — W88</x:t>
   </x:si>
   <x:si>
     <x:t>33</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ POT FAIL</x:t>
+    <x:t>| ant 1c18 — DI 7-112 = W89</x:t>
   </x:si>
   <x:si>
     <x:t>34</x:t>
   </x:si>
   <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS A RLY FAIL</x:t>
+    <x:t>|| RESERVED FOR 115KV LINE Pos. 2x ll 1c19 = DI 8-113 = w90</x:t>
   </x:si>
   <x:si>
     <x:t>35</x:t>
   </x:si>
   <x:si>
-    <x:t>EAST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+    <x:t>{|_| PROTECTION RELAYS ALARMS | DI 8-114 = w91</x:t>
   </x:si>
   <x:si>
     <x:t>36</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY FAIL</x:t>
+    <x:t>| I] = DI 8-115 [RM 7-51/52 w92</x:t>
   </x:si>
   <x:si>
     <x:t>37</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS A RLY TRIP</x:t>
+    <x:t>| I] = DI 8-116 = =</x:t>
   </x:si>
   <x:si>
     <x:t>38</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KVID6O</x:t>
+    <x:t>| I] DI 8-117 = W93</x:t>
   </x:si>
   <x:si>
     <x:t>39</x:t>
   </x:si>
   <x:si>
-    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP</x:t>
+    <x:t>| | DI 8-118 = wo4</x:t>
   </x:si>
   <x:si>
     <x:t>40</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KVD60JA/S</x:t>
+    <x:t>| I] 1¢23 DI 8-119 = w95</x:t>
   </x:si>
   <x:si>
     <x:t>41</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV DFR FAIL</x:t>
+    <x:t>|F I] DI 8-120 = w96</x:t>
   </x:si>
   <x:si>
     <x:t>42</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
+    <x:t>| I| = DI 8-121 = WoT</x:t>
   </x:si>
   <x:si>
     <x:t>43</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV DFR OPERATION</x:t>
+    <x:t>| I — DI 8-122 [RM 7-53/54 =</x:t>
   </x:si>
   <x:si>
     <x:t>44</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
+    <x:t>|| L RESERVED FOR 115KV LINE Pos. 1__l| 1D-1 DI 8-123 = w98</x:t>
   </x:si>
   <x:si>
     <x:t>45</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ RELAY PICK UP</x:t>
+    <x:t>|| [ PROTECTION RELAYS ALARMS I 1D-2 DI 8-124 — w99</x:t>
   </x:si>
   <x:si>
     <x:t>46</x:t>
   </x:si>
   <x:si>
-    <x:t>115KV UNDERFREQ RELAY FAIL</x:t>
+    <x:t>| I] 10-3 DI 8-125 = W100</x:t>
   </x:si>
   <x:si>
     <x:t>47</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
+    <x:t>| I] 10-4 DI 8-126 _— W101</x:t>
   </x:si>
   <x:si>
     <x:t>48</x:t>
   </x:si>
   <x:si>
-    <x:t>HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
+    <x:t>|| I| = DI 8-127 = W102 NOTES:</x:t>
   </x:si>
   <x:si>
     <x:t>49</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA DIABLO REACTOR OV</x:t>
+    <x:t>| | = DI 8-128 [RM 7-55/56 =</x:t>
   </x:si>
   <x:si>
     <x:t>50</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA DIABLO REACTOR UV</x:t>
+    <x:t>| F[_ 10-5 DI 9-129 = W103 ane SINE RO SSE TRIPPING RECS.</x:t>
   </x:si>
   <x:si>
     <x:t>51</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KVD60RLY FAIL</x:t>
+    <x:t>| I| 10-6 DI 9-130 — W104 AN INDICATION IS TAKEN FROM EACH</x:t>
   </x:si>
   <x:si>
     <x:t>52</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA D-SHERWIN REACTOR CS</x:t>
+    <x:t>| I] 10-7 DI 9-131 — W105 RUA</x:t>
   </x:si>
   <x:si>
     <x:t>53</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KVD60/A/S</x:t>
+    <x:t>| I] 10-8 DI 9-132 = W106</x:t>
   </x:si>
   <x:si>
     <x:t>54</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA D-SHERWIN REACTOR OV</x:t>
+    <x:t>|| I = DI 9-133 — W107 OY</x:t>
   </x:si>
   <x:si>
     <x:t>55</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L TRIP</x:t>
+    <x:t>| 115KV_UNDERFREQ POT FAIL NORMAL | ALARM | 74/AT RK Z58 —_ DI 4-55 a W35 136_||_l RESERVED FOR 115KV LINE POS. 2_|| 1D-9 DI 9-135 _ W108 TS INTERCHANGED BETWEEN THE PLC</x:t>
   </x:si>
   <x:si>
     <x:t>56</x:t>
   </x:si>
   <x:si>
-    <x:t>CASA D-SHERWIN REACTOR UV</x:t>
+    <x:t>[NORMAL ALARM 1B14 —___| or 4-56 = 6A W36 137_|F i135 10-10 DI 9-136 | — W109 Ma a PROTOS Lee CALLY</x:t>
   </x:si>
   <x:si>
     <x:t>57</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HATNEE-IINYOKERN 115KV SEL-311L RLY FAIL</x:t>
+    <x:t>|| I! 10-11 DI 9-137 — WH10 MEANS</x:t>
   </x:si>
   <x:si>
     <x:t>58</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L CHAN FAIL</x:t>
+    <x:t>| I| 10-12 DI 9-138 = Witt</x:t>
   </x:si>
   <x:si>
     <x:t>59</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DIFF A/S</x:t>
+    <x:t>| || = DI 9-139 = Wi12</x:t>
   </x:si>
   <x:si>
     <x:t>60</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAIWEE-IINYOKERN 115KV SEL-311L A/S</x:t>
+    <x:t>{I [139 _ DI 9-140 [RM 8-59/60 = FOR CASE NUMBER REFER TO DWG.</x:t>
   </x:si>
   <x:si>
     <x:t>61</x:t>
   </x:si>
   <x:si>
-    <x:t>CD SHUNT REACTOR TROUBLE AL</x:t>
+    <x:t>[J _J| DI 9-141 = Wi13</x:t>
   </x:si>
   <x:si>
     <x:t>62</x:t>
   </x:si>
   <x:si>
-    <x:t>HATWEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
+    <x:t>F743 | HAIWEE-INYOKERN 115KV1D60] TRIP ALARM | NORMAL DI 9-142 = 6B | (5804239 wit4</x:t>
   </x:si>
   <x:si>
     <x:t>63</x:t>
   </x:si>
   <x:si>
-    <x:t>CD-S SHUNT REACTOR TROUBLE AL</x:t>
+    <x:t>| HAIWEE-INYOKERN 115KVID6O|RLY FAIL | NORMAL | ALARM 1D15 DI 9-143 = 6B | | | wits</x:t>
   </x:si>
   <x:si>
     <x:t>64</x:t>
   </x:si>
   <x:si>
-    <x:t>COSO-HAINEE-IINYOKERN 115KV SEL-311L DTT RECD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SILVERPEAK A C TCT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>i RESERVED FOR 115KV LINE Pos.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F L RESERVED FOR 115KV LINE POs.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB ARMED</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV LBFB TRIP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15KV CB 1 LBFB RELAY PS % FAIL \</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115KV CB 11" LBFB RELAY PS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>l115KV cB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>115K CB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEL-2020 COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE A TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE B TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lcoso HWE GRD TGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SILVERPEAK C C TCT</x:t>
+    <x:t>HAIWEE-INYOKERN 115KV[D60JA/S auTo SOLID 8-2/AT RK DI 9-144 _ =|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HAIWEE-INYOKERN 115KV SEL-311L TRIP | ALARM | NORMAL 1D16 DI 10-145] — 6B WIIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL[ NORMAL | ALARM 1D17 DI 10-146 6B WHI?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-148] — —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HAIWEE-INYOKERN 115KV SEL-311L A/S | AUTO | SOLID | 8-1/AT RK DI_10-149|RM 8-63/64 2B, | = *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“Ts 7| COSO-HAIWEE-INYOKERN T15KV{D60) TRIP | ALARM | NORMAL 1D19 DI 10-150 = 6B | (5804244) | wii9 &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV(D60[RLY FAIL NORMAL | ALARM DI 10-151 = 6B | | 5804244| | W120 é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COSO-HAIWEE-INYOKERN 115KV[D60/A/S AUTO SOLID 6-2/AT RK DI 10-152| 2B, |se042aap —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP| ALARM | NORMAL DI 10-153] — 6B wi2t Q</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL | NORMAL | ALARM DI 10-154] — 6B W122 a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL | NORMAL | ALARM DI 10-155, — 6A W123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-156] — =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S| AuTO | SOLID | 8-1/AT RK DI_10-157|RM 9-67/68 2B, | =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HATWEE-INYOKERN 115KV SEL-311L DTT RECD | ALARM | NORMAL DI 10-158] — 6B wi24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD| ALARM | NORMAL 1E1 DI 10-159] — 6B W128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| ADDED POINT FOR 115KV LINE POS. RELAY | 03-05-24 | | VM VM ve | S&amp;L | S&amp;L | VM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV LINE POS. RELAY DIGITAL POINT LISTING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[DIG PT LISTING RTU SYSTEM T15KV SH. | ROOED,POINTS FOR | 06-24-22 | | VM vM ve | sa | sac | vM RTU aa he</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. RLY'S SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>83</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ONE LINE FOR CONSTRUCTION | REPL'D RLY SEL-311C WITH D60 FOR 115KV LINE POS. | 07-31-25 | | VM vM SSF | | S&amp;L | vM [| | ISSUED FOR CONSTRUCTION 08-31-20 | | VM vB ve | sat | set | vw SOUTHERN CALIFORNIA SCALE+___NONE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DscRPT DSCRIPT] RELAY NO. RELAY NO. (NOTE 3)] we. | DscRPT DSCRIPT| RELAY NO. RELAY NO. (NOTE 3)} pwc.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(SILVERPEAK A A ToT ' \ = -</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ISILVERPEAK A B TCT | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ISILVERPEAK A C TCT E = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FSTLVERPEAK A GRD ToT Ji 904562788) — rT _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(HAIWEE-INYOKERN 115KV D60 OPD A/S || NORMAL | ALARM | 16-15 DI 15-228 { 6A "| ) wig92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||HAIWEE-INYOKERN 115KV D60 OPD ALARM|| x NORMAL | ALARM | 16-16 DI 15-229 | 6A || W193</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|[HAIWEE-INYOKERN 115KV D60 OPD TRIP_]| li NORMAL | ALARM J 16-17 DI 15-230 6A }| W194</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(COSO-HAIWEE-INYOKERN 115KV D60 OPD A/S || [ NORMAL | ALARM | 16-18 DI 15-231 f 6A | )| wig95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| COSO-HAIWEE-INYOKERN 115KV D60 OPD ALARM || x NORMAL | ALARM | 16-19 DI 15-232 | 6A || W196</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[\COSO-HAIWEESINYOKERN 115KV OPO TRIP _)| Lt NORMAL | ALARM J 16-20 DI 15-233 \_6A_, |_ J] W197</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= DI 11-170|RM 9-69/70 = 251_| SPARE L Lt 16-21 DI 15-234 LT gn4562794 | W198</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE 16-22 DI 15-235 W199</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1E10 DI 11-172 W139 253_| SPARE 16-23 DI 15-236 W200</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE 16-24 DI 15-237 W201</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| PMU TROUBLE ALARM = DI 15-238 W202</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE DI 15-239 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE DI 15-240 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-241 W203</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE _— DI 16-242 W204</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-243 W205</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE = DI 16-244 W206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE = DI 16-245 W207</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-246 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE — DI 16-247|RM 10-77/78 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE = DI 16-248]RM 10-79/80 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-249]RM 11-81/82 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-250|/RM 11-83/84 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE = DI 16-251|RM 11-85/86 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-252]RM 11-87/88 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = DI 16-253|RM 12-89/90 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE _ DI 16-254]RM 12-91/92 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV LBFB TRIP 1F2 DI 12-191 NOTE W155 272_| SPARE = DI 16-255|/RM 12-93/94 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE on = DI 16-256]/RM 12-95/96 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F4 DI 13-193 WI57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[f115KV CB LBFB RELAY PS % FAIL F | 1F5 DI 13-194 W158</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV CB LBFB RELAY FAIL }|_194 1F6 DI 13-195 W159</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F7 DI 13-196 W160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F8 DI 13-197 W161</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F9 DI 13-198 wi62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F10 DI 13-199 W163</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL Tal DI 13-200 W164</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F12 DI 13-201 W165</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS 1% FAIL 1F13 DI 13-202 W166</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F14 DI 13-203 W167</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(TS5KV CB 11" LBFB RELAY PS FAIL \| 1F15 DI 13-204 W168</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F16 DI 13-205 W169</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F17 DI 13-206 W170</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ff115KV CB LBFB RELAY FAIL FI 1F18 DI 13-207 WIT7I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY PS FAIL || 1F19 DI 13-208 Wi72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F20 DI 14-209 WI73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F21 DI 14-210 wi74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV CB LBFB RELAY FAIL J | 1F22 DI 14-211 W175</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS % FAIL 2u1 1F23 DI 14-212 W176</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F24 DI 14-213 WI77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE DI 14-214 W178</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE DI 14-215 Wi79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|f115Kv cB TCM | 2t5 DI 14-216 W180</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM DI 14-217 wie!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{l115KV cB TCM DI 14-218 W182 ONE SINGLE RTU CONTROL OUTPUT RESETS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[[115KV CB TCM [| DI 14-219 W183</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F15KV CB TCM |_| DI 14-220 W184 INDIVIDUAL SUDDEN PRESSURE TRIPPING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV cB TCM F DI 14-222 W186 a) "Vv" IN A BLOCK INDICATES A VIRTUAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I115KV CB TCM |__| DI 14-223 W187 POINT. A VIRTUAL POINT DOES NOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[115K CB TCM |_| GH DI 14-204 W188 Mo eO ROR ONCER BoT WEN att pee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{l115KV CB TCM |_| DI 15-225 W189 AND THE RTU ELECTRONICALLY VIA THE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM | DI 15-226</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A TGT — —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_ FOR CASE NUMBER REFER TO DWG. *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_fHWE-INYOKERN C TGT |__| = _ &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= = Ey BEB RN LAVS,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE A TGT | | = = a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE B TGT |_| = _ @</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|lcoso_HWE C_TGT | | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE GRD TGT | | = = é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|ISILVERPEAK C A TCT F | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ISILVERPEAK C C TCT | | = _ °</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||SILVERPEAK C GRD TcT ps (| = _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|DIG PT LISTING RTU SYSTEM 115KV SH. | ADDED OPD ALARMS FOR D60 115KV LINE POS. | 07-31-25 | | VM vM SSF | S&amp;L | S&amp;L | VM RTU aa a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ED RTU SYSTEM 115-55KV ——] ADDED OPD ALARMS FOR D60 115KV LINE POS. |————| SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ONE LINE FOR CONSTRUCTION | ISSUED FOR CONSTRUCTION 08-31-20 | | VM VB ve | sa | S&amp;L | VM SOUTHERN CALIFORNIA SCALE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>- SIZE wh</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -830,7 +1148,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B66"/>
+  <x:dimension ref="A1:B85"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1362,6 +1680,158 @@
       </x:c>
       <x:c r="B66" s="0" t="s">
         <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:2">
+      <x:c r="A76" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:2">
+      <x:c r="A77" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:2">
+      <x:c r="A78" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:2">
+      <x:c r="A79" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:2">
+      <x:c r="A80" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:2">
+      <x:c r="A81" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:2">
+      <x:c r="A82" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:2">
+      <x:c r="A83" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:2">
+      <x:c r="A84" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:2">
+      <x:c r="A85" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>169</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1378,7 +1848,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B37"/>
+  <x:dimension ref="A1:B86"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1397,7 +1867,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1405,7 +1875,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1413,7 +1883,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1421,7 +1891,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1429,7 +1899,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>174</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1437,7 +1907,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1445,7 +1915,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1453,7 +1923,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1461,7 +1931,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1469,7 +1939,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1477,7 +1947,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1485,7 +1955,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1493,7 +1963,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1501,7 +1971,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1509,7 +1979,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1517,7 +1987,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1525,7 +1995,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1533,7 +2003,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1541,7 +2011,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1549,7 +2019,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1557,7 +2027,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1565,7 +2035,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1573,7 +2043,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -1581,7 +2051,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1589,7 +2059,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1597,7 +2067,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>195</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1605,7 +2075,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>196</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -1613,7 +2083,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -1621,7 +2091,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -1629,7 +2099,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>199</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -1637,7 +2107,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -1645,7 +2115,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -1653,7 +2123,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>202</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1661,7 +2131,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -1669,7 +2139,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -1677,7 +2147,399 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:2">
+      <x:c r="A38" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:2">
+      <x:c r="A39" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:2">
+      <x:c r="A40" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:2">
+      <x:c r="A41" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:2">
+      <x:c r="A42" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:2">
+      <x:c r="A43" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:2">
+      <x:c r="A44" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:2">
+      <x:c r="A45" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:2">
+      <x:c r="A46" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:2">
+      <x:c r="A47" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:2">
+      <x:c r="A48" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:2">
+      <x:c r="A49" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:2">
+      <x:c r="A50" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:2">
+      <x:c r="A51" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:2">
+      <x:c r="A52" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:2">
+      <x:c r="A53" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:2">
+      <x:c r="A54" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:2">
+      <x:c r="A55" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:2">
+      <x:c r="A56" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:2">
+      <x:c r="A57" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:2">
+      <x:c r="A58" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:2">
+      <x:c r="A59" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:2">
+      <x:c r="A60" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:2">
+      <x:c r="A61" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:2">
+      <x:c r="A62" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:2">
+      <x:c r="A63" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:2">
+      <x:c r="A64" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:2">
+      <x:c r="A65" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:2">
+      <x:c r="A66" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:2">
+      <x:c r="A68" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:2">
+      <x:c r="A69" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:2">
+      <x:c r="A70" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:2">
+      <x:c r="A71" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:2">
+      <x:c r="A72" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:2">
+      <x:c r="A73" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:2">
+      <x:c r="A74" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:2">
+      <x:c r="A75" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:2">
+      <x:c r="A76" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:2">
+      <x:c r="A77" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>245</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:2">
+      <x:c r="A78" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:2">
+      <x:c r="A79" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:2">
+      <x:c r="A80" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>248</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:2">
+      <x:c r="A81" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:2">
+      <x:c r="A82" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:2">
+      <x:c r="A83" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:2">
+      <x:c r="A84" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:2">
+      <x:c r="A85" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:2">
+      <x:c r="A86" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>255</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Fix table end Y detection for side-by-side tables
Co-authored-by: bartonrd <57229074+bartonrd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
+++ b/ExamplePointlists/Example1/TestOutput/Control_rtu837_DNP_pointlist_rev00.xlsx
@@ -38,498 +38,963 @@
     <x:t>2</x:t>
   </x:si>
   <x:si>
+    <x:t>| STINGER SWITCH 115KV auto | SOLID = — [or 1-2 = = |FUPS TROUBLE F 1c8 DI 6-81 — W59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[ftnyo 115KV CB F———-~| CLOSE | OPEN | 95-I/AT RK Z — [or 1-3 [RM 1-172 1B, 2A _ [UI15KV CONTROL BUS AL) 95-1 DI 6-82 = W60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|[INYO 115KV CB [3 CLOSE | OPEN | 95-2/AT RK Z — [or 1-4 [Rm 1-374 1B, 2A _ | 115KV RELAY BUS AL 95-2 DI 6-83 = W61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_||CASA DIABLO 115KV CB | CLOSE OPEN | 95-3/AT RK Z _— DI 1-5 [RM 1-5/6 1B, 2A — | 115KV BACK-UP BUS AL 95-3 DI 6-84 = W62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[CASA DIABLO-SHERWIN 115KV CB | CLOSE | OPEN | 95-5/AT RK Z — [or 1-6 [RM 1-7/8 1B, 2A _ | 115KV OPERATING BUS AL 95-4 DI 6-85 = W63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-7/AT RK — [or t-7__ [RM 2-9/10 1B, 2A | = 87_| 115KV ELECTRONIC BUS AL 95-5 = DI 6-86 = W64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| COSO-HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-9/AT RK — [or i-8 [RM 2-11712 1B, | = 88__| 115KV DUPLICATE ELECTRONIC BUS 95-6 = DI 6-87 = W65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(BISHOP CREEK PLANT NO. &amp; 115KV CB CLOSE | OPEN | 95-15/AT RK Z — fori-9 [RM 2-13/14 1B, 2A = 89_| 115KV _LBFB BUS 95-7 = DI 6-88 — W66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[lOXBOW 115KV CB lg CLOSE | OPEN | 95-I7/AT RK Z — [or 1-10 [RM 2-15/16 1B, 2A = __| 115KV INTERFACE BUS 95-8 = DI 6-89 = W67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|/OXBOW CUST CB I} CLOSE OPEN | 95- X/AT RK Z = DI 1-11 [RM 3-17/18 1B, 2A = __|E115KVFMETER BUS F 95-9 = DI 6-90 = W68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[WWIXIE VALLEY CUST CBF Tn CLOSE | OPEN | 95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A = 92_| SPARE = DI 6-91 = = W69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[| BUS TIE 115KV CB CLOSE | OPEN | 95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B, | = 93__| SPARE = DI 6-92 = = W70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE [— | — = = = — [or 1-14 [RM 3-23/24 = = = _|(115KV W/BUS POT ALE = DI 6-93 = Ww</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE 4f{[—|[— = = = — [or 1-15 [RM 4-25/26 = = = _|LI5KV_E/BUS POT ALJ = DI 6-94 = W712</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[fNO. BANK T15KV CB 11) CLOSE | OPEN | 95-1I/AT RK Z — [or 1-16 [RM 4-27/28 1B, 2A = _| LOW DC VOLTAGE 1c-9 = DI 6-95 = W713</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{INO. BANK 115KV CB F CLOSE OPEN | 95-13/AT RK Z _— DI 2-17 |RM 4-29/30 1B, 2A _ | BATT CHG FAIL FAIL LOSS OF AC 1C-10 _— DI 6-96 _— w74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE = = = = — [ot 2-18 [RM 4-31/32 = = = __| POSITIVE DC GRD 1c-11 = DI 7-97 = W75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| ENTRY ALARM NORMAL | ALARM TAI — [or 2-19 = = _| NEGATIVE DC GRD 1C-12 = DI 7-98 = W76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|fi1S5KV CB LOW GAS7AIR NORMAL | ALARM TA2 — [pI 2-20 = 6C W1 |(SEL-2030 FAIL -—~—~~~~—~\({—«C98 1C-13 = DI 7-99 = WT?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(115KV_CB GEN ALARM F NORMAL | ALARM 1A3 — [or 2-21 = 6C Ww2 INO. BANK LTC AUTO/MAN I| = — DI 7-100 |RM 5-37/38 Ww78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE = = = 1A4 — __|b1 2-22 = = = = INO. BANK LTC AUTO/MAN || = = DI 7-101 [RM 5-39/40 w79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANKTHIGH TEMP AL = | ALARM | NORMAL 1A5 — [or 2-23 — 6B W3 INO. BANK TAP RATSE/LOWER I] = = DI 7-102 [RM 6-41/42 W80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|INO. BANK GEN AL | o | ALARM | NORMAL 1A6 — [pr 2-24 = 6B W4 |INO. BANK TAP RAISE/LOWER I| — = DI 7-103 [RM 6-43/44 W81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|INO. BANK ITM FAIL | o | ALARM | NORMAL TAT — [or 2-25 — 6B W5 _|ISPARE I] = = DI 7-104 [RM 6-45/46 — W82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_||NO. BANK HYDROGEN | o | ALARM | NORMAL 1A8 — [or 2-26 — 6B W6 ||SPARE JI = — DI 7-105 _ W83</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FINO. BANK WATER F | ALARM | NORMAL 1A9 — [ol 2-27 — 6B WT | 115KV BUS TIE POS. 1X SEL-311C TRIP | ALARM | NORMAL — DI 7-106 = 6B Ww84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|INO. BANK HI GAS ALARM | | ALARM | NORMAL TAI0 — [oI 2-28 = 6B W8 | 115KV BUS TIE POS. 1X SEL-31IC RLY FAIL| NORMAL | ALARM 1C15 = DI 7-107 = 6B W85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|INO. BANK HIGH TEMP AL J | ALARM | NORMAL TAIT — [or 2-29 — 6B W9 [115KV BUS TIE POS. 1X SEL-311C A/S [| AuTO | SOLID | 8-1/AT RK Z51 = DI 7-108 = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE 2a | — | — = = 1A12 — [oI 2-30 — = = w10 [f- F[ 1C16 = DI 7-109 = W86</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE | — | — = = 1A13 — [or 2-31 — = = Wi mt | I| = = DI 7-110 [RM 7-49/50 W87</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| I| ici? = DI ?-111 — W88</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| —|— = = 1A15 — [or 3-33 — = = W13 | ant 1c18 — DI 7-112 = W89</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE ]—i/— = = 1A16 — | or 3-34 = = = wi4 || RESERVED FOR 115KV LINE Pos. 2x ll 1c19 = DI 8-113 = w90</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|(NO. BANK HIGH TEMP AL | | ALARM | NORMAL 1A17 — DI 3-35 = 6B W15 {|_| PROTECTION RELAYS ALARMS | DI 8-114 = w91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FINO. BANK GEN AL F | ALARM | NORMAL 1A18 — [or 3-36 = 6B Wi6 | I] = DI 8-115 [RM 7-51/52 w92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANKFITM FAI ) [ ALARM | NORMAL TAS — [or 3-37 — 6B WI7 | I] = DI 8-116 = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE x f[—i[— = = 1A20 — | oI 3-38 = - = Wi8 | I] DI 8-117 = W93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE | — | — = = 1A21 — [or 3-39 = = — wig | | DI 8-118 = wo4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>__| SPARE | —| — = = — | oI 3-40 = - = w20 | I] 1¢23 DI 8-119 = w95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|FTRANS BK SUDDENTPRESS RESET “1 - = = — [RM 5-33/34 = |F I] DI 8-120 = w96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANK SEL-387 DIFF FAIL || NORMAL | ALARM 1A23 — |or 3-41 — 6B W21 | I| = DI 8-121 = WoT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANK SEL-387 DIFF TRIP Ifa NORMAL | ALARM 1A24 — [pr 3-42 = 6B W22 | I — DI 8-122 [RM 7-53/54 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANK SEL-351 OC FAIL | NORMAL | ALARM 1B1 — [or 3-43 = 6B W23 || L RESERVED FOR 115KV LINE Pos. 1__l| 1D-1 DI 8-123 = w98</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|INO. BANK SEL-351 0C TRIP || NORMAL | ALARM 1B2 _— DI 3-44 _ 6B W24 || [ PROTECTION RELAYS ALARMS I 1D-2 DI 8-124 — w99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|FNO. BANK C30 FAIL || NORMAL | ALARM 1B3 — [or 3-45 — 6B W25 | I] 10-3 DI 8-125 = W100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BANK C30 TRIP F | NORMAL | ALARM 1B4 — [ol 3-46 = 6B W26 | I] 10-4 DI 8-126 _— W101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| NO. BANK 63X FAIL || NORMAL | ALARM 1B5 — [or 3-47 — 6B W27 || I| = DI 8-127 = W102 NOTES:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| NO. BANK SEL-387 DIFF FAIL I | NORMAL | ALARM 1B6 — [or 3-48 — 6B W28 | | = DI 8-128 [RM 7-55/56 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| NO. BANK SEL-387 DIFF TRIP | NORMAL | ALARM — [or 4-49 — 6B W29 | F[_ 10-5 DI 9-129 = W103 ane SINE RO SSE TRIPPING RECS.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| NO. BANK SEL-351 OC FAIL | | NORMAL | ALARM 1B8 — [dI 4-50 = 6B W30 | I| 10-6 DI 9-130 — W104 AN INDICATION IS TAKEN FROM EACH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|INO. BANK SEL-351 OC TRIP NORMAL ALARM — [or 4-51 = 6B W31 | I] 10-7 DI 9-131 — W105 RUA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO. BANK C30 FAIL I] NORMAL | ALARM 1B10 — [ol 4-52 = 6B W32 | I] 10-8 DI 9-132 = W106</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||NO. BANK C30 TRIP F | NORMAL | ALARM 1B11 — DI 4-53 = 6B W33 || I = DI 9-133 — W107 OY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|INO. BANK 63X FAIL J) | NORMAL ALARM 1B12 — DI 4-54 _— 6B W34 || I] _ DI 9-134 |RM 8-57/58 —_ USED A HARD WIRE CONNECTION. DATA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV_UNDERFREQ POT FAIL NORMAL | ALARM | 74/AT RK Z58 —_ DI 4-55 a W35 136_||_l RESERVED FOR 115KV LINE POS. 2_|| 1D-9 DI 9-135 _ W108 TS INTERCHANGED BETWEEN THE PLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[NORMAL ALARM 1B14 —___| or 4-56 = 6A W36 137_|F i135 10-10 DI 9-136 | — W109 Ma a PROTOS Lee CALLY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| EAST 115KV BUS DIFF SYS A RLY FAIL | NORMAL | ALARM 1B15 — [ol 4-57 6A W37 || I! 10-11 DI 9-137 — WH10 MEANS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| EAST 115KV BUS DIFF SYS B RLY FAIL | NORMAL | ALARM 1B16 — | ol 4-58 = 6A W438 | I| 10-12 DI 9-138 = Witt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL | ALARM 1B17 — [oI = 6A | W39 | || = DI 9-139 = Wi12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| WEST 115KV BUS DIFF SYS B RLY FAIL | NORMAL | ALARM 1B18 = DI 4-60 = 6A w40 {I [139 _ DI 9-140 [RM 8-59/60 = FOR CASE NUMBER REFER TO DWG.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL | ALARM = — [or 4-61 = 6A | wal [J _J| DI 9-141 = Wi13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORMAL | ALARM = — [oI — 6A | w42__| F743 | HAIWEE-INYOKERN 115KV1D60] TRIP ALARM | NORMAL DI 9-142 = 6B | (5804239 wit4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| WEST 115KV BUS DIFF SYS A RLY TRIP | NORMAL | ALARM = — [di 4-63 = 6A | W43 | HAIWEE-INYOKERN 115KVID6O|RLY FAIL | NORMAL | ALARM 1D15 DI 9-143 = 6B | | | wits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WEST 115KV BUS DIFF SYS B RLY TRIP NORMAL ALARM _ — or 4-64 = 6A waa HAIWEE-INYOKERN 115KV[D60JA/S auTo SOLID 8-2/AT RK DI 9-144 _ =|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV DFR FAIL 1B19 — | dI 5-65 = 6B | W45 | HAIWEE-INYOKERN 115KV SEL-311L TRIP | ALARM | NORMAL 1D16 DI 10-145] — 6B WIIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV DFR OPERATION — | oI 5-66 = 6B | Ww46 | HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL[ NORMAL | ALARM 1D17 DI 10-146 6B WHI?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV UNDERFREQ RELAY PICK UP NORMAL | ALARM — | oI 5-67 = 6A | W47 | HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL | NORMAL | ALARM DI 10-147, — 6A Wwi18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV UNDERFREQ RELAY FAIL NORMAL | ALARM — [br 5-68 = 6B | w48 | HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-148] — —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>70</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|FCASA DIABLO REACTOR CS 7} 95-21/AT RK Z — | or 5-69 = 1B, 2A = | HAIWEE-INYOKERN 115KV SEL-311L A/S | AUTO | SOLID | 8-1/AT RK DI_10-149|RM 8-63/64 2B, | = *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ICASA DIABLO REACTOR OV | 1C1 = DI 5-70 = 6A wag | “Ts 7| COSO-HAIWEE-INYOKERN T15KV{D60) TRIP | ALARM | NORMAL 1D19 DI 10-150 = 6B | (5804244) | wii9 &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ICASA DIABLO REACTOR UV ] 1¢2 — |[ors-71 = 6A W50 | COSO-HAIWEE-INYOKERN 115KV(D60[RLY FAIL NORMAL | ALARM DI 10-151 = 6B | | 5804244| | W120 é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ICASA D-SHERWIN REACTOR CSF 95-22/AT RKZ| — DI 5-72 = 1B, 2A = COSO-HAIWEE-INYOKERN 115KV[D60/A/S AUTO SOLID 6-2/AT RK DI 10-152| 2B, |se042aap —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ICASA D-SHERWIN REACTOR OV | 1C3 — [or 5-73 = 6A W51 | COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP| ALARM | NORMAL DI 10-153] — 6B wi2t Q</x:t>
+  </x:si>
+  <x:si>
+    <x:t>75</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|FCASA D-SHERWIN REACTOR UV ] 1c4 — | or 5-74 = 6A W52 | COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL | NORMAL | ALARM DI 10-154] — 6B W122 a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||REACTOR OC RELAY BUS AL ] 95-7 AT PNLC3| — _—‘| DI 5-75 = W53 | COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL | NORMAL | ALARM DI 10-155, — 6A W123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||REACTOR DC BACK-UP BUS AL ] 95-8 AT C3 — [ol 5-76 = W54 | COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-156] — =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>78</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||REACTOR OPERATING BUS AL F 95-9 AT C3 — [or 5-7 = W55 | COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S| AuTO | SOLID | 8-1/AT RK DI_10-157|RM 9-67/68 2B, | =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[[cD SHUNT REACTOR TROUBLE AL | TT — |p 5-78 = 6A W56 | HATWEE-INYOKERN 115KV SEL-311L DTT RECD | ALARM | NORMAL DI 10-158] — 6B wi24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|[CD-S SHUNT REACTOR TROUBLE AL | 1C6 — [or 5-79 = 6A W57 | COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD| ALARM | NORMAL 1E1 DI 10-159] — 6B W128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| ADDED POINT FOR 115KV LINE POS. RELAY | 03-05-24 | | VM VM ve | S&amp;L | S&amp;L | VM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV LINE POS. RELAY DIGITAL POINT LISTING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>83</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[DIG PT LISTING RTU SYSTEM T15KV SH. | ROOED,POINTS FOR | 06-24-22 | | VM vM ve | sa | sac | vM RTU aa he</x:t>
+  </x:si>
+  <x:si>
+    <x:t>84</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. RLY'S SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>85</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ONE LINE FOR CONSTRUCTION | REPL'D RLY SEL-311C WITH D60 FOR 115KV LINE POS. | 07-31-25 | | VM vM SSF | | S&amp;L | vM [| | ISSUED FOR CONSTRUCTION 08-31-20 | | VM vB ve | sat | set | vw SOUTHERN CALIFORNIA SCALE+___NONE</x:t>
+  </x:si>
+  <x:si>
     <x:t>|FUPS TROUBLE F 1c8 DI 6-81 — W59</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
     <x:t>[UI15KV CONTROL BUS AL) 95-1 DI 6-82 = W60</x:t>
   </x:si>
   <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
     <x:t>| 115KV RELAY BUS AL 95-2 DI 6-83 = W61</x:t>
   </x:si>
   <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
     <x:t>| 115KV BACK-UP BUS AL 95-3 DI 6-84 = W62</x:t>
   </x:si>
   <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
     <x:t>| 115KV OPERATING BUS AL 95-4 DI 6-85 = W63</x:t>
   </x:si>
   <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-7/AT RK — [or t-7__ [RM 2-9/10 1B, 2A | = 87_| 115KV ELECTRONIC BUS AL 95-5 = DI 6-86 = W64</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| COSO-HAIWEE-INYOKERN 115KV CB CLOSE | OPEN | 95-9/AT RK — [or i-8 [RM 2-11712 1B, | = 88__| 115KV DUPLICATE ELECTRONIC BUS 95-6 = DI 6-87 = W65</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|(BISHOP CREEK PLANT NO. &amp; 115KV CB CLOSE | OPEN | 95-15/AT RK Z — fori-9 [RM 2-13/14 1B, 2A = 89_| 115KV _LBFB BUS 95-7 = DI 6-88 — W66</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
     <x:t>__| 115KV INTERFACE BUS 95-8 = DI 6-89 = W67</x:t>
   </x:si>
   <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
     <x:t>__|E115KVFMETER BUS F 95-9 = DI 6-90 = W68</x:t>
   </x:si>
   <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[WWIXIE VALLEY CUST CBF Tn CLOSE | OPEN | 95-XX/AT RK Z — [or 1-12 [RM 3-19/20 1B, 2A = 92_| SPARE = DI 6-91 = = W69</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[| BUS TIE 115KV CB CLOSE | OPEN | 95-23/AT RK Z31 — [or 1-13 [RM 3-21722 1B, | = 93__| SPARE = DI 6-92 = = W70</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14</x:t>
-  </x:si>
-  <x:si>
     <x:t>_|(115KV W/BUS POT ALE = DI 6-93 = Ww</x:t>
   </x:si>
   <x:si>
-    <x:t>15</x:t>
-  </x:si>
-  <x:si>
     <x:t>_|LI5KV_E/BUS POT ALJ = DI 6-94 = W712</x:t>
   </x:si>
   <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
     <x:t>_| LOW DC VOLTAGE 1c-9 = DI 6-95 = W713</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
     <x:t>| BATT CHG FAIL FAIL LOSS OF AC 1C-10 _— DI 6-96 _— w74</x:t>
   </x:si>
   <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
     <x:t>__| POSITIVE DC GRD 1c-11 = DI 7-97 = W75</x:t>
   </x:si>
   <x:si>
-    <x:t>19</x:t>
-  </x:si>
-  <x:si>
     <x:t>_| NEGATIVE DC GRD 1C-12 = DI 7-98 = W76</x:t>
   </x:si>
   <x:si>
-    <x:t>20</x:t>
-  </x:si>
-  <x:si>
     <x:t>|(SEL-2030 FAIL -—~—~~~~—~\({—«C98 1C-13 = DI 7-99 = WT?</x:t>
   </x:si>
   <x:si>
-    <x:t>21</x:t>
-  </x:si>
-  <x:si>
     <x:t>INO. BANK LTC AUTO/MAN I| = — DI 7-100 |RM 5-37/38 Ww78</x:t>
   </x:si>
   <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
     <x:t>INO. BANK LTC AUTO/MAN || = = DI 7-101 [RM 5-39/40 w79</x:t>
   </x:si>
   <x:si>
-    <x:t>23</x:t>
-  </x:si>
-  <x:si>
     <x:t>INO. BANK TAP RATSE/LOWER I] = = DI 7-102 [RM 6-41/42 W80</x:t>
   </x:si>
   <x:si>
-    <x:t>24</x:t>
-  </x:si>
-  <x:si>
     <x:t>|INO. BANK TAP RAISE/LOWER I| — = DI 7-103 [RM 6-43/44 W81</x:t>
   </x:si>
   <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
     <x:t>_|ISPARE I] = = DI 7-104 [RM 6-45/46 — W82</x:t>
   </x:si>
   <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
     <x:t>||SPARE JI = — DI 7-105 _ W83</x:t>
   </x:si>
   <x:si>
-    <x:t>27</x:t>
-  </x:si>
-  <x:si>
     <x:t>| 115KV BUS TIE POS. 1X SEL-311C TRIP | ALARM | NORMAL — DI 7-106 = 6B Ww84</x:t>
   </x:si>
   <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
     <x:t>| 115KV BUS TIE POS. 1X SEL-31IC RLY FAIL| NORMAL | ALARM 1C15 = DI 7-107 = 6B W85</x:t>
   </x:si>
   <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
     <x:t>[115KV BUS TIE POS. 1X SEL-311C A/S [| AuTO | SOLID | 8-1/AT RK Z51 = DI 7-108 = =</x:t>
   </x:si>
   <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
     <x:t>[f- F[ 1C16 = DI 7-109 = W86</x:t>
   </x:si>
   <x:si>
-    <x:t>31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| SPARE | — | — = = 1A13 — [or 2-31 — = = Wi mt | I| = = DI 7-110 [RM 7-49/50 W87</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| I| ici? = DI ?-111 — W88</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
     <x:t>| ant 1c18 — DI 7-112 = W89</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| RESERVED FOR 115KV LINE Pos. 2x ll 1c19 = DI 8-113 = w90</x:t>
   </x:si>
   <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
     <x:t>{|_| PROTECTION RELAYS ALARMS | DI 8-114 = w91</x:t>
   </x:si>
   <x:si>
-    <x:t>36</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] = DI 8-115 [RM 7-51/52 w92</x:t>
   </x:si>
   <x:si>
-    <x:t>37</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] = DI 8-116 = =</x:t>
   </x:si>
   <x:si>
-    <x:t>38</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] DI 8-117 = W93</x:t>
   </x:si>
   <x:si>
-    <x:t>39</x:t>
-  </x:si>
-  <x:si>
     <x:t>| | DI 8-118 = wo4</x:t>
   </x:si>
   <x:si>
-    <x:t>40</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] 1¢23 DI 8-119 = w95</x:t>
   </x:si>
   <x:si>
-    <x:t>41</x:t>
-  </x:si>
-  <x:si>
     <x:t>|F I] DI 8-120 = w96</x:t>
   </x:si>
   <x:si>
-    <x:t>42</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I| = DI 8-121 = WoT</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I — DI 8-122 [RM 7-53/54 =</x:t>
   </x:si>
   <x:si>
-    <x:t>44</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| L RESERVED FOR 115KV LINE Pos. 1__l| 1D-1 DI 8-123 = w98</x:t>
   </x:si>
   <x:si>
-    <x:t>45</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| [ PROTECTION RELAYS ALARMS I 1D-2 DI 8-124 — w99</x:t>
   </x:si>
   <x:si>
-    <x:t>46</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] 10-3 DI 8-125 = W100</x:t>
   </x:si>
   <x:si>
-    <x:t>47</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] 10-4 DI 8-126 _— W101</x:t>
   </x:si>
   <x:si>
-    <x:t>48</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| I| = DI 8-127 = W102 NOTES:</x:t>
   </x:si>
   <x:si>
-    <x:t>49</x:t>
-  </x:si>
-  <x:si>
     <x:t>| | = DI 8-128 [RM 7-55/56 =</x:t>
   </x:si>
   <x:si>
-    <x:t>50</x:t>
-  </x:si>
-  <x:si>
     <x:t>| F[_ 10-5 DI 9-129 = W103 ane SINE RO SSE TRIPPING RECS.</x:t>
   </x:si>
   <x:si>
-    <x:t>51</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I| 10-6 DI 9-130 — W104 AN INDICATION IS TAKEN FROM EACH</x:t>
   </x:si>
   <x:si>
-    <x:t>52</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] 10-7 DI 9-131 — W105 RUA</x:t>
   </x:si>
   <x:si>
-    <x:t>53</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I] 10-8 DI 9-132 = W106</x:t>
   </x:si>
   <x:si>
-    <x:t>54</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| I = DI 9-133 — W107 OY</x:t>
   </x:si>
   <x:si>
-    <x:t>55</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV_UNDERFREQ POT FAIL NORMAL | ALARM | 74/AT RK Z58 —_ DI 4-55 a W35 136_||_l RESERVED FOR 115KV LINE POS. 2_|| 1D-9 DI 9-135 _ W108 TS INTERCHANGED BETWEEN THE PLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[NORMAL ALARM 1B14 —___| or 4-56 = 6A W36 137_|F i135 10-10 DI 9-136 | — W109 Ma a PROTOS Lee CALLY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>57</x:t>
-  </x:si>
-  <x:si>
     <x:t>|| I! 10-11 DI 9-137 — WH10 MEANS</x:t>
   </x:si>
   <x:si>
-    <x:t>58</x:t>
-  </x:si>
-  <x:si>
     <x:t>| I| 10-12 DI 9-138 = Witt</x:t>
   </x:si>
   <x:si>
-    <x:t>59</x:t>
-  </x:si>
-  <x:si>
     <x:t>| || = DI 9-139 = Wi12</x:t>
   </x:si>
   <x:si>
-    <x:t>60</x:t>
-  </x:si>
-  <x:si>
     <x:t>{I [139 _ DI 9-140 [RM 8-59/60 = FOR CASE NUMBER REFER TO DWG.</x:t>
   </x:si>
   <x:si>
-    <x:t>61</x:t>
-  </x:si>
-  <x:si>
     <x:t>[J _J| DI 9-141 = Wi13</x:t>
   </x:si>
   <x:si>
-    <x:t>62</x:t>
-  </x:si>
-  <x:si>
     <x:t>F743 | HAIWEE-INYOKERN 115KV1D60] TRIP ALARM | NORMAL DI 9-142 = 6B | (5804239 wit4</x:t>
   </x:si>
   <x:si>
-    <x:t>63</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HAIWEE-INYOKERN 115KVID6O|RLY FAIL | NORMAL | ALARM 1D15 DI 9-143 = 6B | | | wits</x:t>
   </x:si>
   <x:si>
-    <x:t>64</x:t>
-  </x:si>
-  <x:si>
     <x:t>HAIWEE-INYOKERN 115KV[D60JA/S auTo SOLID 8-2/AT RK DI 9-144 _ =|</x:t>
   </x:si>
   <x:si>
-    <x:t>65</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HAIWEE-INYOKERN 115KV SEL-311L TRIP | ALARM | NORMAL 1D16 DI 10-145] — 6B WIIG</x:t>
   </x:si>
   <x:si>
-    <x:t>66</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HAIWEE-INYOKERN 115KV SEL-311L RLY FAIL[ NORMAL | ALARM 1D17 DI 10-146 6B WHI?</x:t>
   </x:si>
   <x:si>
-    <x:t>67</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HAIWEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-148] — —</x:t>
   </x:si>
   <x:si>
-    <x:t>68</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HAIWEE-INYOKERN 115KV SEL-311L A/S | AUTO | SOLID | 8-1/AT RK DI_10-149|RM 8-63/64 2B, | = *</x:t>
   </x:si>
   <x:si>
-    <x:t>69</x:t>
-  </x:si>
-  <x:si>
     <x:t>“Ts 7| COSO-HAIWEE-INYOKERN T15KV{D60) TRIP | ALARM | NORMAL 1D19 DI 10-150 = 6B | (5804244) | wii9 &gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>70</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAIWEE-INYOKERN 115KV(D60[RLY FAIL NORMAL | ALARM DI 10-151 = 6B | | 5804244| | W120 é</x:t>
   </x:si>
   <x:si>
-    <x:t>71</x:t>
-  </x:si>
-  <x:si>
     <x:t>COSO-HAIWEE-INYOKERN 115KV[D60/A/S AUTO SOLID 6-2/AT RK DI 10-152| 2B, |se042aap —</x:t>
   </x:si>
   <x:si>
-    <x:t>72</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L TRIP| ALARM | NORMAL DI 10-153] — 6B wi2t Q</x:t>
   </x:si>
   <x:si>
-    <x:t>73</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HATNEE-INYOKERN 115KV SEL-311L RLY FAIL | NORMAL | ALARM DI 10-154] — 6B W122 a</x:t>
   </x:si>
   <x:si>
-    <x:t>74</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L CHAN FAIL | NORMAL | ALARM DI 10-155, — 6A W123</x:t>
   </x:si>
   <x:si>
-    <x:t>75</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAINEE-INYOKERN 115KV SEL-311L DIFF A/S| AUTO | SOLID |43-2/AT RK DI 10-156] — =</x:t>
   </x:si>
   <x:si>
-    <x:t>76</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAIWEE-INYOKERN 115KV SEL-311L A/S| AuTO | SOLID | 8-1/AT RK DI_10-157|RM 9-67/68 2B, | =</x:t>
   </x:si>
   <x:si>
-    <x:t>77</x:t>
-  </x:si>
-  <x:si>
     <x:t>| HATWEE-INYOKERN 115KV SEL-311L DTT RECD | ALARM | NORMAL DI 10-158] — 6B wi24</x:t>
   </x:si>
   <x:si>
-    <x:t>78</x:t>
-  </x:si>
-  <x:si>
     <x:t>| COSO-HAINEE-INYOKERN 115KV SEL-311L DTT RECD| ALARM | NORMAL 1E1 DI 10-159] — 6B W128</x:t>
   </x:si>
   <x:si>
-    <x:t>79</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| ADDED POINT FOR 115KV LINE POS. RELAY | 03-05-24 | | VM VM ve | S&amp;L | S&amp;L | VM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>80</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV ADDED POINT FOR 115KV LINE POS. RELAY DIGITAL POINT LISTING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>81</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[DIG PT LISTING RTU SYSTEM T15KV SH. | ROOED,POINTS FOR | 06-24-22 | | VM vM ve | sa | sac | vM RTU aa he</x:t>
-  </x:si>
-  <x:si>
-    <x:t>82</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ED RTU/EPAC SYSTEM 115-55KV ADDED POINTS FOR 115KV LINE POS. RLY'S SH.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>83</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ONE LINE FOR CONSTRUCTION | REPL'D RLY SEL-311C WITH D60 FOR 115KV LINE POS. | 07-31-25 | | VM vM SSF | | S&amp;L | vM [| | ISSUED FOR CONSTRUCTION 08-31-20 | | VM vB ve | sat | set | vw SOUTHERN CALIFORNIA SCALE+___NONE</x:t>
-  </x:si>
-  <x:si>
     <x:t>DscRPT DSCRIPT] RELAY NO. RELAY NO. (NOTE 3)] we. | DscRPT DSCRIPT| RELAY NO. RELAY NO. (NOTE 3)} pwc.</x:t>
   </x:si>
   <x:si>
+    <x:t>|| |] 1£2 = DI 10-160 = W129 |(SILVERPEAK A A ToT ' \ = -</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1E3 DI 11-161 W130 |ISILVERPEAK A B TCT | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DI 11-162 TA, 2A W131 |ISILVERPEAK A C TCT E = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| PROTECTION RELAYS ALARMS || _— DI 11-163 W132 FSTLVERPEAK A GRD ToT Ji 904562788) — rT _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| | | _— DI 11-164|RM 9-67/68 = |(HAIWEE-INYOKERN 115KV D60 OPD A/S || NORMAL | ALARM | 16-15 DI 15-228 { 6A "| ) wig92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[fF F| DI 11-165 W133 ||HAIWEE-INYOKERN 115KV D60 OPD ALARM|| x NORMAL | ALARM | 16-16 DI 15-229 | 6A || W193</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I || DI 11-166 W134 |[HAIWEE-INYOKERN 115KV D60 OPD TRIP_]| li NORMAL | ALARM J 16-17 DI 15-230 6A }| W194</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || DI 11-167 W135 |(COSO-HAIWEE-INYOKERN 115KV D60 OPD A/S || [ NORMAL | ALARM | 16-18 DI 15-231 f 6A | )| wig95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I || DI 11-168 W136 || COSO-HAIWEE-INYOKERN 115KV D60 OPD ALARM || x NORMAL | ALARM | 16-19 DI 15-232 | 6A || W196</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || = DI 11-169 W137 [\COSO-HAIWEESINYOKERN 115KV OPO TRIP _)| Lt NORMAL | ALARM J 16-20 DI 15-233 \_6A_, |_ J] W197</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= DI 11-170|RM 9-69/70 = 251_| SPARE L Lt 16-21 DI 15-234 LT gn4562794 | W198</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[i RESERVED FOR 115KV LINE Pos. 7_[| 1E9 DI 11-171 W138 _| SPARE 16-22 DI 15-235 W199</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1E10 DI 11-172 W139 253_| SPARE 16-23 DI 15-236 W200</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I || 1E11 DI 11-173 W140 | SPARE 16-24 DI 15-237 W201</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || — DI 11-175 W142 | SPARE DI 15-239 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || = DI 11-176|RM 9-71/72 _ | SPARE DI 15-240 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|F || 1E13 DI 12-177 W143 | SPARE = DI 16-241 W203</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|] || 1E14 DI 12-178 W144 | SPARE _— DI 16-242 W204</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || 1E15 DI 12-179 W145 | SPARE = DI 16-243 W205</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || 1E16 DI 12-180 W146 _| SPARE = DI 16-244 W206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= DI 12-181 W147 _| SPARE = DI 16-245 W207</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| || = DI 12-182|RM 10-73/74 = | SPARE = DI 16-246 —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[fF L RESERVED FOR 115KV LINE POs. _| | 1E17 DI 12-183 W148 | SPARE — DI 16-247|RM 10-77/78 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| { PROTECTION RELAYS ALARMS || 1E18 DI 12-184 _| SPARE = DI 16-248]RM 10-79/80 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|I | | 1E19 DI 12-185 W150 | SPARE = DI 16-249]RM 11-81/82 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| Fl 1£20 DI 12-186 W151 | SPARE = DI 16-250|/RM 11-83/84 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= DI 12-187 W152 _| SPARE = DI 16-251|RM 11-85/86 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| | | = DI 12-188]RM 10-75/76 _ | SPARE = DI 16-252]RM 11-87/88 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|| p_____J | DI 12-189 W153 | SPARE = DI 16-253|RM 12-89/90 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV LBFB ARMED 1F1 DI 12-190 NOTE W154 | SPARE _ DI 16-254]RM 12-91/92 _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV LBFB TRIP 1F2 DI 12-191 NOTE W155 272_| SPARE = DI 16-255|/RM 12-93/94 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(15KV CB I'LBFB RELAY PS % FAIL \| 1F3 DI 12-192 W156 | SPARE on = DI 16-256]/RM 12-95/96 =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F4 DI 13-193 WI57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[f115KV CB LBFB RELAY PS % FAIL F | 1F5 DI 13-194 W158</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV CB LBFB RELAY FAIL }|_194 1F6 DI 13-195 W159</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F7 DI 13-196 W160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F8 DI 13-197 W161</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F9 DI 13-198 wi62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F10 DI 13-199 W163</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS FAIL Tal DI 13-200 W164</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F12 DI 13-201 W165</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS 1% FAIL 1F13 DI 13-202 W166</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F14 DI 13-203 W167</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|(TS5KV CB 11" LBFB RELAY PS FAIL \| 1F15 DI 13-204 W168</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F16 DI 13-205 W169</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F17 DI 13-206 W170</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ff115KV CB LBFB RELAY FAIL FI 1F18 DI 13-207 WIT7I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY PS FAIL || 1F19 DI 13-208 Wi72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|I115KV CB LBFB RELAY FAIL || 1F20 DI 14-209 WI73</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F21 DI 14-210 wi74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV CB LBFB RELAY FAIL J | 1F22 DI 14-211 W175</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY PS % FAIL 2u1 1F23 DI 14-212 W176</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| 115KV CB LBFB RELAY FAIL 1F24 DI 14-213 WI77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_| SPARE DI 14-214 W178</x:t>
+  </x:si>
+  <x:si>
+    <x:t>| SPARE DI 14-215 Wi79</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|f115Kv cB TCM | 2t5 DI 14-216 W180</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM DI 14-217 wie!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{l115KV cB TCM DI 14-218 W182 ONE SINGLE RTU CONTROL OUTPUT RESETS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[[115KV CB TCM [| DI 14-219 W183</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F15KV CB TCM |_| DI 14-220 W184 INDIVIDUAL SUDDEN PRESSURE TRIPPING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|l115KV cB TCM F DI 14-222 W186 a) "Vv" IN A BLOCK INDICATES A VIRTUAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I115KV CB TCM |__| DI 14-223 W187 POINT. A VIRTUAL POINT DOES NOT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[115K CB TCM |_| GH DI 14-204 W188 Mo eO ROR ONCER BoT WEN att pee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{l115KV CB TCM |_| DI 15-225 W189 AND THE RTU ELECTRONICALLY VIA THE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CB TCM | DI 15-226</x:t>
+  </x:si>
+  <x:si>
+    <x:t>COM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A TGT — —</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_ FOR CASE NUMBER REFER TO DWG. *</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_fHWE-INYOKERN C TGT |__| = _ &gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= = Ey BEB RN LAVS,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE A TGT | | = = a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE B TGT |_| = _ @</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|lcoso_HWE C_TGT | | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|lcoso HWE GRD TGT | | = = é</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_|ISILVERPEAK C A TCT F | = =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ISILVERPEAK C C TCT | | = _ °</x:t>
+  </x:si>
+  <x:si>
+    <x:t>||SILVERPEAK C GRD TcT ps (| = _</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|DIG PT LISTING RTU SYSTEM 115KV SH. | ADDED OPD ALARMS FOR D60 115KV LINE POS. | 07-31-25 | | VM vM SSF | S&amp;L | S&amp;L | VM RTU aa a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ED RTU SYSTEM 115-55KV ——] ADDED OPD ALARMS FOR D60 115KV LINE POS. |————| SH.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|ONE LINE FOR CONSTRUCTION | ISSUED FOR CONSTRUCTION 08-31-20 | | VM VB ve | sa | S&amp;L | VM SOUTHERN CALIFORNIA SCALE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>- SIZE wh</x:t>
+  </x:si>
+  <x:si>
     <x:t>|(SILVERPEAK A A ToT ' \ = -</x:t>
   </x:si>
   <x:si>
@@ -560,15 +1025,9 @@
     <x:t>[\COSO-HAIWEESINYOKERN 115KV OPO TRIP _)| Lt NORMAL | ALARM J 16-20 DI 15-233 \_6A_, |_ J] W197</x:t>
   </x:si>
   <x:si>
-    <x:t>= DI 11-170|RM 9-69/70 = 251_| SPARE L Lt 16-21 DI 15-234 LT gn4562794 | W198</x:t>
-  </x:si>
-  <x:si>
     <x:t>_| SPARE 16-22 DI 15-235 W199</x:t>
   </x:si>
   <x:si>
-    <x:t>1E10 DI 11-172 W139 253_| SPARE 16-23 DI 15-236 W200</x:t>
-  </x:si>
-  <x:si>
     <x:t>| SPARE 16-24 DI 15-237 W201</x:t>
   </x:si>
   <x:si>
@@ -623,166 +1082,7 @@
     <x:t>| SPARE _ DI 16-254]RM 12-91/92 _</x:t>
   </x:si>
   <x:si>
-    <x:t>| 115KV LBFB TRIP 1F2 DI 12-191 NOTE W155 272_| SPARE = DI 16-255|/RM 12-93/94 =</x:t>
-  </x:si>
-  <x:si>
     <x:t>| SPARE on = DI 16-256]/RM 12-95/96 =</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|I115KV CB LBFB RELAY FAIL || 1F4 DI 13-193 WI57</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[f115KV CB LBFB RELAY PS % FAIL F | 1F5 DI 13-194 W158</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|l115KV CB LBFB RELAY FAIL }|_194 1F6 DI 13-195 W159</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F7 DI 13-196 W160</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY FAIL 1F8 DI 13-197 W161</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY PS FAIL 1F9 DI 13-198 wi62</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY FAIL 1F10 DI 13-199 W163</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY PS FAIL Tal DI 13-200 W164</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY FAIL 1F12 DI 13-201 W165</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY PS 1% FAIL 1F13 DI 13-202 W166</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY FAIL 1F14 DI 13-203 W167</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|(TS5KV CB 11" LBFB RELAY PS FAIL \| 1F15 DI 13-204 W168</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|I115KV CB LBFB RELAY FAIL || 1F16 DI 13-205 W169</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F17 DI 13-206 W170</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ff115KV CB LBFB RELAY FAIL FI 1F18 DI 13-207 WIT7I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|I115KV CB LBFB RELAY PS FAIL || 1F19 DI 13-208 Wi72</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|I115KV CB LBFB RELAY FAIL || 1F20 DI 14-209 WI73</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|IN15KV CB LBFB RELAY PS FAIL || 1F21 DI 14-210 wi74</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|l115KV CB LBFB RELAY FAIL J | 1F22 DI 14-211 W175</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY PS % FAIL 2u1 1F23 DI 14-212 W176</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| 115KV CB LBFB RELAY FAIL 1F24 DI 14-213 WI77</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_| SPARE DI 14-214 W178</x:t>
-  </x:si>
-  <x:si>
-    <x:t>| SPARE DI 14-215 Wi79</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_|f115Kv cB TCM | 2t5 DI 14-216 W180</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CB TCM DI 14-217 wie!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{l115KV cB TCM DI 14-218 W182 ONE SINGLE RTU CONTROL OUTPUT RESETS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[[115KV CB TCM [| DI 14-219 W183</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F15KV CB TCM |_| DI 14-220 W184 INDIVIDUAL SUDDEN PRESSURE TRIPPING</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CB TCM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|l115KV cB TCM F DI 14-222 W186 a) "Vv" IN A BLOCK INDICATES A VIRTUAL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I115KV CB TCM |__| DI 14-223 W187 POINT. A VIRTUAL POINT DOES NOT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[115K CB TCM |_| GH DI 14-204 W188 Mo eO ROR ONCER BoT WEN att pee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{l115KV CB TCM |_| DI 15-225 W189 AND THE RTU ELECTRONICALLY VIA THE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CB TCM | DI 15-226</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A TGT — —</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_ FOR CASE NUMBER REFER TO DWG. *</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_fHWE-INYOKERN C TGT |__| = _ &gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>= = Ey BEB RN LAVS,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|lcoso HWE A TGT | | = = a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|lcoso HWE B TGT |_| = _ @</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_|lcoso_HWE C_TGT | | = =</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|lcoso HWE GRD TGT | | = = é</x:t>
-  </x:si>
-  <x:si>
-    <x:t>_|ISILVERPEAK C A TCT F | = =</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ISILVERPEAK C C TCT | | = _ °</x:t>
-  </x:si>
-  <x:si>
-    <x:t>||SILVERPEAK C GRD TcT ps (| = _</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ANALOG PT LISTING RTU SYSTEM 115KV DIGITAL POINT LISTING ae</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|DIG PT LISTING RTU SYSTEM 115KV SH. | ADDED OPD ALARMS FOR D60 115KV LINE POS. | 07-31-25 | | VM vM SSF | S&amp;L | S&amp;L | VM RTU aa a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ED RTU SYSTEM 115-55KV ——] ADDED OPD ALARMS FOR D60 115KV LINE POS. |————| SH.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|ONE LINE FOR CONSTRUCTION | ISSUED FOR CONSTRUCTION 08-31-20 | | VM VB ve | sa | S&amp;L | VM SOUTHERN CALIFORNIA SCALE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>84</x:t>
-  </x:si>
-  <x:si>
-    <x:t>- SIZE wh</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1148,7 +1448,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B85"/>
+  <x:dimension ref="A1:B171"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1832,6 +2132,694 @@
       </x:c>
       <x:c r="B85" s="0" t="s">
         <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:2">
+      <x:c r="A86" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:2">
+      <x:c r="A87" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:2">
+      <x:c r="A88" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:2">
+      <x:c r="A89" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:2">
+      <x:c r="A90" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:2">
+      <x:c r="A91" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:2">
+      <x:c r="A92" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:2">
+      <x:c r="A93" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:2">
+      <x:c r="A94" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:2">
+      <x:c r="A95" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:2">
+      <x:c r="A96" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:2">
+      <x:c r="A97" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:2">
+      <x:c r="A98" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:2">
+      <x:c r="A99" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:2">
+      <x:c r="A100" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:2">
+      <x:c r="A101" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:2">
+      <x:c r="A102" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:2">
+      <x:c r="A103" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:2">
+      <x:c r="A104" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:2">
+      <x:c r="A105" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:2">
+      <x:c r="A106" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:2">
+      <x:c r="A107" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:2">
+      <x:c r="A108" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:2">
+      <x:c r="A109" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:2">
+      <x:c r="A110" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:2">
+      <x:c r="A111" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:2">
+      <x:c r="A112" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:2">
+      <x:c r="A113" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:2">
+      <x:c r="A114" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:2">
+      <x:c r="A115" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:2">
+      <x:c r="A116" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:2">
+      <x:c r="A117" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:2">
+      <x:c r="A118" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:2">
+      <x:c r="A119" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:2">
+      <x:c r="A120" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:2">
+      <x:c r="A121" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122" spans="1:2">
+      <x:c r="A122" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B122" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:2">
+      <x:c r="A123" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:2">
+      <x:c r="A124" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:2">
+      <x:c r="A125" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:2">
+      <x:c r="A126" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:2">
+      <x:c r="A127" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:2">
+      <x:c r="A128" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:2">
+      <x:c r="A129" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:2">
+      <x:c r="A130" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:2">
+      <x:c r="A131" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:2">
+      <x:c r="A132" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:2">
+      <x:c r="A133" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:2">
+      <x:c r="A134" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:2">
+      <x:c r="A135" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:2">
+      <x:c r="A136" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" spans="1:2">
+      <x:c r="A137" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B137" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138" spans="1:2">
+      <x:c r="A138" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:2">
+      <x:c r="A139" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:2">
+      <x:c r="A140" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:2">
+      <x:c r="A141" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:2">
+      <x:c r="A142" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:2">
+      <x:c r="A143" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:2">
+      <x:c r="A144" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B144" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:2">
+      <x:c r="A145" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B145" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:2">
+      <x:c r="A146" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:2">
+      <x:c r="A147" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:2">
+      <x:c r="A148" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B148" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:2">
+      <x:c r="A149" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B149" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:2">
+      <x:c r="A150" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B150" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:2">
+      <x:c r="A151" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B151" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152" spans="1:2">
+      <x:c r="A152" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B152" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153" spans="1:2">
+      <x:c r="A153" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B153" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154" spans="1:2">
+      <x:c r="A154" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B154" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:2">
+      <x:c r="A155" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:2">
+      <x:c r="A156" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:2">
+      <x:c r="A157" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:2">
+      <x:c r="A158" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:2">
+      <x:c r="A159" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160" spans="1:2">
+      <x:c r="A160" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B160" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161" spans="1:2">
+      <x:c r="A161" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B161" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162" spans="1:2">
+      <x:c r="A162" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163" spans="1:2">
+      <x:c r="A163" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B163" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164" spans="1:2">
+      <x:c r="A164" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B164" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165" spans="1:2">
+      <x:c r="A165" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B165" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166" spans="1:2">
+      <x:c r="A166" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B166" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="167" spans="1:2">
+      <x:c r="A167" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B167" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="168" spans="1:2">
+      <x:c r="A168" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B168" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="169" spans="1:2">
+      <x:c r="A169" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B169" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="170" spans="1:2">
+      <x:c r="A170" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B170" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="171" spans="1:2">
+      <x:c r="A171" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="B171" s="0" t="s">
+        <x:v>173</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1848,7 +2836,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B86"/>
+  <x:dimension ref="A1:B170"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1867,7 +2855,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1875,7 +2863,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1883,7 +2871,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1891,7 +2879,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1899,7 +2887,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1907,7 +2895,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>247</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1915,7 +2903,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1923,7 +2911,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1931,7 +2919,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>250</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1939,7 +2927,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1947,7 +2935,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1955,7 +2943,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1963,7 +2951,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1971,7 +2959,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>255</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1979,7 +2967,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1987,7 +2975,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1995,7 +2983,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>258</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -2003,7 +2991,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -2011,7 +2999,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -2019,7 +3007,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -2027,7 +3015,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -2035,7 +3023,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -2043,7 +3031,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -2051,7 +3039,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -2059,7 +3047,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>266</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -2067,7 +3055,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -2075,7 +3063,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>268</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -2083,7 +3071,7 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -2091,7 +3079,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>270</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -2099,7 +3087,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>271</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -2107,7 +3095,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>272</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -2115,7 +3103,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>273</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -2123,7 +3111,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>274</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -2131,7 +3119,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -2139,7 +3127,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>276</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -2147,7 +3135,7 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>277</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
@@ -2155,7 +3143,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
@@ -2163,7 +3151,7 @@
         <x:v>76</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>279</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
@@ -2171,7 +3159,7 @@
         <x:v>78</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>280</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
@@ -2179,7 +3167,7 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
@@ -2187,7 +3175,7 @@
         <x:v>82</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>282</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
@@ -2195,7 +3183,7 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>283</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
@@ -2203,7 +3191,7 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
@@ -2211,7 +3199,7 @@
         <x:v>88</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
@@ -2219,7 +3207,7 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>286</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
@@ -2227,7 +3215,7 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>287</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
@@ -2235,7 +3223,7 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>288</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:2">
@@ -2243,7 +3231,7 @@
         <x:v>96</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>289</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:2">
@@ -2251,7 +3239,7 @@
         <x:v>98</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:2">
@@ -2259,7 +3247,7 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>291</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:2">
@@ -2267,7 +3255,7 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>292</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:2">
@@ -2275,7 +3263,7 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:2">
@@ -2283,7 +3271,7 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>294</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:2">
@@ -2291,7 +3279,7 @@
         <x:v>108</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>295</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:2">
@@ -2299,7 +3287,7 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:2">
@@ -2307,7 +3295,7 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:2">
@@ -2315,7 +3303,7 @@
         <x:v>114</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>298</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:2">
@@ -2323,7 +3311,7 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>299</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:2">
@@ -2331,7 +3319,7 @@
         <x:v>118</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:2">
@@ -2339,7 +3327,7 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>301</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:2">
@@ -2347,7 +3335,7 @@
         <x:v>122</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>302</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:2">
@@ -2355,7 +3343,7 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>303</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:2">
@@ -2363,7 +3351,7 @@
         <x:v>126</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>304</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:2">
@@ -2371,7 +3359,7 @@
         <x:v>128</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>305</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:2">
@@ -2379,7 +3367,7 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>306</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:2">
@@ -2387,7 +3375,7 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>307</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:2">
@@ -2395,7 +3383,7 @@
         <x:v>134</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:2">
@@ -2403,7 +3391,7 @@
         <x:v>136</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>309</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:2">
@@ -2411,7 +3399,7 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:2">
@@ -2419,7 +3407,7 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>311</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:2">
@@ -2427,7 +3415,7 @@
         <x:v>142</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>312</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:2">
@@ -2435,7 +3423,7 @@
         <x:v>144</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>313</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:2">
@@ -2443,7 +3431,7 @@
         <x:v>146</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:2">
@@ -2451,7 +3439,7 @@
         <x:v>148</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>315</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:2">
@@ -2459,7 +3447,7 @@
         <x:v>150</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>316</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:2">
@@ -2467,7 +3455,7 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:2">
@@ -2475,7 +3463,7 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>318</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:2">
@@ -2483,7 +3471,7 @@
         <x:v>156</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>319</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:2">
@@ -2491,7 +3479,7 @@
         <x:v>158</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>320</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:2">
@@ -2499,7 +3487,7 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>321</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:2">
@@ -2507,7 +3495,7 @@
         <x:v>162</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>322</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:2">
@@ -2515,7 +3503,7 @@
         <x:v>164</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:2">
@@ -2523,7 +3511,7 @@
         <x:v>166</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>324</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:2">
@@ -2531,15 +3519,687 @@
         <x:v>168</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>325</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:2">
       <x:c r="A86" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:2">
+      <x:c r="A87" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:2">
+      <x:c r="A88" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:2">
+      <x:c r="A89" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:2">
+      <x:c r="A90" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:2">
+      <x:c r="A91" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:2">
+      <x:c r="A92" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:2">
+      <x:c r="A93" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:2">
+      <x:c r="A94" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:2">
+      <x:c r="A95" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:2">
+      <x:c r="A96" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:2">
+      <x:c r="A97" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:2">
+      <x:c r="A98" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:2">
+      <x:c r="A99" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
         <x:v>255</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:2">
+      <x:c r="A100" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:2">
+      <x:c r="A101" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:2">
+      <x:c r="A102" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:2">
+      <x:c r="A103" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:2">
+      <x:c r="A104" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:2">
+      <x:c r="A105" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:2">
+      <x:c r="A106" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:2">
+      <x:c r="A107" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:2">
+      <x:c r="A108" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:2">
+      <x:c r="A109" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:2">
+      <x:c r="A110" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:2">
+      <x:c r="A111" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:2">
+      <x:c r="A112" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:2">
+      <x:c r="A113" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:2">
+      <x:c r="A114" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:2">
+      <x:c r="A115" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:2">
+      <x:c r="A116" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:2">
+      <x:c r="A117" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:2">
+      <x:c r="A118" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:2">
+      <x:c r="A119" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:2">
+      <x:c r="A120" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:2">
+      <x:c r="A121" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122" spans="1:2">
+      <x:c r="A122" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B122" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:2">
+      <x:c r="A123" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:2">
+      <x:c r="A124" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:2">
+      <x:c r="A125" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:2">
+      <x:c r="A126" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:2">
+      <x:c r="A127" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:2">
+      <x:c r="A128" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:2">
+      <x:c r="A129" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:2">
+      <x:c r="A130" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:2">
+      <x:c r="A131" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:2">
+      <x:c r="A132" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:2">
+      <x:c r="A133" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:2">
+      <x:c r="A134" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:2">
+      <x:c r="A135" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:2">
+      <x:c r="A136" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" spans="1:2">
+      <x:c r="A137" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B137" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138" spans="1:2">
+      <x:c r="A138" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:2">
+      <x:c r="A139" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:2">
+      <x:c r="A140" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:2">
+      <x:c r="A141" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:2">
+      <x:c r="A142" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:2">
+      <x:c r="A143" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:2">
+      <x:c r="A144" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B144" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:2">
+      <x:c r="A145" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B145" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:2">
+      <x:c r="A146" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:2">
+      <x:c r="A147" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:2">
+      <x:c r="A148" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B148" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:2">
+      <x:c r="A149" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B149" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:2">
+      <x:c r="A150" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B150" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:2">
+      <x:c r="A151" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B151" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152" spans="1:2">
+      <x:c r="A152" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B152" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153" spans="1:2">
+      <x:c r="A153" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B153" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154" spans="1:2">
+      <x:c r="A154" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B154" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:2">
+      <x:c r="A155" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:2">
+      <x:c r="A156" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:2">
+      <x:c r="A157" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:2">
+      <x:c r="A158" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:2">
+      <x:c r="A159" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160" spans="1:2">
+      <x:c r="A160" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B160" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161" spans="1:2">
+      <x:c r="A161" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B161" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162" spans="1:2">
+      <x:c r="A162" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163" spans="1:2">
+      <x:c r="A163" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B163" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164" spans="1:2">
+      <x:c r="A164" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B164" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165" spans="1:2">
+      <x:c r="A165" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B165" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166" spans="1:2">
+      <x:c r="A166" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B166" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="167" spans="1:2">
+      <x:c r="A167" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B167" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="168" spans="1:2">
+      <x:c r="A168" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B168" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="169" spans="1:2">
+      <x:c r="A169" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="B169" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="170" spans="1:2">
+      <x:c r="A170" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B170" s="0" t="s">
+        <x:v>325</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>